<commit_message>
Generic deconvolution works now.
Fixed remaining bugs in the generic deconvolution method.
Checkd it out from the "benchmark" project.
</commit_message>
<xml_diff>
--- a/inst/extdata/cell_type_mapping.xlsx
+++ b/inst/extdata/cell_type_mapping.xlsx
@@ -9,11 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11370"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11370" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="cell_type2methods" sheetId="3" r:id="rId1"/>
-    <sheet name="cell_type2datasets" sheetId="4" r:id="rId2"/>
+    <sheet name="celltype2method" sheetId="3" r:id="rId1"/>
+    <sheet name="celltype2dataset" sheetId="4" r:id="rId2"/>
     <sheet name="extended mapping" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="171027"/>
@@ -632,7 +632,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
@@ -1005,7 +1005,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
add methods to cope with cibersort and timer.
</commit_message>
<xml_diff>
--- a/inst/extdata/cell_type_mapping.xlsx
+++ b/inst/extdata/cell_type_mapping.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11370" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11370"/>
   </bookViews>
   <sheets>
     <sheet name="celltype2method" sheetId="3" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="79">
   <si>
     <t>IKDC</t>
   </si>
@@ -260,6 +260,9 @@
   </si>
   <si>
     <t>mcp_counter</t>
+  </si>
+  <si>
+    <t>cibersort_abs</t>
   </si>
 </sst>
 </file>
@@ -630,26 +633,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H27"/>
+  <dimension ref="A1:I27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="29.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.42578125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="20.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.42578125" style="1"/>
-    <col min="6" max="6" width="24.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="11.42578125" style="1"/>
+    <col min="1" max="1" width="27.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="29.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.42578125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="20.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.42578125" style="1"/>
+    <col min="7" max="7" width="24.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>58</v>
       </c>
@@ -657,25 +660,28 @@
         <v>4</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>59</v>
       </c>
@@ -683,51 +689,58 @@
         <v>29</v>
       </c>
       <c r="C2" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="E2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="3"/>
       <c r="F2" s="3"/>
-      <c r="G2" s="3" t="s">
+      <c r="G2" s="3"/>
+      <c r="H2" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="I2" s="3" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>60</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="3"/>
+      <c r="E3" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="3"/>
       <c r="F3" s="3"/>
       <c r="G3" s="3"/>
       <c r="H3" s="3"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I3" s="3"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>61</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3" t="s">
+      <c r="C4" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="E4" s="3"/>
       <c r="F4" s="3"/>
       <c r="G4" s="3"/>
       <c r="H4" s="3"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I4" s="3"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>62</v>
       </c>
@@ -735,45 +748,51 @@
         <v>27</v>
       </c>
       <c r="C5" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D5" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="E5" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3" t="s">
+      <c r="F5" s="3"/>
+      <c r="G5" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="G5" s="3" t="s">
+      <c r="H5" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="H5" s="3" t="s">
+      <c r="I5" s="3" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>14</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3" t="s">
+      <c r="C6" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3" t="s">
+      <c r="F6" s="3"/>
+      <c r="G6" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="G6" s="3" t="s">
+      <c r="H6" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="H6" s="3" t="s">
+      <c r="I6" s="3" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>0</v>
       </c>
@@ -784,8 +803,9 @@
       <c r="F7" s="3"/>
       <c r="G7" s="3"/>
       <c r="H7" s="3"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I7" s="3"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>1</v>
       </c>
@@ -793,53 +813,60 @@
         <v>33</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>1</v>
+        <v>33</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3" t="s">
+      <c r="E8" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="G8" s="3" t="s">
+      <c r="H8" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="H8" s="3"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I8" s="3"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>63</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3" t="s">
+      <c r="C9" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="E9" s="3"/>
       <c r="F9" s="3"/>
-      <c r="G9" s="3" t="s">
+      <c r="G9" s="3"/>
+      <c r="H9" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="H9" s="3"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I9" s="3"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
-      <c r="D10" s="3" t="s">
+      <c r="D10" s="3"/>
+      <c r="E10" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E10" s="3"/>
       <c r="F10" s="3"/>
       <c r="G10" s="3"/>
       <c r="H10" s="3"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I10" s="3"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>3</v>
       </c>
@@ -847,55 +874,64 @@
         <v>18</v>
       </c>
       <c r="C11" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D11" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="D11" s="3" t="s">
+      <c r="E11" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E11" s="3"/>
       <c r="F11" s="3"/>
       <c r="G11" s="3"/>
-      <c r="H11" s="3" t="s">
+      <c r="H11" s="3"/>
+      <c r="I11" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>19</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3" t="s">
+      <c r="C12" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="E12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3" t="s">
+        <v>19</v>
+      </c>
       <c r="F12" s="3"/>
-      <c r="G12" s="3" t="s">
+      <c r="G12" s="3"/>
+      <c r="H12" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="H12" s="3"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I12" s="3"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>20</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3" t="s">
+      <c r="C13" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="E13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3" t="s">
+        <v>20</v>
+      </c>
       <c r="F13" s="3"/>
-      <c r="G13" s="3" t="s">
+      <c r="G13" s="3"/>
+      <c r="H13" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="H13" s="3"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I13" s="3"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>21</v>
       </c>
@@ -903,43 +939,49 @@
         <v>28</v>
       </c>
       <c r="C14" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D14" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D14" s="3" t="s">
+      <c r="E14" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3" t="s">
+      <c r="F14" s="3"/>
+      <c r="G14" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="G14" s="3" t="s">
+      <c r="H14" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="H14" s="3" t="s">
+      <c r="I14" s="3" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>41</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3" t="s">
+      <c r="C15" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3" t="s">
+      <c r="D15" s="3"/>
+      <c r="E15" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="G15" s="3" t="s">
+      <c r="H15" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="H15" s="3"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I15" s="3"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>34</v>
       </c>
@@ -947,53 +989,56 @@
         <v>34</v>
       </c>
       <c r="C16" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D16" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="D16" s="3"/>
       <c r="E16" s="3"/>
-      <c r="F16" s="3" t="s">
-        <v>34</v>
-      </c>
+      <c r="F16" s="3"/>
       <c r="G16" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="H16" s="3"/>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H16" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="I16" s="3"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="D17" s="1" t="s">
+      <c r="E17" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="F17" s="3" t="s">
+      <c r="G17" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="H17" s="3" t="s">
+      <c r="I17" s="3" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="D18" s="1" t="s">
+      <c r="E18" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="F18" s="3" t="s">
+      <c r="G18" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="H18" s="3" t="s">
+      <c r="I18" s="3" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="F26" s="3"/>
-      <c r="H26" s="3"/>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="F27" s="3"/>
-      <c r="H27" s="3"/>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G26" s="3"/>
+      <c r="I26" s="3"/>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G27" s="3"/>
+      <c r="I27" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -1005,7 +1050,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
update cell type mapping (purified immune cell dataset)
</commit_message>
<xml_diff>
--- a/inst/extdata/cell_type_mapping.xlsx
+++ b/inst/extdata/cell_type_mapping.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="151">
   <si>
     <t>IKDC</t>
   </si>
@@ -474,6 +474,12 @@
   </si>
   <si>
     <t>DC activated</t>
+  </si>
+  <si>
+    <t>quantiseq_reference</t>
+  </si>
+  <si>
+    <t>T cells CD4</t>
   </si>
 </sst>
 </file>
@@ -1379,107 +1385,135 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B20"/>
+  <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="27.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>54</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C1" s="2" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>55</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C2" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>56</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C3" s="1" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>57</v>
       </c>
       <c r="B4" s="1"/>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>58</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>147</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>146</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>148</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C9" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C10" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>59</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C11" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B12" s="1"/>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>3</v>
       </c>
@@ -1487,45 +1521,60 @@
         <v>65</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>18</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C14" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>19</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C15" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>20</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C16" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>37</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C17" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>30</v>
       </c>
       <c r="B18" s="1"/>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C18" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>39</v>
       </c>
@@ -1533,7 +1582,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>68</v>
       </c>
@@ -1543,6 +1592,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
@@ -1550,7 +1600,7 @@
           <x14:formula1>
             <xm:f>available_signatures!$H$2:$H$35</xm:f>
           </x14:formula1>
-          <xm:sqref>B2:B7 B22:B30 B9:B20</xm:sqref>
+          <xm:sqref>B2:B7 B22:B30 B9:B20 C9:C10</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
add new validation datasets to mapping
</commit_message>
<xml_diff>
--- a/inst/extdata/cell_type_mapping.xlsx
+++ b/inst/extdata/cell_type_mapping.xlsx
@@ -9,13 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11370" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="celltype2method" sheetId="3" r:id="rId1"/>
     <sheet name="celltype2dataset" sheetId="4" r:id="rId2"/>
-    <sheet name="available_signatures" sheetId="5" r:id="rId3"/>
-    <sheet name="extended mapping" sheetId="2" r:id="rId4"/>
+    <sheet name="hierarchy" sheetId="6" r:id="rId3"/>
+    <sheet name="available_signatures" sheetId="5" r:id="rId4"/>
+    <sheet name="extended mapping" sheetId="2" r:id="rId5"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="170">
   <si>
     <t>IKDC</t>
   </si>
@@ -480,6 +481,63 @@
   </si>
   <si>
     <t>T cells CD4</t>
+  </si>
+  <si>
+    <t>hoeck</t>
+  </si>
+  <si>
+    <t>mono</t>
+  </si>
+  <si>
+    <t>NK</t>
+  </si>
+  <si>
+    <t>Tcell</t>
+  </si>
+  <si>
+    <t>zimmermann</t>
+  </si>
+  <si>
+    <t>CD4 T cells</t>
+  </si>
+  <si>
+    <t>racle</t>
+  </si>
+  <si>
+    <t>parent of</t>
+  </si>
+  <si>
+    <t>root</t>
+  </si>
+  <si>
+    <t>immune cell</t>
+  </si>
+  <si>
+    <t>other cell</t>
+  </si>
+  <si>
+    <t>cancer cell</t>
+  </si>
+  <si>
+    <t>B cell</t>
+  </si>
+  <si>
+    <t>T cell</t>
+  </si>
+  <si>
+    <t>Monocyte</t>
+  </si>
+  <si>
+    <t>NK cell</t>
+  </si>
+  <si>
+    <t>Dendritic cell</t>
+  </si>
+  <si>
+    <t>M1 Macrophage</t>
+  </si>
+  <si>
+    <t>M2 Macrophge</t>
   </si>
 </sst>
 </file>
@@ -872,7 +930,7 @@
   <dimension ref="A1:I29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A20"/>
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1385,19 +1443,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C20"/>
+  <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="27.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>54</v>
       </c>
@@ -1407,8 +1466,17 @@
       <c r="C1" s="2" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>55</v>
       </c>
@@ -1418,8 +1486,17 @@
       <c r="C2" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2" t="s">
+        <v>154</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="F2" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>56</v>
       </c>
@@ -1429,14 +1506,27 @@
       <c r="C3" s="1" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D3" t="s">
+        <v>154</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="F3" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>57</v>
       </c>
       <c r="B4" s="1"/>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D4" t="s">
+        <v>154</v>
+      </c>
+      <c r="E4" s="1"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>58</v>
       </c>
@@ -1446,8 +1536,17 @@
       <c r="C5" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D5" t="s">
+        <v>154</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="F5" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>147</v>
       </c>
@@ -1457,8 +1556,17 @@
       <c r="C6" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D6" t="s">
+        <v>153</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>146</v>
       </c>
@@ -1468,13 +1576,23 @@
       <c r="C7" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D7" t="s">
+        <v>153</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E8" s="1"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>148</v>
       </c>
@@ -1484,8 +1602,9 @@
       <c r="C9" s="1" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E9" s="1"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>1</v>
       </c>
@@ -1495,8 +1614,14 @@
       <c r="C10" s="1" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D10" t="s">
+        <v>1</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>59</v>
       </c>
@@ -1506,22 +1631,33 @@
       <c r="C11" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D11" t="s">
+        <v>154</v>
+      </c>
+      <c r="E11" s="1"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B12" s="1"/>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E12" s="1"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D13" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>18</v>
       </c>
@@ -1531,8 +1667,14 @@
       <c r="C14" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D14" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>19</v>
       </c>
@@ -1542,8 +1684,14 @@
       <c r="C15" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D15" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>20</v>
       </c>
@@ -1553,8 +1701,17 @@
       <c r="C16" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D16" t="s">
+        <v>48</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="F16" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>37</v>
       </c>
@@ -1564,8 +1721,14 @@
       <c r="C17" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D17" t="s">
+        <v>152</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>30</v>
       </c>
@@ -1573,22 +1736,25 @@
       <c r="C18" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E18" s="1"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>39</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E19" s="1"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>68</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>68</v>
       </c>
+      <c r="E20" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1609,6 +1775,125 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F32" sqref="F32"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B1" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>160</v>
+      </c>
+      <c r="B3" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>161</v>
+      </c>
+      <c r="B4" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>162</v>
+      </c>
+      <c r="B5" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>163</v>
+      </c>
+      <c r="B6" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>164</v>
+      </c>
+      <c r="B7" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>165</v>
+      </c>
+      <c r="B8" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>166</v>
+      </c>
+      <c r="B9" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>167</v>
+      </c>
+      <c r="B11" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>168</v>
+      </c>
+      <c r="B12" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>169</v>
+      </c>
+      <c r="B13" t="s">
+        <v>25</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O68"/>
   <sheetViews>
@@ -2934,7 +3219,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H27"/>
   <sheetViews>

</xml_diff>

<commit_message>
add possibility to define cell types as 'optional'
</commit_message>
<xml_diff>
--- a/inst/extdata/cell_type_mapping.xlsx
+++ b/inst/extdata/cell_type_mapping.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="44160" windowHeight="10275" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="10875" windowHeight="10275" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="controlled_vocabulary" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="542" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="582" uniqueCount="190">
   <si>
     <t xml:space="preserve">controlled vocabulary is a list of entities (cell types) of different granularity (e.g. T cell, CD8 T cell). We use this vocabulary to build a tree and to map cell type names between different methods/datasets. </t>
   </si>
@@ -151,9 +151,6 @@
     <t>parent</t>
   </si>
   <si>
-    <t xml:space="preserve">would they appear as t cell in a flow cytometry panel? </t>
-  </si>
-  <si>
     <t>cell</t>
   </si>
   <si>
@@ -575,6 +572,30 @@
   </si>
   <si>
     <t>Melanoma cell</t>
+  </si>
+  <si>
+    <t>quantiseq_reference</t>
+  </si>
+  <si>
+    <t>T cells CD4</t>
+  </si>
+  <si>
+    <t>optional</t>
+  </si>
+  <si>
+    <t>only in cibersort, still count all other subtypes as "all t cells" if they do not predict gdT</t>
+  </si>
+  <si>
+    <t>only in cibersort, still count all other subtypes as "all t cells" if they do only distinguish M1/M2</t>
+  </si>
+  <si>
+    <t>test_method1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">method for unit test. </t>
+  </si>
+  <si>
+    <t>Macrophages.M0</t>
   </si>
 </sst>
 </file>
@@ -984,14 +1005,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O43"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A43" sqref="A43"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="30.140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="21.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="22.85546875" style="1" customWidth="1"/>
     <col min="4" max="14" width="9.140625" style="1"/>
     <col min="15" max="15" width="27.140625" style="1" bestFit="1" customWidth="1"/>
@@ -999,13 +1020,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
     </row>
@@ -1014,7 +1038,7 @@
         <v>4</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
@@ -1062,7 +1086,7 @@
         <v>14</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
@@ -1070,7 +1094,7 @@
         <v>16</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
@@ -1092,16 +1116,19 @@
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
+      </c>
+      <c r="C12" s="1" t="b">
+        <v>1</v>
       </c>
       <c r="O12" s="2"/>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>10</v>
@@ -1110,13 +1137,16 @@
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C14" s="1" t="s">
-        <v>41</v>
+      <c r="C14" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>185</v>
       </c>
       <c r="O14" s="2"/>
     </row>
@@ -1149,7 +1179,7 @@
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>13</v>
@@ -1248,7 +1278,7 @@
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>29</v>
@@ -1260,7 +1290,7 @@
         <v>31</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="O30" s="2"/>
     </row>
@@ -1269,7 +1299,7 @@
         <v>30</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.25">
@@ -1279,6 +1309,12 @@
       <c r="B32" s="1" t="s">
         <v>30</v>
       </c>
+      <c r="C32" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>186</v>
+      </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
@@ -1325,12 +1361,12 @@
         <v>5</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>5</v>
@@ -1338,7 +1374,7 @@
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B40" s="1" t="s">
         <v>5</v>
@@ -1354,7 +1390,7 @@
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B42" s="1" t="s">
         <v>6</v>
@@ -1362,7 +1398,7 @@
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B43" s="1" t="s">
         <v>6</v>
@@ -1370,7 +1406,7 @@
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B39:B1048576 B30:B37 B3:B28 B1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B39:B1048576 B30:B37 B1 B3:B7 B10:B11 B13:B28">
       <formula1>$A:$A</formula1>
     </dataValidation>
   </dataValidations>
@@ -1381,39 +1417,39 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E168"/>
+  <dimension ref="A1:E180"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A139" workbookViewId="0">
-      <selection activeCell="C165" sqref="C165"/>
+    <sheetView tabSelected="1" topLeftCell="A157" workbookViewId="0">
+      <selection activeCell="A181" sqref="A181"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="26.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="29.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>43</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>44</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C2" t="s">
         <v>21</v>
@@ -1421,10 +1457,10 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C3" t="s">
         <v>22</v>
@@ -1432,21 +1468,21 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C5" t="s">
         <v>9</v>
@@ -1454,10 +1490,10 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C6" t="s">
         <v>14</v>
@@ -1465,10 +1501,10 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C7" t="s">
         <v>15</v>
@@ -1476,10 +1512,10 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C8" t="s">
         <v>17</v>
@@ -1487,43 +1523,43 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>18</v>
       </c>
       <c r="C9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>19</v>
       </c>
       <c r="C10" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="13" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>20</v>
       </c>
       <c r="C11" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="13" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C12" t="s">
         <v>24</v>
@@ -1531,10 +1567,10 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="13" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C13" t="s">
         <v>25</v>
@@ -1542,10 +1578,10 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="13" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C14" t="s">
         <v>31</v>
@@ -1553,10 +1589,10 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="13" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C15" t="s">
         <v>37</v>
@@ -1564,10 +1600,10 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="13" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C16" t="s">
         <v>38</v>
@@ -1575,10 +1611,10 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="13" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C17" t="s">
         <v>39</v>
@@ -1586,10 +1622,10 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="13" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C18" t="s">
         <v>35</v>
@@ -1597,10 +1633,10 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="13" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C19" t="s">
         <v>36</v>
@@ -1608,10 +1644,10 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="13" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C20" t="s">
         <v>28</v>
@@ -1619,10 +1655,10 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="13" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C21" t="s">
         <v>27</v>
@@ -1630,10 +1666,10 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="13" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C22" t="s">
         <v>33</v>
@@ -1642,10 +1678,10 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="13" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C23" t="s">
         <v>32</v>
@@ -1653,10 +1689,10 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="13" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B24" s="12" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C24" s="13" t="s">
         <v>21</v>
@@ -1664,10 +1700,10 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="13" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B25" s="12" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C25" s="13" t="s">
         <v>22</v>
@@ -1675,21 +1711,21 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="13" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B26" s="12" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C26" s="13" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="13" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B27" s="12" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C27" s="13" t="s">
         <v>9</v>
@@ -1697,10 +1733,10 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="13" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B28" s="12" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C28" s="13" t="s">
         <v>14</v>
@@ -1708,10 +1744,10 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="13" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B29" s="12" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C29" s="13" t="s">
         <v>15</v>
@@ -1719,10 +1755,10 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="13" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B30" s="12" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C30" s="13" t="s">
         <v>17</v>
@@ -1730,43 +1766,43 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="13" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B31" s="12" t="s">
         <v>18</v>
       </c>
       <c r="C31" s="13" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="13" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B32" s="12" t="s">
         <v>19</v>
       </c>
       <c r="C32" s="13" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="13" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B33" s="12" t="s">
         <v>20</v>
       </c>
       <c r="C33" s="13" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="13" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B34" s="12" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C34" s="13" t="s">
         <v>24</v>
@@ -1774,10 +1810,10 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="13" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B35" s="12" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C35" s="13" t="s">
         <v>25</v>
@@ -1785,10 +1821,10 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="13" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B36" s="12" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C36" s="13" t="s">
         <v>31</v>
@@ -1796,10 +1832,10 @@
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="13" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B37" s="12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C37" s="13" t="s">
         <v>37</v>
@@ -1807,10 +1843,10 @@
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="13" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B38" s="12" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C38" s="13" t="s">
         <v>38</v>
@@ -1818,10 +1854,10 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="13" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B39" s="12" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C39" s="13" t="s">
         <v>39</v>
@@ -1829,10 +1865,10 @@
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="13" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B40" s="12" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C40" s="13" t="s">
         <v>35</v>
@@ -1840,10 +1876,10 @@
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="13" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B41" s="12" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C41" s="13" t="s">
         <v>36</v>
@@ -1851,10 +1887,10 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="13" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B42" s="12" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C42" s="13" t="s">
         <v>28</v>
@@ -1862,10 +1898,10 @@
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="13" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B43" s="12" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C43" s="13" t="s">
         <v>27</v>
@@ -1873,10 +1909,10 @@
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="13" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B44" s="12" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C44" s="13" t="s">
         <v>33</v>
@@ -1884,10 +1920,10 @@
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="13" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B45" s="12" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C45" s="13" t="s">
         <v>32</v>
@@ -1895,10 +1931,10 @@
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B46" s="5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C46" t="s">
         <v>13</v>
@@ -1906,10 +1942,10 @@
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" s="13" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B47" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C47" t="s">
         <v>10</v>
@@ -1917,10 +1953,10 @@
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="13" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B48" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C48" t="s">
         <v>9</v>
@@ -1928,7 +1964,7 @@
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" s="13" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B49" s="5" t="s">
         <v>32</v>
@@ -1939,7 +1975,7 @@
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" s="13" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B50" s="5" t="s">
         <v>30</v>
@@ -1950,10 +1986,10 @@
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" s="13" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B51" s="5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C51" t="s">
         <v>34</v>
@@ -1961,42 +1997,42 @@
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B52" s="7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" s="13" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B53" s="7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" s="13" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B54" s="7" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" s="13" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B55" s="7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" s="13" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B56" s="7" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C56" t="s">
         <v>13</v>
@@ -2004,10 +2040,10 @@
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" s="13" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B57" s="7" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C57" t="s">
         <v>16</v>
@@ -2015,10 +2051,10 @@
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" s="13" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B58" s="7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C58" t="s">
         <v>14</v>
@@ -2026,10 +2062,10 @@
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" s="13" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B59" s="7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C59" t="s">
         <v>11</v>
@@ -2037,34 +2073,34 @@
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" s="13" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B60" s="7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" s="13" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B61" s="7" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" s="13" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B62" s="7" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" s="13" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B63" s="7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C63" t="s">
         <v>9</v>
@@ -2072,66 +2108,66 @@
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" s="13" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B64" s="7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" s="13" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B65" s="7" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" s="13" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B66" s="7" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" s="13" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B67" s="7" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" s="13" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B68" s="7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" s="13" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B69" s="7" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" s="13" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B70" s="7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" s="13" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B71" s="7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C71" t="s">
         <v>34</v>
@@ -2139,21 +2175,21 @@
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" s="13" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B72" s="7" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C72" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" s="13" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B73" s="7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C73" t="s">
         <v>33</v>
@@ -2161,85 +2197,85 @@
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" s="13" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B74" s="7" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" s="13" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B75" s="7" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" s="13" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B76" s="7" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C76" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" s="13" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B77" s="7" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" s="13" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B78" s="7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" s="13" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B79" s="7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" s="13" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B80" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" s="13" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B81" s="7" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" s="13" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B82" s="7" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" s="13" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B83" s="7" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C83" t="s">
         <v>30</v>
@@ -2247,10 +2283,10 @@
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" s="13" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B84" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C84" t="s">
         <v>38</v>
@@ -2258,10 +2294,10 @@
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" s="13" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B85" s="7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C85" t="s">
         <v>39</v>
@@ -2269,10 +2305,10 @@
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" s="13" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B86" s="7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C86" t="s">
         <v>26</v>
@@ -2280,50 +2316,50 @@
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" s="13" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B87" s="7" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88" s="13" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B88" s="7" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89" s="13" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B89" s="7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90" s="13" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B90" s="7" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91" s="13" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B91" s="7" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92" s="13" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B92" s="7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C92" t="s">
         <v>31</v>
@@ -2331,58 +2367,58 @@
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93" s="13" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B93" s="7" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94" s="13" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B94" s="7" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95" s="13" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B95" s="7" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96" s="13" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B96" s="7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97" s="13" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B97" s="7" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98" s="13" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B98" s="7" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99" s="13" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B99" s="7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C99" t="s">
         <v>32</v>
@@ -2390,10 +2426,10 @@
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100" s="13" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B100" s="7" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C100" t="s">
         <v>12</v>
@@ -2401,157 +2437,157 @@
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101" s="13" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B101" s="7" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102" s="13" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B102" s="7" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103" s="13" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B103" s="7" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A104" s="13" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B104" s="7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105" s="13" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B105" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A106" s="13" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B106" s="7" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A107" s="13" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B107" s="7" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A108" s="13" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B108" s="7" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A109" s="13" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B109" s="7" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A110" s="13" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B110" s="7" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A111" s="13" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B111" s="7" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A112" s="13" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B112" s="7" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A113" s="13" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B113" s="7" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A114" s="13" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B114" s="7" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A115" s="13" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B115" s="7" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C115" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A116" s="13" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B116" s="7" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A117" s="13" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B117" s="7" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A118" s="13" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B118" s="7" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B119" s="8" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C119" t="s">
         <v>7</v>
@@ -2559,29 +2595,29 @@
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A120" s="13" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B120" s="8" t="s">
-        <v>134</v>
+        <v>133</v>
+      </c>
+      <c r="C120" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A121" s="13" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B121" s="8" t="s">
-        <v>135</v>
-      </c>
-      <c r="C121" t="s">
-        <v>9</v>
+        <v>134</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A122" s="13" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B122" s="8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C122" t="s">
         <v>12</v>
@@ -2589,10 +2625,10 @@
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A123" s="13" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B123" s="8" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C123" t="s">
         <v>13</v>
@@ -2600,7 +2636,7 @@
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A124" s="13" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B124" s="8" t="s">
         <v>29</v>
@@ -2611,10 +2647,10 @@
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A125" s="13" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B125" s="8" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C125" t="s">
         <v>34</v>
@@ -2622,10 +2658,10 @@
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A126" s="13" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B126" s="8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C126" t="s">
         <v>32</v>
@@ -2633,32 +2669,32 @@
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A127" s="13" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B127" s="8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C127" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A128" s="13" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B128" s="8" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C128" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B129" s="9" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C129" t="s">
         <v>13</v>
@@ -2666,10 +2702,10 @@
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A130" s="13" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B130" s="9" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C130" t="s">
         <v>38</v>
@@ -2677,10 +2713,10 @@
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A131" s="13" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B131" s="9" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C131" t="s">
         <v>39</v>
@@ -2688,10 +2724,10 @@
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A132" s="13" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B132" s="9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C132" t="s">
         <v>31</v>
@@ -2699,10 +2735,10 @@
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A133" s="13" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B133" s="9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C133" t="s">
         <v>32</v>
@@ -2710,10 +2746,10 @@
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A134" s="13" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B134" s="9" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C134" t="s">
         <v>12</v>
@@ -2721,10 +2757,10 @@
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A135" s="13" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B135" s="9" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C135" t="s">
         <v>11</v>
@@ -2732,10 +2768,10 @@
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A136" s="13" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B136" s="9" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C136" t="s">
         <v>9</v>
@@ -2743,21 +2779,21 @@
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A137" s="13" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B137" s="9" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C137" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A138" s="13" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B138" s="9" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C138" t="s">
         <v>34</v>
@@ -2765,10 +2801,10 @@
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B139" s="10" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C139" t="s">
         <v>13</v>
@@ -2776,21 +2812,21 @@
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A140" s="13" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B140" s="10" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C140" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A141" s="13" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B141" s="10" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C141" t="s">
         <v>10</v>
@@ -2798,10 +2834,10 @@
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A142" s="13" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B142" s="10" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C142" t="s">
         <v>9</v>
@@ -2809,21 +2845,21 @@
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A143" s="13" t="s">
+        <v>177</v>
+      </c>
+      <c r="B143" s="10" t="s">
+        <v>148</v>
+      </c>
+      <c r="C143" t="s">
         <v>178</v>
-      </c>
-      <c r="B143" s="10" t="s">
-        <v>149</v>
-      </c>
-      <c r="C143" t="s">
-        <v>179</v>
       </c>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A144" s="13" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B144" s="10" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C144" t="s">
         <v>30</v>
@@ -2831,10 +2867,10 @@
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A145" s="13" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B145" s="10" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C145" t="s">
         <v>12</v>
@@ -2842,18 +2878,18 @@
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A146" s="13" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B146" s="10" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B147" s="12" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C147" t="s">
         <v>13</v>
@@ -2861,10 +2897,10 @@
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A148" s="11" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B148" s="12" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C148" t="s">
         <v>9</v>
@@ -2872,21 +2908,21 @@
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A149" s="11" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B149" s="12" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C149" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A150" s="11" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B150" s="12" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C150" s="11" t="s">
         <v>11</v>
@@ -2894,51 +2930,51 @@
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A151" s="11" t="s">
+        <v>162</v>
+      </c>
+      <c r="B151" s="12" t="s">
+        <v>155</v>
+      </c>
+      <c r="C151" t="s">
         <v>163</v>
-      </c>
-      <c r="B151" s="12" t="s">
-        <v>156</v>
-      </c>
-      <c r="C151" t="s">
-        <v>164</v>
       </c>
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A152" s="11" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B152" s="12" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A153" s="11" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B153" s="12" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C153" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A154" s="11" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B154" s="12" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C154" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A155" s="11" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B155" s="12" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C155" t="s">
         <v>34</v>
@@ -2946,21 +2982,21 @@
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A156" s="11" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B156" s="12" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C156" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A157" s="11" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B157" s="12" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C157" t="s">
         <v>12</v>
@@ -2968,21 +3004,21 @@
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A158" s="11" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B158" s="12" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C158" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B159" s="13" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C159" t="s">
         <v>7</v>
@@ -2990,10 +3026,10 @@
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A160" s="13" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B160" s="13" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C160" t="s">
         <v>12</v>
@@ -3001,10 +3037,10 @@
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A161" s="13" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B161" s="13" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C161" t="s">
         <v>34</v>
@@ -3012,21 +3048,21 @@
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A162" s="13" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B162" s="13" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C162" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A163" s="13" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B163" s="13" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C163" t="s">
         <v>13</v>
@@ -3034,10 +3070,10 @@
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B164" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C164" t="s">
         <v>13</v>
@@ -3045,10 +3081,10 @@
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A165" s="13" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B165" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C165" t="s">
         <v>10</v>
@@ -3056,10 +3092,10 @@
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A166" s="13" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B166" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C166" t="s">
         <v>9</v>
@@ -3067,10 +3103,10 @@
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A167" s="13" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B167" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C167" t="s">
         <v>12</v>
@@ -3078,13 +3114,151 @@
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A168" s="13" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B168" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C168" t="s">
         <v>6</v>
+      </c>
+    </row>
+    <row r="169" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A169" t="s">
+        <v>182</v>
+      </c>
+      <c r="B169" t="s">
+        <v>151</v>
+      </c>
+      <c r="C169" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="170" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A170" s="13" t="s">
+        <v>182</v>
+      </c>
+      <c r="B170" t="s">
+        <v>159</v>
+      </c>
+      <c r="C170" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="171" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A171" s="13" t="s">
+        <v>182</v>
+      </c>
+      <c r="B171" t="s">
+        <v>55</v>
+      </c>
+      <c r="C171" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="172" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A172" s="13" t="s">
+        <v>182</v>
+      </c>
+      <c r="B172" t="s">
+        <v>56</v>
+      </c>
+      <c r="C172" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="173" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A173" s="13" t="s">
+        <v>182</v>
+      </c>
+      <c r="B173" t="s">
+        <v>53</v>
+      </c>
+      <c r="C173" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="174" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A174" s="13" t="s">
+        <v>182</v>
+      </c>
+      <c r="B174" t="s">
+        <v>62</v>
+      </c>
+      <c r="C174" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="175" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A175" s="13" t="s">
+        <v>182</v>
+      </c>
+      <c r="B175" t="s">
+        <v>113</v>
+      </c>
+      <c r="C175" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="176" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A176" s="13" t="s">
+        <v>182</v>
+      </c>
+      <c r="B176" t="s">
+        <v>183</v>
+      </c>
+      <c r="C176" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="177" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A177" s="13" t="s">
+        <v>182</v>
+      </c>
+      <c r="B177" t="s">
+        <v>47</v>
+      </c>
+      <c r="C177" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="178" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A178" s="13" t="s">
+        <v>182</v>
+      </c>
+      <c r="B178" t="s">
+        <v>127</v>
+      </c>
+      <c r="C178" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="179" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A179" s="13" t="s">
+        <v>187</v>
+      </c>
+      <c r="B179" s="12" t="s">
+        <v>138</v>
+      </c>
+      <c r="C179" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="D179" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="180" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A180" s="13" t="s">
+        <v>187</v>
+      </c>
+      <c r="B180" s="12" t="s">
+        <v>189</v>
+      </c>
+      <c r="C180" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="D180" s="13" t="s">
+        <v>188</v>
       </c>
     </row>
   </sheetData>
@@ -3098,7 +3272,7 @@
           <x14:formula1>
             <xm:f>controlled_vocabulary!$A:$A</xm:f>
           </x14:formula1>
-          <xm:sqref>C1:C1048576</xm:sqref>
+          <xm:sqref>C1:C120 C122:C1048576</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
update cell type mapping
</commit_message>
<xml_diff>
--- a/inst/extdata/cell_type_mapping.xlsx
+++ b/inst/extdata/cell_type_mapping.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="10875" windowHeight="10275"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11370"/>
   </bookViews>
   <sheets>
     <sheet name="controlled_vocabulary" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="582" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="586" uniqueCount="192">
   <si>
     <t xml:space="preserve">controlled vocabulary is a list of entities (cell types) of different granularity (e.g. T cell, CD8 T cell). We use this vocabulary to build a tree and to map cell type names between different methods/datasets. </t>
   </si>
@@ -70,9 +70,6 @@
     <t>B cell</t>
   </si>
   <si>
-    <t>T cell CD4+ naïve</t>
-  </si>
-  <si>
     <t>T cell CD4+ memory resting</t>
   </si>
   <si>
@@ -91,9 +88,6 @@
     <t>T cells gamma delta</t>
   </si>
   <si>
-    <t>B cell naïve</t>
-  </si>
-  <si>
     <t>B cell memory</t>
   </si>
   <si>
@@ -596,6 +590,18 @@
   </si>
   <si>
     <t>Macrophages.M0</t>
+  </si>
+  <si>
+    <t>T cell CD4+ naive</t>
+  </si>
+  <si>
+    <t>B cell naive</t>
+  </si>
+  <si>
+    <t>T cell CD8+ naive</t>
+  </si>
+  <si>
+    <t>T cell CD8+ memory</t>
   </si>
 </sst>
 </file>
@@ -1003,10 +1009,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O43"/>
+  <dimension ref="A1:O45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1024,10 +1030,10 @@
         <v>3</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>2</v>
@@ -1038,7 +1044,7 @@
         <v>4</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
@@ -1067,119 +1073,117 @@
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>10</v>
+        <v>190</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>11</v>
+        <v>191</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>15</v>
+        <v>188</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="O11" s="2"/>
+        <v>11</v>
+      </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>64</v>
+        <v>14</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C12" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="O12" s="2"/>
+        <v>15</v>
+      </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>65</v>
+        <v>16</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="O13" s="2"/>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C14" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="D14" s="1" t="s">
-        <v>185</v>
-      </c>
       <c r="O14" s="2"/>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>13</v>
+        <v>63</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="O15" s="2"/>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>21</v>
+        <v>64</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>13</v>
+        <v>7</v>
+      </c>
+      <c r="C16" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>183</v>
       </c>
       <c r="O16" s="2"/>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="O17" s="2"/>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>63</v>
+        <v>189</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>13</v>
@@ -1188,228 +1192,246 @@
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="O19" s="2"/>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>24</v>
+        <v>61</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="O20" s="2"/>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="O21" s="2"/>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="O22" s="2"/>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="O23" s="2"/>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>33</v>
+        <v>21</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>23</v>
+        <v>4</v>
       </c>
       <c r="O24" s="2"/>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="O25" s="2"/>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="O26" s="2"/>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="O27" s="2"/>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="O28" s="2"/>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>163</v>
+        <v>26</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="O29" s="2"/>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="C30" s="1" t="b">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="O30" s="2"/>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>30</v>
+        <v>161</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>163</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="O31" s="2"/>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>30</v>
+        <v>161</v>
       </c>
       <c r="C32" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="D32" s="1" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="O32" s="2"/>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C34" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B40" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B34" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="B39" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40" s="1" t="s">
-        <v>179</v>
-      </c>
-      <c r="B40" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>6</v>
+        <v>176</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="B42" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A43" s="1" t="s">
-        <v>181</v>
-      </c>
       <c r="B43" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="B45" s="1" t="s">
         <v>6</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B39:B1048576 B30:B37 B1 B3:B7 B10:B11 B13:B28">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B41:B1048576 B8:B9 B3:B6 B1 B15:B30 B12:B13 B32:B39">
       <formula1>$A:$A</formula1>
     </dataValidation>
   </dataValidations>
@@ -1422,8 +1444,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E180"/>
   <sheetViews>
-    <sheetView topLeftCell="A157" workbookViewId="0">
-      <selection activeCell="A181" sqref="A181"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1435,57 +1457,57 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C2" t="s">
-        <v>21</v>
+        <v>189</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C4" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C5" t="s">
         <v>9</v>
@@ -1493,242 +1515,242 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C6" t="s">
-        <v>14</v>
+        <v>188</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C9" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C10" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="13" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C11" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="13" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C12" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="13" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C13" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="13" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C14" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="13" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C15" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="13" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C16" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="13" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C17" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="13" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C18" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="13" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C19" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="13" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C20" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="13" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C21" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="13" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C22" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E22" s="13"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="13" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C23" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="13" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B24" s="12" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C24" s="13" t="s">
-        <v>21</v>
+        <v>189</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="13" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B25" s="12" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C25" s="13" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="13" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B26" s="12" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C26" s="13" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="13" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B27" s="12" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C27" s="13" t="s">
         <v>9</v>
@@ -1736,208 +1758,208 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="13" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B28" s="12" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C28" s="13" t="s">
-        <v>14</v>
+        <v>188</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="13" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B29" s="12" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C29" s="13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="13" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B30" s="12" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C30" s="13" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="13" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B31" s="12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C31" s="13" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="13" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B32" s="12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C32" s="13" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="13" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B33" s="12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C33" s="13" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="13" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B34" s="12" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C34" s="13" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="13" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B35" s="12" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C35" s="13" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="13" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B36" s="12" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C36" s="13" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="13" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B37" s="12" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C37" s="13" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="13" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B38" s="12" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C38" s="13" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="13" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B39" s="12" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C39" s="13" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="13" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B40" s="12" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C40" s="13" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="13" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B41" s="12" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C41" s="13" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="13" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B42" s="12" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C42" s="13" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="13" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B43" s="12" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C43" s="13" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="13" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B44" s="12" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C44" s="13" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="13" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B45" s="12" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C45" s="13" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B46" s="5" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C46" t="s">
         <v>13</v>
@@ -1945,10 +1967,10 @@
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" s="13" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B47" s="5" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C47" t="s">
         <v>10</v>
@@ -1956,10 +1978,10 @@
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="13" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B48" s="5" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C48" t="s">
         <v>9</v>
@@ -1967,75 +1989,75 @@
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" s="13" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B49" s="5" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C49" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" s="13" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B50" s="5" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C50" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" s="13" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B51" s="5" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C51" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B52" s="7" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" s="13" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B53" s="7" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" s="13" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B54" s="7" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" s="13" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B55" s="7" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" s="13" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B56" s="7" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C56" t="s">
         <v>13</v>
@@ -2043,32 +2065,32 @@
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" s="13" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B57" s="7" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C57" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" s="13" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B58" s="7" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C58" t="s">
-        <v>14</v>
+        <v>188</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" s="13" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B59" s="7" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C59" t="s">
         <v>11</v>
@@ -2076,34 +2098,34 @@
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" s="13" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B60" s="7" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" s="13" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B61" s="7" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" s="13" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B62" s="7" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" s="13" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B63" s="7" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C63" t="s">
         <v>9</v>
@@ -2111,328 +2133,328 @@
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" s="13" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B64" s="7" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" s="13" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B65" s="7" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" s="13" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B66" s="7" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" s="13" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B67" s="7" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" s="13" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B68" s="7" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" s="13" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B69" s="7" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" s="13" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B70" s="7" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" s="13" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B71" s="7" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C71" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" s="13" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B72" s="7" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C72" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" s="13" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B73" s="7" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C73" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" s="13" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B74" s="7" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" s="13" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B75" s="7" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" s="13" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B76" s="7" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C76" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" s="13" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B77" s="7" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" s="13" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B78" s="7" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" s="13" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B79" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" s="13" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B80" s="7" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" s="13" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B81" s="7" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" s="13" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B82" s="7" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" s="13" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B83" s="7" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C83" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" s="13" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B84" s="7" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C84" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" s="13" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B85" s="7" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C85" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" s="13" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B86" s="7" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C86" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" s="13" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B87" s="7" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88" s="13" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B88" s="7" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89" s="13" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B89" s="7" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90" s="13" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B90" s="7" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91" s="13" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B91" s="7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92" s="13" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B92" s="7" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C92" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93" s="13" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B93" s="7" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94" s="13" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B94" s="7" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95" s="13" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B95" s="7" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96" s="13" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B96" s="7" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97" s="13" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B97" s="7" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98" s="13" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B98" s="7" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99" s="13" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B99" s="7" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C99" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100" s="13" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B100" s="7" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C100" t="s">
         <v>12</v>
@@ -2440,157 +2462,157 @@
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101" s="13" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B101" s="7" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102" s="13" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B102" s="7" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103" s="13" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B103" s="7" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A104" s="13" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B104" s="7" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105" s="13" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B105" s="7" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A106" s="13" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B106" s="7" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A107" s="13" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B107" s="7" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A108" s="13" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B108" s="7" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A109" s="13" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B109" s="7" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A110" s="13" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B110" s="7" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A111" s="13" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B111" s="7" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A112" s="13" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B112" s="7" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A113" s="13" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B113" s="7" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A114" s="13" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B114" s="7" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A115" s="13" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B115" s="7" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C115" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A116" s="13" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B116" s="7" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A117" s="13" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B117" s="7" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A118" s="13" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B118" s="7" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B119" s="8" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C119" t="s">
         <v>7</v>
@@ -2598,10 +2620,10 @@
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A120" s="13" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B120" s="8" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C120" t="s">
         <v>9</v>
@@ -2609,18 +2631,18 @@
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A121" s="13" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B121" s="8" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A122" s="13" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B122" s="8" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C122" t="s">
         <v>12</v>
@@ -2628,10 +2650,10 @@
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A123" s="13" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B123" s="8" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C123" t="s">
         <v>13</v>
@@ -2639,65 +2661,65 @@
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A124" s="13" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B124" s="8" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C124" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A125" s="13" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B125" s="8" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C125" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A126" s="13" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B126" s="8" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C126" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A127" s="13" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B127" s="8" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C127" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A128" s="13" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B128" s="8" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C128" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B129" s="9" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C129" t="s">
         <v>13</v>
@@ -2705,54 +2727,54 @@
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A130" s="13" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B130" s="9" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C130" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A131" s="13" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B131" s="9" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C131" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A132" s="13" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B132" s="9" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C132" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A133" s="13" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B133" s="9" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C133" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A134" s="13" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B134" s="9" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C134" t="s">
         <v>12</v>
@@ -2760,10 +2782,10 @@
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A135" s="13" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B135" s="9" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C135" t="s">
         <v>11</v>
@@ -2771,10 +2793,10 @@
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A136" s="13" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B136" s="9" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C136" t="s">
         <v>9</v>
@@ -2782,32 +2804,32 @@
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A137" s="13" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B137" s="9" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C137" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A138" s="13" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B138" s="9" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C138" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B139" s="10" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C139" t="s">
         <v>13</v>
@@ -2815,21 +2837,21 @@
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A140" s="13" t="s">
+        <v>175</v>
+      </c>
+      <c r="B140" s="10" t="s">
+        <v>143</v>
+      </c>
+      <c r="C140" t="s">
         <v>177</v>
-      </c>
-      <c r="B140" s="10" t="s">
-        <v>145</v>
-      </c>
-      <c r="C140" t="s">
-        <v>179</v>
       </c>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A141" s="13" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B141" s="10" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C141" t="s">
         <v>10</v>
@@ -2837,10 +2859,10 @@
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A142" s="13" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B142" s="10" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C142" t="s">
         <v>9</v>
@@ -2848,32 +2870,32 @@
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A143" s="13" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B143" s="10" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C143" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A144" s="13" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B144" s="10" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C144" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A145" s="13" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B145" s="10" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C145" t="s">
         <v>12</v>
@@ -2881,18 +2903,18 @@
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A146" s="13" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B146" s="10" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B147" s="12" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C147" t="s">
         <v>13</v>
@@ -2900,10 +2922,10 @@
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A148" s="11" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B148" s="12" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C148" t="s">
         <v>9</v>
@@ -2911,21 +2933,21 @@
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A149" s="11" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B149" s="12" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C149" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A150" s="11" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B150" s="12" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C150" s="11" t="s">
         <v>11</v>
@@ -2933,73 +2955,73 @@
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A151" s="11" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B151" s="12" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C151" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A152" s="11" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B152" s="12" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A153" s="11" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B153" s="12" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C153" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A154" s="11" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B154" s="12" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C154" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A155" s="11" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B155" s="12" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C155" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A156" s="11" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B156" s="12" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C156" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A157" s="11" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B157" s="12" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C157" t="s">
         <v>12</v>
@@ -3007,21 +3029,21 @@
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A158" s="11" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B158" s="12" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C158" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B159" s="13" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C159" t="s">
         <v>7</v>
@@ -3029,10 +3051,10 @@
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A160" s="13" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B160" s="13" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C160" t="s">
         <v>12</v>
@@ -3040,32 +3062,32 @@
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A161" s="13" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B161" s="13" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C161" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A162" s="13" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B162" s="13" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C162" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A163" s="13" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B163" s="13" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C163" t="s">
         <v>13</v>
@@ -3073,10 +3095,10 @@
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B164" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C164" t="s">
         <v>13</v>
@@ -3084,10 +3106,10 @@
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A165" s="13" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B165" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C165" t="s">
         <v>10</v>
@@ -3095,10 +3117,10 @@
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A166" s="13" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B166" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C166" t="s">
         <v>9</v>
@@ -3106,10 +3128,10 @@
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A167" s="13" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B167" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C167" t="s">
         <v>12</v>
@@ -3117,10 +3139,10 @@
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A168" s="13" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B168" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C168" t="s">
         <v>6</v>
@@ -3128,10 +3150,10 @@
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B169" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C169" t="s">
         <v>13</v>
@@ -3139,65 +3161,65 @@
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A170" s="13" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B170" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C170" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A171" s="13" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B171" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C171" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A172" s="13" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B172" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C172" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="173" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A173" s="13" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B173" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C173" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="174" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A174" s="13" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B174" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C174" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="175" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A175" s="13" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B175" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C175" t="s">
         <v>12</v>
@@ -3205,10 +3227,10 @@
     </row>
     <row r="176" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A176" s="13" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B176" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C176" t="s">
         <v>10</v>
@@ -3216,10 +3238,10 @@
     </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A177" s="13" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B177" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C177" t="s">
         <v>9</v>
@@ -3227,41 +3249,41 @@
     </row>
     <row r="178" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A178" s="13" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B178" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C178" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A179" s="13" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B179" s="12" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C179" s="13" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D179" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="180" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A180" s="13" t="s">
+        <v>185</v>
+      </c>
+      <c r="B180" s="12" t="s">
         <v>187</v>
       </c>
-      <c r="B180" s="12" t="s">
-        <v>189</v>
-      </c>
       <c r="C180" s="13" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D180" s="13" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add dummy 'random' method
</commit_message>
<xml_diff>
--- a/inst/extdata/cell_type_mapping.xlsx
+++ b/inst/extdata/cell_type_mapping.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="586" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="601" uniqueCount="195">
   <si>
     <t xml:space="preserve">cell_type</t>
   </si>
@@ -592,6 +592,15 @@
   </si>
   <si>
     <t xml:space="preserve">Macrophages.M0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">random</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CD4+ Tcell</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CD8+ Tcell</t>
   </si>
   <si>
     <t xml:space="preserve">controlled vocabulary is a list of entities (cell types) of different granularity (e.g. T cell, CD8 T cell). We use this vocabulary to build a tree and to map cell type names between different methods/datasets. </t>
@@ -1191,10 +1200,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E180"/>
+  <dimension ref="A1:E185"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A142" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B184" activeCellId="0" sqref="B184"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A165" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G183" activeCellId="0" sqref="G183"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1226,7 +1235,7 @@
       <c r="B2" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="C2" s="5" t="s">
         <v>22</v>
       </c>
     </row>
@@ -1237,7 +1246,7 @@
       <c r="B3" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="C3" s="5" t="s">
         <v>23</v>
       </c>
     </row>
@@ -1248,7 +1257,7 @@
       <c r="B4" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="C4" s="5" t="s">
         <v>24</v>
       </c>
     </row>
@@ -1259,7 +1268,7 @@
       <c r="B5" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="C5" s="0" t="s">
+      <c r="C5" s="5" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1270,7 +1279,7 @@
       <c r="B6" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="C6" s="0" t="s">
+      <c r="C6" s="5" t="s">
         <v>13</v>
       </c>
     </row>
@@ -1281,7 +1290,7 @@
       <c r="B7" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="C7" s="0" t="s">
+      <c r="C7" s="5" t="s">
         <v>15</v>
       </c>
     </row>
@@ -1292,7 +1301,7 @@
       <c r="B8" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="C8" s="0" t="s">
+      <c r="C8" s="5" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1303,7 +1312,7 @@
       <c r="B9" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="C9" s="0" t="s">
+      <c r="C9" s="5" t="s">
         <v>17</v>
       </c>
     </row>
@@ -1314,7 +1323,7 @@
       <c r="B10" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="C10" s="0" t="s">
+      <c r="C10" s="5" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1325,7 +1334,7 @@
       <c r="B11" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="C11" s="0" t="s">
+      <c r="C11" s="5" t="s">
         <v>19</v>
       </c>
     </row>
@@ -1336,7 +1345,7 @@
       <c r="B12" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C12" s="0" t="s">
+      <c r="C12" s="5" t="s">
         <v>26</v>
       </c>
     </row>
@@ -1347,7 +1356,7 @@
       <c r="B13" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="C13" s="0" t="s">
+      <c r="C13" s="5" t="s">
         <v>27</v>
       </c>
     </row>
@@ -1358,7 +1367,7 @@
       <c r="B14" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="C14" s="0" t="s">
+      <c r="C14" s="5" t="s">
         <v>36</v>
       </c>
     </row>
@@ -1369,7 +1378,7 @@
       <c r="B15" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="C15" s="0" t="s">
+      <c r="C15" s="5" t="s">
         <v>38</v>
       </c>
     </row>
@@ -1380,7 +1389,7 @@
       <c r="B16" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="C16" s="0" t="s">
+      <c r="C16" s="5" t="s">
         <v>40</v>
       </c>
     </row>
@@ -1391,7 +1400,7 @@
       <c r="B17" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="C17" s="0" t="s">
+      <c r="C17" s="5" t="s">
         <v>41</v>
       </c>
     </row>
@@ -1402,7 +1411,7 @@
       <c r="B18" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="C18" s="0" t="s">
+      <c r="C18" s="5" t="s">
         <v>43</v>
       </c>
     </row>
@@ -1413,7 +1422,7 @@
       <c r="B19" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="C19" s="0" t="s">
+      <c r="C19" s="5" t="s">
         <v>44</v>
       </c>
     </row>
@@ -1424,7 +1433,7 @@
       <c r="B20" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="C20" s="0" t="s">
+      <c r="C20" s="5" t="s">
         <v>33</v>
       </c>
     </row>
@@ -1435,7 +1444,7 @@
       <c r="B21" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="C21" s="0" t="s">
+      <c r="C21" s="5" t="s">
         <v>32</v>
       </c>
     </row>
@@ -1446,7 +1455,7 @@
       <c r="B22" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="C22" s="0" t="s">
+      <c r="C22" s="5" t="s">
         <v>30</v>
       </c>
       <c r="E22" s="5"/>
@@ -1458,7 +1467,7 @@
       <c r="B23" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="C23" s="0" t="s">
+      <c r="C23" s="5" t="s">
         <v>29</v>
       </c>
     </row>
@@ -1711,7 +1720,7 @@
       <c r="B46" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="C46" s="0" t="s">
+      <c r="C46" s="5" t="s">
         <v>21</v>
       </c>
     </row>
@@ -1722,7 +1731,7 @@
       <c r="B47" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="C47" s="0" t="s">
+      <c r="C47" s="5" t="s">
         <v>11</v>
       </c>
     </row>
@@ -1733,7 +1742,7 @@
       <c r="B48" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="C48" s="0" t="s">
+      <c r="C48" s="5" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1744,7 +1753,7 @@
       <c r="B49" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="C49" s="0" t="s">
+      <c r="C49" s="5" t="s">
         <v>29</v>
       </c>
     </row>
@@ -1755,7 +1764,7 @@
       <c r="B50" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="C50" s="0" t="s">
+      <c r="C50" s="5" t="s">
         <v>37</v>
       </c>
     </row>
@@ -1766,7 +1775,7 @@
       <c r="B51" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="C51" s="0" t="s">
+      <c r="C51" s="5" t="s">
         <v>42</v>
       </c>
     </row>
@@ -1777,6 +1786,7 @@
       <c r="B52" s="4" t="s">
         <v>84</v>
       </c>
+      <c r="C52" s="5"/>
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="5" t="s">
@@ -1785,6 +1795,7 @@
       <c r="B53" s="4" t="s">
         <v>85</v>
       </c>
+      <c r="C53" s="5"/>
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="5" t="s">
@@ -1793,6 +1804,7 @@
       <c r="B54" s="4" t="s">
         <v>86</v>
       </c>
+      <c r="C54" s="5"/>
     </row>
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="5" t="s">
@@ -1801,6 +1813,7 @@
       <c r="B55" s="4" t="s">
         <v>87</v>
       </c>
+      <c r="C55" s="5"/>
     </row>
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="5" t="s">
@@ -1809,7 +1822,7 @@
       <c r="B56" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="C56" s="0" t="s">
+      <c r="C56" s="5" t="s">
         <v>21</v>
       </c>
     </row>
@@ -1820,7 +1833,7 @@
       <c r="B57" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="C57" s="0" t="s">
+      <c r="C57" s="5" t="s">
         <v>14</v>
       </c>
     </row>
@@ -1831,7 +1844,7 @@
       <c r="B58" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="C58" s="0" t="s">
+      <c r="C58" s="5" t="s">
         <v>13</v>
       </c>
     </row>
@@ -1842,7 +1855,7 @@
       <c r="B59" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="C59" s="0" t="s">
+      <c r="C59" s="5" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1853,6 +1866,7 @@
       <c r="B60" s="4" t="s">
         <v>92</v>
       </c>
+      <c r="C60" s="5"/>
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="5" t="s">
@@ -1861,6 +1875,7 @@
       <c r="B61" s="4" t="s">
         <v>93</v>
       </c>
+      <c r="C61" s="5"/>
     </row>
     <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="5" t="s">
@@ -1869,6 +1884,7 @@
       <c r="B62" s="4" t="s">
         <v>94</v>
       </c>
+      <c r="C62" s="5"/>
     </row>
     <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="5" t="s">
@@ -1877,7 +1893,7 @@
       <c r="B63" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="C63" s="0" t="s">
+      <c r="C63" s="5" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1888,6 +1904,7 @@
       <c r="B64" s="4" t="s">
         <v>96</v>
       </c>
+      <c r="C64" s="5"/>
     </row>
     <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="5" t="s">
@@ -1896,6 +1913,7 @@
       <c r="B65" s="4" t="s">
         <v>97</v>
       </c>
+      <c r="C65" s="5"/>
     </row>
     <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="5" t="s">
@@ -1904,6 +1922,7 @@
       <c r="B66" s="4" t="s">
         <v>98</v>
       </c>
+      <c r="C66" s="5"/>
     </row>
     <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="5" t="s">
@@ -1912,6 +1931,7 @@
       <c r="B67" s="4" t="s">
         <v>99</v>
       </c>
+      <c r="C67" s="5"/>
     </row>
     <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="5" t="s">
@@ -1920,6 +1940,7 @@
       <c r="B68" s="4" t="s">
         <v>100</v>
       </c>
+      <c r="C68" s="5"/>
     </row>
     <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="5" t="s">
@@ -1928,6 +1949,7 @@
       <c r="B69" s="4" t="s">
         <v>101</v>
       </c>
+      <c r="C69" s="5"/>
     </row>
     <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="5" t="s">
@@ -1936,6 +1958,7 @@
       <c r="B70" s="4" t="s">
         <v>102</v>
       </c>
+      <c r="C70" s="5"/>
     </row>
     <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="5" t="s">
@@ -1944,7 +1967,7 @@
       <c r="B71" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="C71" s="0" t="s">
+      <c r="C71" s="5" t="s">
         <v>42</v>
       </c>
     </row>
@@ -1955,7 +1978,7 @@
       <c r="B72" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="C72" s="0" t="s">
+      <c r="C72" s="5" t="s">
         <v>46</v>
       </c>
     </row>
@@ -1966,7 +1989,7 @@
       <c r="B73" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="C73" s="0" t="s">
+      <c r="C73" s="5" t="s">
         <v>30</v>
       </c>
     </row>
@@ -1977,6 +2000,7 @@
       <c r="B74" s="4" t="s">
         <v>104</v>
       </c>
+      <c r="C74" s="5"/>
     </row>
     <row r="75" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="5" t="s">
@@ -1985,6 +2009,7 @@
       <c r="B75" s="4" t="s">
         <v>105</v>
       </c>
+      <c r="C75" s="5"/>
     </row>
     <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="5" t="s">
@@ -1993,7 +2018,7 @@
       <c r="B76" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="C76" s="0" t="s">
+      <c r="C76" s="5" t="s">
         <v>47</v>
       </c>
     </row>
@@ -2004,6 +2029,7 @@
       <c r="B77" s="4" t="s">
         <v>107</v>
       </c>
+      <c r="C77" s="5"/>
     </row>
     <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="5" t="s">
@@ -2012,6 +2038,7 @@
       <c r="B78" s="4" t="s">
         <v>108</v>
       </c>
+      <c r="C78" s="5"/>
     </row>
     <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="5" t="s">
@@ -2020,6 +2047,7 @@
       <c r="B79" s="4" t="s">
         <v>109</v>
       </c>
+      <c r="C79" s="5"/>
     </row>
     <row r="80" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="5" t="s">
@@ -2028,6 +2056,7 @@
       <c r="B80" s="4" t="s">
         <v>110</v>
       </c>
+      <c r="C80" s="5"/>
     </row>
     <row r="81" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="5" t="s">
@@ -2036,6 +2065,7 @@
       <c r="B81" s="4" t="s">
         <v>111</v>
       </c>
+      <c r="C81" s="5"/>
     </row>
     <row r="82" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="5" t="s">
@@ -2044,6 +2074,7 @@
       <c r="B82" s="4" t="s">
         <v>112</v>
       </c>
+      <c r="C82" s="5"/>
     </row>
     <row r="83" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="5" t="s">
@@ -2052,7 +2083,7 @@
       <c r="B83" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="C83" s="0" t="s">
+      <c r="C83" s="5" t="s">
         <v>37</v>
       </c>
     </row>
@@ -2063,7 +2094,7 @@
       <c r="B84" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="C84" s="0" t="s">
+      <c r="C84" s="5" t="s">
         <v>40</v>
       </c>
     </row>
@@ -2074,7 +2105,7 @@
       <c r="B85" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="C85" s="0" t="s">
+      <c r="C85" s="5" t="s">
         <v>41</v>
       </c>
     </row>
@@ -2085,7 +2116,7 @@
       <c r="B86" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="C86" s="0" t="s">
+      <c r="C86" s="5" t="s">
         <v>31</v>
       </c>
     </row>
@@ -2096,6 +2127,7 @@
       <c r="B87" s="4" t="s">
         <v>115</v>
       </c>
+      <c r="C87" s="5"/>
     </row>
     <row r="88" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="5" t="s">
@@ -2104,6 +2136,7 @@
       <c r="B88" s="4" t="s">
         <v>116</v>
       </c>
+      <c r="C88" s="5"/>
     </row>
     <row r="89" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="5" t="s">
@@ -2112,6 +2145,7 @@
       <c r="B89" s="4" t="s">
         <v>117</v>
       </c>
+      <c r="C89" s="5"/>
     </row>
     <row r="90" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="5" t="s">
@@ -2120,6 +2154,7 @@
       <c r="B90" s="4" t="s">
         <v>118</v>
       </c>
+      <c r="C90" s="5"/>
     </row>
     <row r="91" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="5" t="s">
@@ -2128,6 +2163,7 @@
       <c r="B91" s="4" t="s">
         <v>119</v>
       </c>
+      <c r="C91" s="5"/>
     </row>
     <row r="92" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="5" t="s">
@@ -2136,7 +2172,7 @@
       <c r="B92" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="C92" s="0" t="s">
+      <c r="C92" s="5" t="s">
         <v>36</v>
       </c>
     </row>
@@ -2147,6 +2183,7 @@
       <c r="B93" s="4" t="s">
         <v>120</v>
       </c>
+      <c r="C93" s="5"/>
     </row>
     <row r="94" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="5" t="s">
@@ -2155,6 +2192,7 @@
       <c r="B94" s="4" t="s">
         <v>121</v>
       </c>
+      <c r="C94" s="5"/>
     </row>
     <row r="95" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="5" t="s">
@@ -2163,6 +2201,7 @@
       <c r="B95" s="4" t="s">
         <v>122</v>
       </c>
+      <c r="C95" s="5"/>
     </row>
     <row r="96" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="5" t="s">
@@ -2171,6 +2210,7 @@
       <c r="B96" s="4" t="s">
         <v>123</v>
       </c>
+      <c r="C96" s="5"/>
     </row>
     <row r="97" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="5" t="s">
@@ -2179,6 +2219,7 @@
       <c r="B97" s="4" t="s">
         <v>124</v>
       </c>
+      <c r="C97" s="5"/>
     </row>
     <row r="98" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="5" t="s">
@@ -2187,6 +2228,7 @@
       <c r="B98" s="4" t="s">
         <v>125</v>
       </c>
+      <c r="C98" s="5"/>
     </row>
     <row r="99" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="5" t="s">
@@ -2195,7 +2237,7 @@
       <c r="B99" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="C99" s="0" t="s">
+      <c r="C99" s="5" t="s">
         <v>29</v>
       </c>
     </row>
@@ -2206,7 +2248,7 @@
       <c r="B100" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="C100" s="0" t="s">
+      <c r="C100" s="5" t="s">
         <v>25</v>
       </c>
     </row>
@@ -2217,6 +2259,7 @@
       <c r="B101" s="4" t="s">
         <v>127</v>
       </c>
+      <c r="C101" s="5"/>
     </row>
     <row r="102" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="5" t="s">
@@ -2225,6 +2268,7 @@
       <c r="B102" s="4" t="s">
         <v>128</v>
       </c>
+      <c r="C102" s="5"/>
     </row>
     <row r="103" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="5" t="s">
@@ -2233,6 +2277,7 @@
       <c r="B103" s="4" t="s">
         <v>129</v>
       </c>
+      <c r="C103" s="5"/>
     </row>
     <row r="104" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="5" t="s">
@@ -2241,6 +2286,7 @@
       <c r="B104" s="4" t="s">
         <v>130</v>
       </c>
+      <c r="C104" s="5"/>
     </row>
     <row r="105" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="5" t="s">
@@ -2249,6 +2295,7 @@
       <c r="B105" s="4" t="s">
         <v>57</v>
       </c>
+      <c r="C105" s="5"/>
     </row>
     <row r="106" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="5" t="s">
@@ -2257,6 +2304,7 @@
       <c r="B106" s="4" t="s">
         <v>131</v>
       </c>
+      <c r="C106" s="5"/>
     </row>
     <row r="107" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="5" t="s">
@@ -2265,6 +2313,7 @@
       <c r="B107" s="4" t="s">
         <v>132</v>
       </c>
+      <c r="C107" s="5"/>
     </row>
     <row r="108" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="5" t="s">
@@ -2273,6 +2322,7 @@
       <c r="B108" s="4" t="s">
         <v>133</v>
       </c>
+      <c r="C108" s="5"/>
     </row>
     <row r="109" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="5" t="s">
@@ -2281,6 +2331,7 @@
       <c r="B109" s="4" t="s">
         <v>134</v>
       </c>
+      <c r="C109" s="5"/>
     </row>
     <row r="110" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="5" t="s">
@@ -2289,6 +2340,7 @@
       <c r="B110" s="4" t="s">
         <v>135</v>
       </c>
+      <c r="C110" s="5"/>
     </row>
     <row r="111" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="5" t="s">
@@ -2297,6 +2349,7 @@
       <c r="B111" s="4" t="s">
         <v>136</v>
       </c>
+      <c r="C111" s="5"/>
     </row>
     <row r="112" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="5" t="s">
@@ -2305,6 +2358,7 @@
       <c r="B112" s="4" t="s">
         <v>137</v>
       </c>
+      <c r="C112" s="5"/>
     </row>
     <row r="113" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="5" t="s">
@@ -2313,6 +2367,7 @@
       <c r="B113" s="4" t="s">
         <v>138</v>
       </c>
+      <c r="C113" s="5"/>
     </row>
     <row r="114" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="5" t="s">
@@ -2321,6 +2376,7 @@
       <c r="B114" s="4" t="s">
         <v>139</v>
       </c>
+      <c r="C114" s="5"/>
     </row>
     <row r="115" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="5" t="s">
@@ -2329,7 +2385,7 @@
       <c r="B115" s="4" t="s">
         <v>140</v>
       </c>
-      <c r="C115" s="0" t="s">
+      <c r="C115" s="5" t="s">
         <v>18</v>
       </c>
     </row>
@@ -2340,6 +2396,7 @@
       <c r="B116" s="4" t="s">
         <v>141</v>
       </c>
+      <c r="C116" s="5"/>
     </row>
     <row r="117" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="5" t="s">
@@ -2348,6 +2405,7 @@
       <c r="B117" s="4" t="s">
         <v>142</v>
       </c>
+      <c r="C117" s="5"/>
     </row>
     <row r="118" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="5" t="s">
@@ -2356,6 +2414,7 @@
       <c r="B118" s="4" t="s">
         <v>143</v>
       </c>
+      <c r="C118" s="5"/>
     </row>
     <row r="119" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="0" t="s">
@@ -2364,7 +2423,7 @@
       <c r="B119" s="4" t="s">
         <v>145</v>
       </c>
-      <c r="C119" s="0" t="s">
+      <c r="C119" s="5" t="s">
         <v>7</v>
       </c>
     </row>
@@ -2375,7 +2434,7 @@
       <c r="B120" s="4" t="s">
         <v>146</v>
       </c>
-      <c r="C120" s="0" t="s">
+      <c r="C120" s="5" t="s">
         <v>8</v>
       </c>
     </row>
@@ -2394,7 +2453,7 @@
       <c r="B122" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="C122" s="0" t="s">
+      <c r="C122" s="5" t="s">
         <v>25</v>
       </c>
     </row>
@@ -2405,7 +2464,7 @@
       <c r="B123" s="4" t="s">
         <v>148</v>
       </c>
-      <c r="C123" s="0" t="s">
+      <c r="C123" s="5" t="s">
         <v>21</v>
       </c>
     </row>
@@ -2416,7 +2475,7 @@
       <c r="B124" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="C124" s="0" t="s">
+      <c r="C124" s="5" t="s">
         <v>34</v>
       </c>
     </row>
@@ -2427,7 +2486,7 @@
       <c r="B125" s="4" t="s">
         <v>149</v>
       </c>
-      <c r="C125" s="0" t="s">
+      <c r="C125" s="5" t="s">
         <v>42</v>
       </c>
     </row>
@@ -2438,7 +2497,7 @@
       <c r="B126" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="C126" s="0" t="s">
+      <c r="C126" s="5" t="s">
         <v>29</v>
       </c>
     </row>
@@ -2449,7 +2508,7 @@
       <c r="B127" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="C127" s="0" t="s">
+      <c r="C127" s="5" t="s">
         <v>46</v>
       </c>
     </row>
@@ -2460,7 +2519,7 @@
       <c r="B128" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="C128" s="0" t="s">
+      <c r="C128" s="5" t="s">
         <v>47</v>
       </c>
     </row>
@@ -2471,7 +2530,7 @@
       <c r="B129" s="4" t="s">
         <v>151</v>
       </c>
-      <c r="C129" s="0" t="s">
+      <c r="C129" s="5" t="s">
         <v>21</v>
       </c>
     </row>
@@ -2482,7 +2541,7 @@
       <c r="B130" s="4" t="s">
         <v>152</v>
       </c>
-      <c r="C130" s="0" t="s">
+      <c r="C130" s="5" t="s">
         <v>40</v>
       </c>
     </row>
@@ -2493,7 +2552,7 @@
       <c r="B131" s="4" t="s">
         <v>153</v>
       </c>
-      <c r="C131" s="0" t="s">
+      <c r="C131" s="5" t="s">
         <v>41</v>
       </c>
     </row>
@@ -2504,7 +2563,7 @@
       <c r="B132" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="C132" s="0" t="s">
+      <c r="C132" s="5" t="s">
         <v>36</v>
       </c>
     </row>
@@ -2515,7 +2574,7 @@
       <c r="B133" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="C133" s="0" t="s">
+      <c r="C133" s="5" t="s">
         <v>29</v>
       </c>
     </row>
@@ -2526,7 +2585,7 @@
       <c r="B134" s="4" t="s">
         <v>154</v>
       </c>
-      <c r="C134" s="0" t="s">
+      <c r="C134" s="5" t="s">
         <v>25</v>
       </c>
     </row>
@@ -2537,7 +2596,7 @@
       <c r="B135" s="4" t="s">
         <v>155</v>
       </c>
-      <c r="C135" s="0" t="s">
+      <c r="C135" s="5" t="s">
         <v>12</v>
       </c>
     </row>
@@ -2548,7 +2607,7 @@
       <c r="B136" s="4" t="s">
         <v>156</v>
       </c>
-      <c r="C136" s="0" t="s">
+      <c r="C136" s="5" t="s">
         <v>8</v>
       </c>
     </row>
@@ -2559,7 +2618,7 @@
       <c r="B137" s="4" t="s">
         <v>140</v>
       </c>
-      <c r="C137" s="0" t="s">
+      <c r="C137" s="5" t="s">
         <v>18</v>
       </c>
     </row>
@@ -2570,7 +2629,7 @@
       <c r="B138" s="4" t="s">
         <v>157</v>
       </c>
-      <c r="C138" s="0" t="s">
+      <c r="C138" s="5" t="s">
         <v>42</v>
       </c>
     </row>
@@ -2581,7 +2640,7 @@
       <c r="B139" s="4" t="s">
         <v>159</v>
       </c>
-      <c r="C139" s="0" t="s">
+      <c r="C139" s="5" t="s">
         <v>21</v>
       </c>
     </row>
@@ -2592,7 +2651,7 @@
       <c r="B140" s="4" t="s">
         <v>160</v>
       </c>
-      <c r="C140" s="0" t="s">
+      <c r="C140" s="5" t="s">
         <v>47</v>
       </c>
     </row>
@@ -2603,7 +2662,7 @@
       <c r="B141" s="4" t="s">
         <v>161</v>
       </c>
-      <c r="C141" s="0" t="s">
+      <c r="C141" s="5" t="s">
         <v>11</v>
       </c>
     </row>
@@ -2614,7 +2673,7 @@
       <c r="B142" s="4" t="s">
         <v>162</v>
       </c>
-      <c r="C142" s="0" t="s">
+      <c r="C142" s="5" t="s">
         <v>8</v>
       </c>
     </row>
@@ -2625,7 +2684,7 @@
       <c r="B143" s="4" t="s">
         <v>163</v>
       </c>
-      <c r="C143" s="0" t="s">
+      <c r="C143" s="5" t="s">
         <v>46</v>
       </c>
     </row>
@@ -2636,7 +2695,7 @@
       <c r="B144" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="C144" s="0" t="s">
+      <c r="C144" s="5" t="s">
         <v>37</v>
       </c>
     </row>
@@ -2647,7 +2706,7 @@
       <c r="B145" s="4" t="s">
         <v>164</v>
       </c>
-      <c r="C145" s="0" t="s">
+      <c r="C145" s="5" t="s">
         <v>25</v>
       </c>
     </row>
@@ -2658,6 +2717,7 @@
       <c r="B146" s="4" t="s">
         <v>165</v>
       </c>
+      <c r="C146" s="5"/>
     </row>
     <row r="147" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A147" s="0" t="s">
@@ -2666,7 +2726,7 @@
       <c r="B147" s="4" t="s">
         <v>167</v>
       </c>
-      <c r="C147" s="0" t="s">
+      <c r="C147" s="5" t="s">
         <v>21</v>
       </c>
     </row>
@@ -2677,7 +2737,7 @@
       <c r="B148" s="4" t="s">
         <v>168</v>
       </c>
-      <c r="C148" s="0" t="s">
+      <c r="C148" s="5" t="s">
         <v>8</v>
       </c>
     </row>
@@ -2688,7 +2748,7 @@
       <c r="B149" s="4" t="s">
         <v>169</v>
       </c>
-      <c r="C149" s="0" t="s">
+      <c r="C149" s="5" t="s">
         <v>50</v>
       </c>
     </row>
@@ -2710,7 +2770,7 @@
       <c r="B151" s="4" t="s">
         <v>171</v>
       </c>
-      <c r="C151" s="0" t="s">
+      <c r="C151" s="5" t="s">
         <v>35</v>
       </c>
     </row>
@@ -2721,6 +2781,7 @@
       <c r="B152" s="4" t="s">
         <v>172</v>
       </c>
+      <c r="C152" s="5"/>
     </row>
     <row r="153" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A153" s="5" t="s">
@@ -2729,7 +2790,7 @@
       <c r="B153" s="4" t="s">
         <v>173</v>
       </c>
-      <c r="C153" s="0" t="s">
+      <c r="C153" s="5" t="s">
         <v>18</v>
       </c>
     </row>
@@ -2740,7 +2801,7 @@
       <c r="B154" s="4" t="s">
         <v>174</v>
       </c>
-      <c r="C154" s="0" t="s">
+      <c r="C154" s="5" t="s">
         <v>47</v>
       </c>
     </row>
@@ -2751,7 +2812,7 @@
       <c r="B155" s="4" t="s">
         <v>175</v>
       </c>
-      <c r="C155" s="0" t="s">
+      <c r="C155" s="5" t="s">
         <v>42</v>
       </c>
     </row>
@@ -2762,7 +2823,7 @@
       <c r="B156" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="C156" s="0" t="s">
+      <c r="C156" s="5" t="s">
         <v>46</v>
       </c>
     </row>
@@ -2773,7 +2834,7 @@
       <c r="B157" s="4" t="s">
         <v>176</v>
       </c>
-      <c r="C157" s="0" t="s">
+      <c r="C157" s="5" t="s">
         <v>25</v>
       </c>
     </row>
@@ -2784,7 +2845,7 @@
       <c r="B158" s="4" t="s">
         <v>177</v>
       </c>
-      <c r="C158" s="0" t="s">
+      <c r="C158" s="5" t="s">
         <v>49</v>
       </c>
     </row>
@@ -2795,7 +2856,7 @@
       <c r="B159" s="5" t="s">
         <v>179</v>
       </c>
-      <c r="C159" s="0" t="s">
+      <c r="C159" s="5" t="s">
         <v>7</v>
       </c>
     </row>
@@ -2806,7 +2867,7 @@
       <c r="B160" s="5" t="s">
         <v>180</v>
       </c>
-      <c r="C160" s="0" t="s">
+      <c r="C160" s="5" t="s">
         <v>25</v>
       </c>
     </row>
@@ -2817,7 +2878,7 @@
       <c r="B161" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="C161" s="0" t="s">
+      <c r="C161" s="5" t="s">
         <v>42</v>
       </c>
     </row>
@@ -2828,7 +2889,7 @@
       <c r="B162" s="5" t="s">
         <v>181</v>
       </c>
-      <c r="C162" s="0" t="s">
+      <c r="C162" s="5" t="s">
         <v>35</v>
       </c>
     </row>
@@ -2839,7 +2900,7 @@
       <c r="B163" s="5" t="s">
         <v>159</v>
       </c>
-      <c r="C163" s="0" t="s">
+      <c r="C163" s="5" t="s">
         <v>21</v>
       </c>
     </row>
@@ -2850,7 +2911,7 @@
       <c r="B164" s="0" t="s">
         <v>167</v>
       </c>
-      <c r="C164" s="0" t="s">
+      <c r="C164" s="5" t="s">
         <v>21</v>
       </c>
     </row>
@@ -2861,7 +2922,7 @@
       <c r="B165" s="0" t="s">
         <v>183</v>
       </c>
-      <c r="C165" s="0" t="s">
+      <c r="C165" s="5" t="s">
         <v>11</v>
       </c>
     </row>
@@ -2872,7 +2933,7 @@
       <c r="B166" s="0" t="s">
         <v>146</v>
       </c>
-      <c r="C166" s="0" t="s">
+      <c r="C166" s="5" t="s">
         <v>8</v>
       </c>
     </row>
@@ -2883,7 +2944,7 @@
       <c r="B167" s="0" t="s">
         <v>126</v>
       </c>
-      <c r="C167" s="0" t="s">
+      <c r="C167" s="5" t="s">
         <v>25</v>
       </c>
     </row>
@@ -2894,7 +2955,7 @@
       <c r="B168" s="0" t="s">
         <v>184</v>
       </c>
-      <c r="C168" s="0" t="s">
+      <c r="C168" s="5" t="s">
         <v>48</v>
       </c>
     </row>
@@ -2905,7 +2966,7 @@
       <c r="B169" s="0" t="s">
         <v>167</v>
       </c>
-      <c r="C169" s="0" t="s">
+      <c r="C169" s="5" t="s">
         <v>21</v>
       </c>
     </row>
@@ -2916,7 +2977,7 @@
       <c r="B170" s="0" t="s">
         <v>175</v>
       </c>
-      <c r="C170" s="0" t="s">
+      <c r="C170" s="5" t="s">
         <v>42</v>
       </c>
     </row>
@@ -2927,7 +2988,7 @@
       <c r="B171" s="0" t="s">
         <v>69</v>
       </c>
-      <c r="C171" s="0" t="s">
+      <c r="C171" s="5" t="s">
         <v>40</v>
       </c>
     </row>
@@ -2938,7 +2999,7 @@
       <c r="B172" s="0" t="s">
         <v>70</v>
       </c>
-      <c r="C172" s="0" t="s">
+      <c r="C172" s="5" t="s">
         <v>41</v>
       </c>
     </row>
@@ -2949,7 +3010,7 @@
       <c r="B173" s="0" t="s">
         <v>67</v>
       </c>
-      <c r="C173" s="0" t="s">
+      <c r="C173" s="5" t="s">
         <v>36</v>
       </c>
     </row>
@@ -2960,7 +3021,7 @@
       <c r="B174" s="0" t="s">
         <v>76</v>
       </c>
-      <c r="C174" s="0" t="s">
+      <c r="C174" s="5" t="s">
         <v>29</v>
       </c>
     </row>
@@ -2971,7 +3032,7 @@
       <c r="B175" s="0" t="s">
         <v>126</v>
       </c>
-      <c r="C175" s="0" t="s">
+      <c r="C175" s="5" t="s">
         <v>25</v>
       </c>
     </row>
@@ -2982,7 +3043,7 @@
       <c r="B176" s="0" t="s">
         <v>186</v>
       </c>
-      <c r="C176" s="0" t="s">
+      <c r="C176" s="5" t="s">
         <v>11</v>
       </c>
     </row>
@@ -2993,7 +3054,7 @@
       <c r="B177" s="0" t="s">
         <v>58</v>
       </c>
-      <c r="C177" s="0" t="s">
+      <c r="C177" s="5" t="s">
         <v>8</v>
       </c>
     </row>
@@ -3004,7 +3065,7 @@
       <c r="B178" s="0" t="s">
         <v>140</v>
       </c>
-      <c r="C178" s="0" t="s">
+      <c r="C178" s="5" t="s">
         <v>18</v>
       </c>
     </row>
@@ -3034,6 +3095,61 @@
       </c>
       <c r="D180" s="5" t="s">
         <v>188</v>
+      </c>
+    </row>
+    <row r="181" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A181" s="0" t="s">
+        <v>190</v>
+      </c>
+      <c r="B181" s="0" t="s">
+        <v>191</v>
+      </c>
+      <c r="C181" s="0" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="182" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A182" s="0" t="s">
+        <v>190</v>
+      </c>
+      <c r="B182" s="0" t="s">
+        <v>192</v>
+      </c>
+      <c r="C182" s="0" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="183" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A183" s="0" t="s">
+        <v>190</v>
+      </c>
+      <c r="B183" s="0" t="s">
+        <v>126</v>
+      </c>
+      <c r="C183" s="0" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="184" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A184" s="0" t="s">
+        <v>190</v>
+      </c>
+      <c r="B184" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="C184" s="0" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="185" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A185" s="0" t="s">
+        <v>190</v>
+      </c>
+      <c r="B185" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="C185" s="0" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -3071,12 +3187,12 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix issue with colnames in random method.
Add a unit test for that problem.
</commit_message>
<xml_diff>
--- a/inst/extdata/cell_type_mapping.xlsx
+++ b/inst/extdata/cell_type_mapping.xlsx
@@ -756,7 +756,7 @@
   </sheetPr>
   <dimension ref="A1:O45"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A26" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
     </sheetView>
   </sheetViews>
@@ -1202,8 +1202,8 @@
   </sheetPr>
   <dimension ref="A1:E185"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A165" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G183" activeCellId="0" sqref="G183"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A169" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B185" activeCellId="0" sqref="B185"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3124,7 +3124,7 @@
         <v>190</v>
       </c>
       <c r="B183" s="0" t="s">
-        <v>126</v>
+        <v>25</v>
       </c>
       <c r="C183" s="0" t="s">
         <v>25</v>

</xml_diff>

<commit_message>
map mcp counter monocytic lineage to macrophage/monocyte
</commit_message>
<xml_diff>
--- a/inst/extdata/cell_type_mapping.xlsx
+++ b/inst/extdata/cell_type_mapping.xlsx
@@ -1,18 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Y:\projects\immune_deconvolution_benchmark\immunedeconv\inst\extdata\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{5413D193-B82C-4539-9C1A-9A2C1867FC31}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14025" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="controlled_vocabulary" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="mapping" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="README" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="controlled_vocabulary" sheetId="1" r:id="rId1"/>
+    <sheet name="mapping" sheetId="2" r:id="rId2"/>
+    <sheet name="README" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr calcId="179017"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -22,622 +27,607 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="601" uniqueCount="195">
-  <si>
-    <t xml:space="preserve">cell_type</t>
-  </si>
-  <si>
-    <t xml:space="preserve">parent</t>
-  </si>
-  <si>
-    <t xml:space="preserve">optional</t>
-  </si>
-  <si>
-    <t xml:space="preserve">description</t>
-  </si>
-  <si>
-    <t xml:space="preserve">immune cell</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cell</t>
-  </si>
-  <si>
-    <t xml:space="preserve">lymphoid</t>
-  </si>
-  <si>
-    <t xml:space="preserve">T cell</t>
-  </si>
-  <si>
-    <t xml:space="preserve">T cell CD8+</t>
-  </si>
-  <si>
-    <t xml:space="preserve">T cell CD8+ naive</t>
-  </si>
-  <si>
-    <t xml:space="preserve">T cell CD8+ memory</t>
-  </si>
-  <si>
-    <t xml:space="preserve">T cell CD4+</t>
-  </si>
-  <si>
-    <t xml:space="preserve">T cell CD4+ (non-regulatory)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">T cell CD4+ naive</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="605" uniqueCount="196">
+  <si>
+    <t>cell_type</t>
+  </si>
+  <si>
+    <t>parent</t>
+  </si>
+  <si>
+    <t>optional</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>immune cell</t>
+  </si>
+  <si>
+    <t>cell</t>
+  </si>
+  <si>
+    <t>lymphoid</t>
+  </si>
+  <si>
+    <t>T cell</t>
+  </si>
+  <si>
+    <t>T cell CD8+</t>
+  </si>
+  <si>
+    <t>T cell CD8+ naive</t>
+  </si>
+  <si>
+    <t>T cell CD8+ memory</t>
+  </si>
+  <si>
+    <t>T cell CD4+</t>
+  </si>
+  <si>
+    <t>T cell CD4+ (non-regulatory)</t>
+  </si>
+  <si>
+    <t>T cell CD4+ naive</t>
   </si>
   <si>
     <t xml:space="preserve">T cell CD4+ memory </t>
   </si>
   <si>
-    <t xml:space="preserve">T cell CD4+ memory resting</t>
-  </si>
-  <si>
-    <t xml:space="preserve">T cell CD4+ memory activated</t>
-  </si>
-  <si>
-    <t xml:space="preserve">T cell follicular helper</t>
-  </si>
-  <si>
-    <t xml:space="preserve">T cell regulatory (Tregs)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">T cell gamma delta</t>
-  </si>
-  <si>
-    <t xml:space="preserve">only in cibersort, still count all other subtypes as "all t cells" if they do not predict gdT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">B cell</t>
-  </si>
-  <si>
-    <t xml:space="preserve">B cell naive</t>
-  </si>
-  <si>
-    <t xml:space="preserve">B cell memory</t>
-  </si>
-  <si>
-    <t xml:space="preserve">B cell plasma</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NK cell</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NK cell resting</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NK cell activated</t>
-  </si>
-  <si>
-    <t xml:space="preserve">myleoid</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Neutrophil</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Eosinophil</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mast cell</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mast cell resting</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mast cell activated</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Monocytic lineage</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Macrophage/Monocyte</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Monocyte</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Macrophage</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Macrophage M0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">only in cibersort, still count all other subtypes as "all t cells" if they do only distinguish M1/M2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Macrophage M1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Macrophage M2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dendritic cell</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dendritic cell resting</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dendritic cell activated</t>
-  </si>
-  <si>
-    <t xml:space="preserve">other cell</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Endothelial cell</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cancer associated fibroblast</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cancer cell</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ovarian carcinoma cell</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Melanoma cell</t>
-  </si>
-  <si>
-    <t xml:space="preserve">method_dataset</t>
-  </si>
-  <si>
-    <t xml:space="preserve">method_cell_type</t>
-  </si>
-  <si>
-    <t xml:space="preserve">comment</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cibersort</t>
-  </si>
-  <si>
-    <t xml:space="preserve">B cells naive</t>
-  </si>
-  <si>
-    <t xml:space="preserve">B cells memory</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Plasma cells</t>
-  </si>
-  <si>
-    <t xml:space="preserve">T cells CD8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">T cells CD4 naive</t>
-  </si>
-  <si>
-    <t xml:space="preserve">T cells CD4 memory resting</t>
-  </si>
-  <si>
-    <t xml:space="preserve">T cells CD4 memory activated</t>
-  </si>
-  <si>
-    <t xml:space="preserve">T cells follicular helper</t>
-  </si>
-  <si>
-    <t xml:space="preserve">T cells regulatory (Tregs)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">T cells gamma delta</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NK cells resting</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NK cells activated</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Monocytes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Macrophages M0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Macrophages M1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Macrophages M2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dendritic cells resting</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dendritic cells activated</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mast cells resting</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mast cells activated</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Eosinophils</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Neutrophils</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cibersort_abs</t>
-  </si>
-  <si>
-    <t xml:space="preserve">timer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">B_cell</t>
-  </si>
-  <si>
-    <t xml:space="preserve">T_cell.CD4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">T_cell.CD8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">xcell</t>
-  </si>
-  <si>
-    <t xml:space="preserve">aDC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Adipocytes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Astrocytes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Basophils</t>
-  </si>
-  <si>
-    <t xml:space="preserve">B-cells</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CD4+ memory T-cells</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CD4+ naive T-cells</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CD4+ T-cells</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CD4+ Tcm</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CD4+ Tem</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CD8+ naive T-cells</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CD8+ T-cells</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CD8+ Tcm</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CD8+ Tem</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cDC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Chondrocytes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Class-switched memory B-cells</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CLP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CMP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Endothelial cells</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Epithelial cells</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Erythrocytes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fibroblasts</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GMP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hepatocytes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HSC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">iDC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Keratinocytes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ly Endothelial cells</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Macrophages</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mast cells</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Megakaryocytes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Melanocytes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Memory B-cells</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MEP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mesangial cells</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MPP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MSC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mv Endothelial cells</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Myocytes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">naive B-cells</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Neurons</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NK cells</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NKT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Osteoblast</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pDC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pericytes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Platelets</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Preadipocytes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pro B-cells</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sebocytes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Skeletal muscle</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Smooth muscle</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tgd cells</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Th1 cells</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Th2 cells</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tregs</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ImmuneScore</t>
-  </si>
-  <si>
-    <t xml:space="preserve">StromaScore</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MicroenvironmentScore</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mcp_counter</t>
-  </si>
-  <si>
-    <t xml:space="preserve">T cells</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CD8 T cells</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cytotoxic lymphocytes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">B lineage</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Myeloid dendritic cells</t>
-  </si>
-  <si>
-    <t xml:space="preserve">quantiseq</t>
-  </si>
-  <si>
-    <t xml:space="preserve">B.cells</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Macrophages.M1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Macrophages.M2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NK.cells</t>
-  </si>
-  <si>
-    <t xml:space="preserve">T.cells.CD4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">T.cells.CD8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dendritic.cells</t>
-  </si>
-  <si>
-    <t xml:space="preserve">epic</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bcells</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CAFs</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CD4_Tcells</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CD8_Tcells</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Endothelial</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NKcells</t>
-  </si>
-  <si>
-    <t xml:space="preserve">otherCells</t>
-  </si>
-  <si>
-    <t xml:space="preserve">schelker_single_cell</t>
-  </si>
-  <si>
-    <t xml:space="preserve">B cells</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CD8+ T cells</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Melanoma cells</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CD4+ T cells</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Macrophages/Monocytes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Unknown</t>
-  </si>
-  <si>
-    <t xml:space="preserve">regulatory T cells</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cancer associated fibroblasts</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dendritic cells</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Natural killer cells</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ovarian carcinoma cells</t>
-  </si>
-  <si>
-    <t xml:space="preserve">hoek</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tcell</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NK</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mono</t>
-  </si>
-  <si>
-    <t xml:space="preserve">racle</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CD4 T cells</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cancer cells</t>
-  </si>
-  <si>
-    <t xml:space="preserve">quantiseq_reference</t>
-  </si>
-  <si>
-    <t xml:space="preserve">T cells CD4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">test_method1</t>
+    <t>T cell CD4+ memory resting</t>
+  </si>
+  <si>
+    <t>T cell CD4+ memory activated</t>
+  </si>
+  <si>
+    <t>T cell follicular helper</t>
+  </si>
+  <si>
+    <t>T cell regulatory (Tregs)</t>
+  </si>
+  <si>
+    <t>T cell gamma delta</t>
+  </si>
+  <si>
+    <t>only in cibersort, still count all other subtypes as "all t cells" if they do not predict gdT</t>
+  </si>
+  <si>
+    <t>B cell</t>
+  </si>
+  <si>
+    <t>B cell naive</t>
+  </si>
+  <si>
+    <t>B cell memory</t>
+  </si>
+  <si>
+    <t>B cell plasma</t>
+  </si>
+  <si>
+    <t>NK cell</t>
+  </si>
+  <si>
+    <t>NK cell resting</t>
+  </si>
+  <si>
+    <t>NK cell activated</t>
+  </si>
+  <si>
+    <t>myleoid</t>
+  </si>
+  <si>
+    <t>Neutrophil</t>
+  </si>
+  <si>
+    <t>Eosinophil</t>
+  </si>
+  <si>
+    <t>Mast cell</t>
+  </si>
+  <si>
+    <t>Mast cell resting</t>
+  </si>
+  <si>
+    <t>Mast cell activated</t>
+  </si>
+  <si>
+    <t>Monocytic lineage</t>
+  </si>
+  <si>
+    <t>Macrophage/Monocyte</t>
+  </si>
+  <si>
+    <t>Monocyte</t>
+  </si>
+  <si>
+    <t>Macrophage</t>
+  </si>
+  <si>
+    <t>Macrophage M0</t>
+  </si>
+  <si>
+    <t>only in cibersort, still count all other subtypes as "all t cells" if they do only distinguish M1/M2</t>
+  </si>
+  <si>
+    <t>Macrophage M1</t>
+  </si>
+  <si>
+    <t>Macrophage M2</t>
+  </si>
+  <si>
+    <t>Dendritic cell</t>
+  </si>
+  <si>
+    <t>Dendritic cell resting</t>
+  </si>
+  <si>
+    <t>Dendritic cell activated</t>
+  </si>
+  <si>
+    <t>other cell</t>
+  </si>
+  <si>
+    <t>Endothelial cell</t>
+  </si>
+  <si>
+    <t>Cancer associated fibroblast</t>
+  </si>
+  <si>
+    <t>cancer cell</t>
+  </si>
+  <si>
+    <t>Ovarian carcinoma cell</t>
+  </si>
+  <si>
+    <t>Melanoma cell</t>
+  </si>
+  <si>
+    <t>method_dataset</t>
+  </si>
+  <si>
+    <t>method_cell_type</t>
+  </si>
+  <si>
+    <t>comment</t>
+  </si>
+  <si>
+    <t>cibersort</t>
+  </si>
+  <si>
+    <t>B cells naive</t>
+  </si>
+  <si>
+    <t>B cells memory</t>
+  </si>
+  <si>
+    <t>Plasma cells</t>
+  </si>
+  <si>
+    <t>T cells CD8</t>
+  </si>
+  <si>
+    <t>T cells CD4 naive</t>
+  </si>
+  <si>
+    <t>T cells CD4 memory resting</t>
+  </si>
+  <si>
+    <t>T cells CD4 memory activated</t>
+  </si>
+  <si>
+    <t>T cells follicular helper</t>
+  </si>
+  <si>
+    <t>T cells regulatory (Tregs)</t>
+  </si>
+  <si>
+    <t>T cells gamma delta</t>
+  </si>
+  <si>
+    <t>NK cells resting</t>
+  </si>
+  <si>
+    <t>NK cells activated</t>
+  </si>
+  <si>
+    <t>Monocytes</t>
+  </si>
+  <si>
+    <t>Macrophages M0</t>
+  </si>
+  <si>
+    <t>Macrophages M1</t>
+  </si>
+  <si>
+    <t>Macrophages M2</t>
+  </si>
+  <si>
+    <t>Dendritic cells resting</t>
+  </si>
+  <si>
+    <t>Dendritic cells activated</t>
+  </si>
+  <si>
+    <t>Mast cells resting</t>
+  </si>
+  <si>
+    <t>Mast cells activated</t>
+  </si>
+  <si>
+    <t>Eosinophils</t>
+  </si>
+  <si>
+    <t>Neutrophils</t>
+  </si>
+  <si>
+    <t>cibersort_abs</t>
+  </si>
+  <si>
+    <t>timer</t>
+  </si>
+  <si>
+    <t>B_cell</t>
+  </si>
+  <si>
+    <t>T_cell.CD4</t>
+  </si>
+  <si>
+    <t>T_cell.CD8</t>
+  </si>
+  <si>
+    <t>DC</t>
+  </si>
+  <si>
+    <t>xcell</t>
+  </si>
+  <si>
+    <t>aDC</t>
+  </si>
+  <si>
+    <t>Adipocytes</t>
+  </si>
+  <si>
+    <t>Astrocytes</t>
+  </si>
+  <si>
+    <t>Basophils</t>
+  </si>
+  <si>
+    <t>B-cells</t>
+  </si>
+  <si>
+    <t>CD4+ memory T-cells</t>
+  </si>
+  <si>
+    <t>CD4+ naive T-cells</t>
+  </si>
+  <si>
+    <t>CD4+ T-cells</t>
+  </si>
+  <si>
+    <t>CD4+ Tcm</t>
+  </si>
+  <si>
+    <t>CD4+ Tem</t>
+  </si>
+  <si>
+    <t>CD8+ naive T-cells</t>
+  </si>
+  <si>
+    <t>CD8+ T-cells</t>
+  </si>
+  <si>
+    <t>CD8+ Tcm</t>
+  </si>
+  <si>
+    <t>CD8+ Tem</t>
+  </si>
+  <si>
+    <t>cDC</t>
+  </si>
+  <si>
+    <t>Chondrocytes</t>
+  </si>
+  <si>
+    <t>Class-switched memory B-cells</t>
+  </si>
+  <si>
+    <t>CLP</t>
+  </si>
+  <si>
+    <t>CMP</t>
+  </si>
+  <si>
+    <t>Endothelial cells</t>
+  </si>
+  <si>
+    <t>Epithelial cells</t>
+  </si>
+  <si>
+    <t>Erythrocytes</t>
+  </si>
+  <si>
+    <t>Fibroblasts</t>
+  </si>
+  <si>
+    <t>GMP</t>
+  </si>
+  <si>
+    <t>Hepatocytes</t>
+  </si>
+  <si>
+    <t>HSC</t>
+  </si>
+  <si>
+    <t>iDC</t>
+  </si>
+  <si>
+    <t>Keratinocytes</t>
+  </si>
+  <si>
+    <t>ly Endothelial cells</t>
+  </si>
+  <si>
+    <t>Macrophages</t>
+  </si>
+  <si>
+    <t>Mast cells</t>
+  </si>
+  <si>
+    <t>Megakaryocytes</t>
+  </si>
+  <si>
+    <t>Melanocytes</t>
+  </si>
+  <si>
+    <t>Memory B-cells</t>
+  </si>
+  <si>
+    <t>MEP</t>
+  </si>
+  <si>
+    <t>Mesangial cells</t>
+  </si>
+  <si>
+    <t>MPP</t>
+  </si>
+  <si>
+    <t>MSC</t>
+  </si>
+  <si>
+    <t>mv Endothelial cells</t>
+  </si>
+  <si>
+    <t>Myocytes</t>
+  </si>
+  <si>
+    <t>naive B-cells</t>
+  </si>
+  <si>
+    <t>Neurons</t>
+  </si>
+  <si>
+    <t>NK cells</t>
+  </si>
+  <si>
+    <t>NKT</t>
+  </si>
+  <si>
+    <t>Osteoblast</t>
+  </si>
+  <si>
+    <t>pDC</t>
+  </si>
+  <si>
+    <t>Pericytes</t>
+  </si>
+  <si>
+    <t>Platelets</t>
+  </si>
+  <si>
+    <t>Preadipocytes</t>
+  </si>
+  <si>
+    <t>pro B-cells</t>
+  </si>
+  <si>
+    <t>Sebocytes</t>
+  </si>
+  <si>
+    <t>Skeletal muscle</t>
+  </si>
+  <si>
+    <t>Smooth muscle</t>
+  </si>
+  <si>
+    <t>Tgd cells</t>
+  </si>
+  <si>
+    <t>Th1 cells</t>
+  </si>
+  <si>
+    <t>Th2 cells</t>
+  </si>
+  <si>
+    <t>Tregs</t>
+  </si>
+  <si>
+    <t>ImmuneScore</t>
+  </si>
+  <si>
+    <t>StromaScore</t>
+  </si>
+  <si>
+    <t>MicroenvironmentScore</t>
+  </si>
+  <si>
+    <t>mcp_counter</t>
+  </si>
+  <si>
+    <t>T cells</t>
+  </si>
+  <si>
+    <t>CD8 T cells</t>
+  </si>
+  <si>
+    <t>Cytotoxic lymphocytes</t>
+  </si>
+  <si>
+    <t>B lineage</t>
+  </si>
+  <si>
+    <t>Myeloid dendritic cells</t>
+  </si>
+  <si>
+    <t>quantiseq</t>
+  </si>
+  <si>
+    <t>B.cells</t>
+  </si>
+  <si>
+    <t>Macrophages.M1</t>
+  </si>
+  <si>
+    <t>Macrophages.M2</t>
+  </si>
+  <si>
+    <t>NK.cells</t>
+  </si>
+  <si>
+    <t>T.cells.CD4</t>
+  </si>
+  <si>
+    <t>T.cells.CD8</t>
+  </si>
+  <si>
+    <t>Dendritic.cells</t>
+  </si>
+  <si>
+    <t>epic</t>
+  </si>
+  <si>
+    <t>Bcells</t>
+  </si>
+  <si>
+    <t>CAFs</t>
+  </si>
+  <si>
+    <t>CD4_Tcells</t>
+  </si>
+  <si>
+    <t>CD8_Tcells</t>
+  </si>
+  <si>
+    <t>Endothelial</t>
+  </si>
+  <si>
+    <t>NKcells</t>
+  </si>
+  <si>
+    <t>otherCells</t>
+  </si>
+  <si>
+    <t>schelker_single_cell</t>
+  </si>
+  <si>
+    <t>B cells</t>
+  </si>
+  <si>
+    <t>CD8+ T cells</t>
+  </si>
+  <si>
+    <t>Melanoma cells</t>
+  </si>
+  <si>
+    <t>CD4+ T cells</t>
+  </si>
+  <si>
+    <t>Macrophages/Monocytes</t>
+  </si>
+  <si>
+    <t>Unknown</t>
+  </si>
+  <si>
+    <t>regulatory T cells</t>
+  </si>
+  <si>
+    <t>Cancer associated fibroblasts</t>
+  </si>
+  <si>
+    <t>Dendritic cells</t>
+  </si>
+  <si>
+    <t>Natural killer cells</t>
+  </si>
+  <si>
+    <t>Ovarian carcinoma cells</t>
+  </si>
+  <si>
+    <t>hoek</t>
+  </si>
+  <si>
+    <t>Tcell</t>
+  </si>
+  <si>
+    <t>NK</t>
+  </si>
+  <si>
+    <t>mono</t>
+  </si>
+  <si>
+    <t>racle</t>
+  </si>
+  <si>
+    <t>CD4 T cells</t>
+  </si>
+  <si>
+    <t>cancer cells</t>
+  </si>
+  <si>
+    <t>quantiseq_reference</t>
+  </si>
+  <si>
+    <t>T cells CD4</t>
+  </si>
+  <si>
+    <t>test_method1</t>
   </si>
   <si>
     <t xml:space="preserve">method for unit test. </t>
   </si>
   <si>
-    <t xml:space="preserve">Macrophages.M0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">random</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CD4+ Tcell</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CD8+ Tcell</t>
+    <t>Macrophages.M0</t>
+  </si>
+  <si>
+    <t>random</t>
+  </si>
+  <si>
+    <t>CD4+ Tcell</t>
+  </si>
+  <si>
+    <t>CD8+ Tcell</t>
   </si>
   <si>
     <t xml:space="preserve">controlled vocabulary is a list of entities (cell types) of different granularity (e.g. T cell, CD8 T cell). We use this vocabulary to build a tree and to map cell type names between different methods/datasets. </t>
   </si>
   <si>
-    <t xml:space="preserve">mapping contains the mapping between methods/datasets</t>
+    <t>mapping contains the mapping between methods/datasets</t>
+  </si>
+  <si>
+    <t xml:space="preserve"># use this as a "proxy" although it would also include dendritc cells. </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="General"/>
-  </numFmts>
-  <fonts count="8">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
     </font>
     <font>
       <sz val="11"/>
@@ -647,7 +637,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
+      <b/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri Light"/>
@@ -655,7 +645,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
+      <b/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -679,7 +669,7 @@
     </fill>
   </fills>
   <borders count="1">
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
@@ -687,90 +677,349 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="6">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+  <cellStyles count="1">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4472C4"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:O45"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:AMK45"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A26" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
+    <sheetView topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C37" sqref="C37:D37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="30.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="25.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="22.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="4" style="1" width="9.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="27.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="16" style="1" width="9.14"/>
+    <col min="1" max="1" width="30.140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="25.140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="22.85546875" style="1" customWidth="1"/>
+    <col min="4" max="14" width="9.140625" style="1" customWidth="1"/>
+    <col min="15" max="15" width="27.140625" style="1" customWidth="1"/>
+    <col min="16" max="1025" width="9.140625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -784,7 +1033,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -792,7 +1041,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
@@ -800,7 +1049,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
@@ -808,7 +1057,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
@@ -816,7 +1065,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
@@ -824,7 +1073,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>10</v>
       </c>
@@ -832,7 +1081,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>11</v>
       </c>
@@ -840,7 +1089,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>12</v>
       </c>
@@ -848,7 +1097,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>13</v>
       </c>
@@ -856,7 +1105,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>14</v>
       </c>
@@ -864,7 +1113,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>15</v>
       </c>
@@ -872,7 +1121,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>16</v>
       </c>
@@ -881,20 +1130,20 @@
       </c>
       <c r="O13" s="2"/>
     </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C14" s="1" t="n">
-        <f aca="false">TRUE()</f>
+      <c r="C14" s="1" t="b">
+        <f>TRUE()</f>
         <v>1</v>
       </c>
       <c r="O14" s="2"/>
     </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>18</v>
       </c>
@@ -903,15 +1152,15 @@
       </c>
       <c r="O15" s="2"/>
     </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C16" s="1" t="n">
-        <f aca="false">TRUE()</f>
+      <c r="C16" s="1" t="b">
+        <f>TRUE()</f>
         <v>1</v>
       </c>
       <c r="D16" s="1" t="s">
@@ -919,7 +1168,7 @@
       </c>
       <c r="O16" s="2"/>
     </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>21</v>
       </c>
@@ -928,7 +1177,7 @@
       </c>
       <c r="O17" s="2"/>
     </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>22</v>
       </c>
@@ -937,7 +1186,7 @@
       </c>
       <c r="O18" s="2"/>
     </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>23</v>
       </c>
@@ -946,7 +1195,7 @@
       </c>
       <c r="O19" s="2"/>
     </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>24</v>
       </c>
@@ -955,7 +1204,7 @@
       </c>
       <c r="O20" s="2"/>
     </row>
-    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>25</v>
       </c>
@@ -964,7 +1213,7 @@
       </c>
       <c r="O21" s="2"/>
     </row>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>26</v>
       </c>
@@ -973,7 +1222,7 @@
       </c>
       <c r="O22" s="2"/>
     </row>
-    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>27</v>
       </c>
@@ -982,7 +1231,7 @@
       </c>
       <c r="O23" s="2"/>
     </row>
-    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>28</v>
       </c>
@@ -991,7 +1240,7 @@
       </c>
       <c r="O24" s="2"/>
     </row>
-    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>29</v>
       </c>
@@ -1000,7 +1249,7 @@
       </c>
       <c r="O25" s="2"/>
     </row>
-    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>30</v>
       </c>
@@ -1009,7 +1258,7 @@
       </c>
       <c r="O26" s="2"/>
     </row>
-    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>31</v>
       </c>
@@ -1018,7 +1267,7 @@
       </c>
       <c r="O27" s="2"/>
     </row>
-    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>32</v>
       </c>
@@ -1027,7 +1276,7 @@
       </c>
       <c r="O28" s="2"/>
     </row>
-    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>33</v>
       </c>
@@ -1036,7 +1285,7 @@
       </c>
       <c r="O29" s="2"/>
     </row>
-    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>34</v>
       </c>
@@ -1045,7 +1294,7 @@
       </c>
       <c r="O30" s="2"/>
     </row>
-    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>35</v>
       </c>
@@ -1054,43 +1303,46 @@
       </c>
       <c r="O31" s="2"/>
     </row>
-    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>36</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C32" s="1" t="n">
-        <f aca="false">TRUE()</f>
+      <c r="C32" s="1" t="b">
+        <f>TRUE()</f>
         <v>1</v>
       </c>
       <c r="O32" s="2"/>
     </row>
-    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>37</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C33" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>38</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C34" s="1" t="n">
-        <f aca="false">TRUE()</f>
+      <c r="C34" s="1" t="b">
+        <f>TRUE()</f>
         <v>1</v>
       </c>
       <c r="D34" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>40</v>
       </c>
@@ -1098,7 +1350,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>41</v>
       </c>
@@ -1106,7 +1358,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>42</v>
       </c>
@@ -1114,7 +1366,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>43</v>
       </c>
@@ -1122,7 +1374,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>44</v>
       </c>
@@ -1130,7 +1382,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>45</v>
       </c>
@@ -1138,7 +1390,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>46</v>
       </c>
@@ -1146,7 +1398,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>47</v>
       </c>
@@ -1154,7 +1406,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>48</v>
       </c>
@@ -1162,7 +1414,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>49</v>
       </c>
@@ -1170,7 +1422,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>50</v>
       </c>
@@ -1180,41 +1432,33 @@
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="B1 B3:B6 B8:B9 B12:B13 B15:B30 B32:B39 B41:B45" type="list">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1 B41:B45 B32:B39 B15:B30 B12:B13 B8:B9 B3:B6" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>$A:$A</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:E185"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:E186"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A169" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B185" activeCellId="0" sqref="B185"/>
+    <sheetView tabSelected="1" topLeftCell="A97" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D125" sqref="D125"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="26.72"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="29.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="8.53"/>
+    <col min="1" max="1" width="19.85546875" customWidth="1"/>
+    <col min="2" max="2" width="26.7109375" customWidth="1"/>
+    <col min="3" max="3" width="29.85546875" customWidth="1"/>
+    <col min="4" max="1025" width="8.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>51</v>
       </c>
@@ -1228,8 +1472,8 @@
         <v>53</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>54</v>
       </c>
       <c r="B2" s="4" t="s">
@@ -1239,7 +1483,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>54</v>
       </c>
@@ -1250,7 +1494,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>54</v>
       </c>
@@ -1261,7 +1505,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>54</v>
       </c>
@@ -1272,7 +1516,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>54</v>
       </c>
@@ -1283,7 +1527,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>54</v>
       </c>
@@ -1294,7 +1538,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>54</v>
       </c>
@@ -1305,7 +1549,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>54</v>
       </c>
@@ -1316,7 +1560,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>54</v>
       </c>
@@ -1327,7 +1571,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>54</v>
       </c>
@@ -1338,7 +1582,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>54</v>
       </c>
@@ -1349,7 +1593,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>54</v>
       </c>
@@ -1360,7 +1604,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>54</v>
       </c>
@@ -1371,7 +1615,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>54</v>
       </c>
@@ -1382,7 +1626,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>54</v>
       </c>
@@ -1393,7 +1637,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
         <v>54</v>
       </c>
@@ -1404,7 +1648,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>54</v>
       </c>
@@ -1415,7 +1659,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
         <v>54</v>
       </c>
@@ -1426,7 +1670,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
         <v>54</v>
       </c>
@@ -1437,7 +1681,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
         <v>54</v>
       </c>
@@ -1448,7 +1692,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
         <v>54</v>
       </c>
@@ -1460,7 +1704,7 @@
       </c>
       <c r="E22" s="5"/>
     </row>
-    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
         <v>54</v>
       </c>
@@ -1471,7 +1715,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
         <v>77</v>
       </c>
@@ -1482,7 +1726,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
         <v>77</v>
       </c>
@@ -1493,7 +1737,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
         <v>77</v>
       </c>
@@ -1504,7 +1748,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
         <v>77</v>
       </c>
@@ -1515,7 +1759,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
         <v>77</v>
       </c>
@@ -1526,7 +1770,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
         <v>77</v>
       </c>
@@ -1537,7 +1781,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
         <v>77</v>
       </c>
@@ -1548,7 +1792,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
         <v>77</v>
       </c>
@@ -1559,7 +1803,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
         <v>77</v>
       </c>
@@ -1570,7 +1814,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
         <v>77</v>
       </c>
@@ -1581,7 +1825,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
         <v>77</v>
       </c>
@@ -1592,7 +1836,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
         <v>77</v>
       </c>
@@ -1603,7 +1847,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
         <v>77</v>
       </c>
@@ -1614,7 +1858,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
         <v>77</v>
       </c>
@@ -1625,7 +1869,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
         <v>77</v>
       </c>
@@ -1636,7 +1880,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="5" t="s">
         <v>77</v>
       </c>
@@ -1647,7 +1891,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="5" t="s">
         <v>77</v>
       </c>
@@ -1658,7 +1902,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="5" t="s">
         <v>77</v>
       </c>
@@ -1669,7 +1913,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="5" t="s">
         <v>77</v>
       </c>
@@ -1680,7 +1924,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="5" t="s">
         <v>77</v>
       </c>
@@ -1691,7 +1935,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="5" t="s">
         <v>77</v>
       </c>
@@ -1702,7 +1946,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="5" t="s">
         <v>77</v>
       </c>
@@ -1713,8 +1957,8 @@
         <v>29</v>
       </c>
     </row>
-    <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="0" t="s">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
         <v>78</v>
       </c>
       <c r="B46" s="4" t="s">
@@ -1724,7 +1968,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" s="5" t="s">
         <v>78</v>
       </c>
@@ -1735,7 +1979,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="5" t="s">
         <v>78</v>
       </c>
@@ -1746,7 +1990,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" s="5" t="s">
         <v>78</v>
       </c>
@@ -1757,7 +2001,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" s="5" t="s">
         <v>78</v>
       </c>
@@ -1768,7 +2012,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" s="5" t="s">
         <v>78</v>
       </c>
@@ -1779,8 +2023,8 @@
         <v>42</v>
       </c>
     </row>
-    <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="0" t="s">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
         <v>83</v>
       </c>
       <c r="B52" s="4" t="s">
@@ -1788,7 +2032,7 @@
       </c>
       <c r="C52" s="5"/>
     </row>
-    <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" s="5" t="s">
         <v>83</v>
       </c>
@@ -1797,7 +2041,7 @@
       </c>
       <c r="C53" s="5"/>
     </row>
-    <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" s="5" t="s">
         <v>83</v>
       </c>
@@ -1806,7 +2050,7 @@
       </c>
       <c r="C54" s="5"/>
     </row>
-    <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" s="5" t="s">
         <v>83</v>
       </c>
@@ -1815,7 +2059,7 @@
       </c>
       <c r="C55" s="5"/>
     </row>
-    <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" s="5" t="s">
         <v>83</v>
       </c>
@@ -1826,7 +2070,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" s="5" t="s">
         <v>83</v>
       </c>
@@ -1837,7 +2081,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" s="5" t="s">
         <v>83</v>
       </c>
@@ -1848,7 +2092,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" s="5" t="s">
         <v>83</v>
       </c>
@@ -1859,7 +2103,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" s="5" t="s">
         <v>83</v>
       </c>
@@ -1868,7 +2112,7 @@
       </c>
       <c r="C60" s="5"/>
     </row>
-    <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" s="5" t="s">
         <v>83</v>
       </c>
@@ -1877,7 +2121,7 @@
       </c>
       <c r="C61" s="5"/>
     </row>
-    <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" s="5" t="s">
         <v>83</v>
       </c>
@@ -1886,7 +2130,7 @@
       </c>
       <c r="C62" s="5"/>
     </row>
-    <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" s="5" t="s">
         <v>83</v>
       </c>
@@ -1897,7 +2141,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" s="5" t="s">
         <v>83</v>
       </c>
@@ -1906,7 +2150,7 @@
       </c>
       <c r="C64" s="5"/>
     </row>
-    <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" s="5" t="s">
         <v>83</v>
       </c>
@@ -1915,7 +2159,7 @@
       </c>
       <c r="C65" s="5"/>
     </row>
-    <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" s="5" t="s">
         <v>83</v>
       </c>
@@ -1924,7 +2168,7 @@
       </c>
       <c r="C66" s="5"/>
     </row>
-    <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" s="5" t="s">
         <v>83</v>
       </c>
@@ -1933,7 +2177,7 @@
       </c>
       <c r="C67" s="5"/>
     </row>
-    <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" s="5" t="s">
         <v>83</v>
       </c>
@@ -1942,7 +2186,7 @@
       </c>
       <c r="C68" s="5"/>
     </row>
-    <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" s="5" t="s">
         <v>83</v>
       </c>
@@ -1951,7 +2195,7 @@
       </c>
       <c r="C69" s="5"/>
     </row>
-    <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" s="5" t="s">
         <v>83</v>
       </c>
@@ -1960,7 +2204,7 @@
       </c>
       <c r="C70" s="5"/>
     </row>
-    <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" s="5" t="s">
         <v>83</v>
       </c>
@@ -1971,7 +2215,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="72" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" s="5" t="s">
         <v>83</v>
       </c>
@@ -1982,7 +2226,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" s="5" t="s">
         <v>83</v>
       </c>
@@ -1993,7 +2237,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="74" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" s="5" t="s">
         <v>83</v>
       </c>
@@ -2002,7 +2246,7 @@
       </c>
       <c r="C74" s="5"/>
     </row>
-    <row r="75" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" s="5" t="s">
         <v>83</v>
       </c>
@@ -2011,7 +2255,7 @@
       </c>
       <c r="C75" s="5"/>
     </row>
-    <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" s="5" t="s">
         <v>83</v>
       </c>
@@ -2022,7 +2266,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" s="5" t="s">
         <v>83</v>
       </c>
@@ -2031,7 +2275,7 @@
       </c>
       <c r="C77" s="5"/>
     </row>
-    <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" s="5" t="s">
         <v>83</v>
       </c>
@@ -2040,7 +2284,7 @@
       </c>
       <c r="C78" s="5"/>
     </row>
-    <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" s="5" t="s">
         <v>83</v>
       </c>
@@ -2049,7 +2293,7 @@
       </c>
       <c r="C79" s="5"/>
     </row>
-    <row r="80" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" s="5" t="s">
         <v>83</v>
       </c>
@@ -2058,7 +2302,7 @@
       </c>
       <c r="C80" s="5"/>
     </row>
-    <row r="81" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" s="5" t="s">
         <v>83</v>
       </c>
@@ -2067,7 +2311,7 @@
       </c>
       <c r="C81" s="5"/>
     </row>
-    <row r="82" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" s="5" t="s">
         <v>83</v>
       </c>
@@ -2076,7 +2320,7 @@
       </c>
       <c r="C82" s="5"/>
     </row>
-    <row r="83" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" s="5" t="s">
         <v>83</v>
       </c>
@@ -2087,7 +2331,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="84" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" s="5" t="s">
         <v>83</v>
       </c>
@@ -2098,7 +2342,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="85" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" s="5" t="s">
         <v>83</v>
       </c>
@@ -2109,7 +2353,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="86" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" s="5" t="s">
         <v>83</v>
       </c>
@@ -2120,7 +2364,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="87" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" s="5" t="s">
         <v>83</v>
       </c>
@@ -2129,7 +2373,7 @@
       </c>
       <c r="C87" s="5"/>
     </row>
-    <row r="88" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88" s="5" t="s">
         <v>83</v>
       </c>
@@ -2138,7 +2382,7 @@
       </c>
       <c r="C88" s="5"/>
     </row>
-    <row r="89" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89" s="5" t="s">
         <v>83</v>
       </c>
@@ -2147,7 +2391,7 @@
       </c>
       <c r="C89" s="5"/>
     </row>
-    <row r="90" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90" s="5" t="s">
         <v>83</v>
       </c>
@@ -2156,7 +2400,7 @@
       </c>
       <c r="C90" s="5"/>
     </row>
-    <row r="91" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91" s="5" t="s">
         <v>83</v>
       </c>
@@ -2165,7 +2409,7 @@
       </c>
       <c r="C91" s="5"/>
     </row>
-    <row r="92" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92" s="5" t="s">
         <v>83</v>
       </c>
@@ -2176,7 +2420,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="93" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93" s="5" t="s">
         <v>83</v>
       </c>
@@ -2185,7 +2429,7 @@
       </c>
       <c r="C93" s="5"/>
     </row>
-    <row r="94" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94" s="5" t="s">
         <v>83</v>
       </c>
@@ -2194,7 +2438,7 @@
       </c>
       <c r="C94" s="5"/>
     </row>
-    <row r="95" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95" s="5" t="s">
         <v>83</v>
       </c>
@@ -2203,7 +2447,7 @@
       </c>
       <c r="C95" s="5"/>
     </row>
-    <row r="96" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96" s="5" t="s">
         <v>83</v>
       </c>
@@ -2212,7 +2456,7 @@
       </c>
       <c r="C96" s="5"/>
     </row>
-    <row r="97" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97" s="5" t="s">
         <v>83</v>
       </c>
@@ -2221,7 +2465,7 @@
       </c>
       <c r="C97" s="5"/>
     </row>
-    <row r="98" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98" s="5" t="s">
         <v>83</v>
       </c>
@@ -2230,7 +2474,7 @@
       </c>
       <c r="C98" s="5"/>
     </row>
-    <row r="99" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99" s="5" t="s">
         <v>83</v>
       </c>
@@ -2241,7 +2485,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="100" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100" s="5" t="s">
         <v>83</v>
       </c>
@@ -2252,7 +2496,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="101" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101" s="5" t="s">
         <v>83</v>
       </c>
@@ -2261,7 +2505,7 @@
       </c>
       <c r="C101" s="5"/>
     </row>
-    <row r="102" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102" s="5" t="s">
         <v>83</v>
       </c>
@@ -2270,7 +2514,7 @@
       </c>
       <c r="C102" s="5"/>
     </row>
-    <row r="103" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103" s="5" t="s">
         <v>83</v>
       </c>
@@ -2279,7 +2523,7 @@
       </c>
       <c r="C103" s="5"/>
     </row>
-    <row r="104" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A104" s="5" t="s">
         <v>83</v>
       </c>
@@ -2288,7 +2532,7 @@
       </c>
       <c r="C104" s="5"/>
     </row>
-    <row r="105" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105" s="5" t="s">
         <v>83</v>
       </c>
@@ -2297,7 +2541,7 @@
       </c>
       <c r="C105" s="5"/>
     </row>
-    <row r="106" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A106" s="5" t="s">
         <v>83</v>
       </c>
@@ -2306,7 +2550,7 @@
       </c>
       <c r="C106" s="5"/>
     </row>
-    <row r="107" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A107" s="5" t="s">
         <v>83</v>
       </c>
@@ -2315,7 +2559,7 @@
       </c>
       <c r="C107" s="5"/>
     </row>
-    <row r="108" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A108" s="5" t="s">
         <v>83</v>
       </c>
@@ -2324,7 +2568,7 @@
       </c>
       <c r="C108" s="5"/>
     </row>
-    <row r="109" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A109" s="5" t="s">
         <v>83</v>
       </c>
@@ -2333,7 +2577,7 @@
       </c>
       <c r="C109" s="5"/>
     </row>
-    <row r="110" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A110" s="5" t="s">
         <v>83</v>
       </c>
@@ -2342,7 +2586,7 @@
       </c>
       <c r="C110" s="5"/>
     </row>
-    <row r="111" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A111" s="5" t="s">
         <v>83</v>
       </c>
@@ -2351,7 +2595,7 @@
       </c>
       <c r="C111" s="5"/>
     </row>
-    <row r="112" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A112" s="5" t="s">
         <v>83</v>
       </c>
@@ -2360,7 +2604,7 @@
       </c>
       <c r="C112" s="5"/>
     </row>
-    <row r="113" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113" s="5" t="s">
         <v>83</v>
       </c>
@@ -2369,7 +2613,7 @@
       </c>
       <c r="C113" s="5"/>
     </row>
-    <row r="114" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A114" s="5" t="s">
         <v>83</v>
       </c>
@@ -2378,7 +2622,7 @@
       </c>
       <c r="C114" s="5"/>
     </row>
-    <row r="115" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A115" s="5" t="s">
         <v>83</v>
       </c>
@@ -2389,7 +2633,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="116" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A116" s="5" t="s">
         <v>83</v>
       </c>
@@ -2398,7 +2642,7 @@
       </c>
       <c r="C116" s="5"/>
     </row>
-    <row r="117" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A117" s="5" t="s">
         <v>83</v>
       </c>
@@ -2407,7 +2651,7 @@
       </c>
       <c r="C117" s="5"/>
     </row>
-    <row r="118" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118" s="5" t="s">
         <v>83</v>
       </c>
@@ -2416,8 +2660,8 @@
       </c>
       <c r="C118" s="5"/>
     </row>
-    <row r="119" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A119" s="0" t="s">
+    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A119" t="s">
         <v>144</v>
       </c>
       <c r="B119" s="4" t="s">
@@ -2427,7 +2671,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="120" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A120" s="5" t="s">
         <v>144</v>
       </c>
@@ -2438,7 +2682,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="121" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A121" s="5" t="s">
         <v>144</v>
       </c>
@@ -2446,7 +2690,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="122" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A122" s="5" t="s">
         <v>144</v>
       </c>
@@ -2457,7 +2701,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="123" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A123" s="5" t="s">
         <v>144</v>
       </c>
@@ -2468,7 +2712,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="124" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A124" s="5" t="s">
         <v>144</v>
       </c>
@@ -2476,10 +2720,13 @@
         <v>34</v>
       </c>
       <c r="C124" s="5" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="125" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>35</v>
+      </c>
+      <c r="D124" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A125" s="5" t="s">
         <v>144</v>
       </c>
@@ -2490,7 +2737,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="126" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A126" s="5" t="s">
         <v>144</v>
       </c>
@@ -2501,7 +2748,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="127" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A127" s="5" t="s">
         <v>144</v>
       </c>
@@ -2512,7 +2759,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="128" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A128" s="5" t="s">
         <v>144</v>
       </c>
@@ -2523,8 +2770,8 @@
         <v>47</v>
       </c>
     </row>
-    <row r="129" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A129" s="0" t="s">
+    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A129" t="s">
         <v>150</v>
       </c>
       <c r="B129" s="4" t="s">
@@ -2534,7 +2781,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="130" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A130" s="5" t="s">
         <v>150</v>
       </c>
@@ -2545,7 +2792,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="131" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A131" s="5" t="s">
         <v>150</v>
       </c>
@@ -2556,7 +2803,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="132" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A132" s="5" t="s">
         <v>150</v>
       </c>
@@ -2567,7 +2814,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="133" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A133" s="5" t="s">
         <v>150</v>
       </c>
@@ -2578,7 +2825,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="134" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A134" s="5" t="s">
         <v>150</v>
       </c>
@@ -2589,7 +2836,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="135" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A135" s="5" t="s">
         <v>150</v>
       </c>
@@ -2600,7 +2847,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="136" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A136" s="5" t="s">
         <v>150</v>
       </c>
@@ -2611,7 +2858,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="137" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A137" s="5" t="s">
         <v>150</v>
       </c>
@@ -2622,7 +2869,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="138" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A138" s="5" t="s">
         <v>150</v>
       </c>
@@ -2633,8 +2880,8 @@
         <v>42</v>
       </c>
     </row>
-    <row r="139" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A139" s="0" t="s">
+    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A139" t="s">
         <v>158</v>
       </c>
       <c r="B139" s="4" t="s">
@@ -2644,7 +2891,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="140" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A140" s="5" t="s">
         <v>158</v>
       </c>
@@ -2655,7 +2902,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="141" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A141" s="5" t="s">
         <v>158</v>
       </c>
@@ -2666,7 +2913,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="142" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="142" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A142" s="5" t="s">
         <v>158</v>
       </c>
@@ -2677,7 +2924,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="143" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="143" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A143" s="5" t="s">
         <v>158</v>
       </c>
@@ -2688,7 +2935,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="144" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="144" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A144" s="5" t="s">
         <v>158</v>
       </c>
@@ -2699,509 +2946,516 @@
         <v>37</v>
       </c>
     </row>
-    <row r="145" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="145" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A145" s="5" t="s">
         <v>158</v>
       </c>
       <c r="B145" s="4" t="s">
-        <v>164</v>
+        <v>67</v>
       </c>
       <c r="C145" s="5" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="146" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="146" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A146" s="5" t="s">
         <v>158</v>
       </c>
       <c r="B146" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="C146" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="147" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A147" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="B147" s="4" t="s">
         <v>165</v>
       </c>
-      <c r="C146" s="5"/>
-    </row>
-    <row r="147" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A147" s="0" t="s">
+      <c r="C147" s="5"/>
+    </row>
+    <row r="148" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A148" t="s">
         <v>166</v>
       </c>
-      <c r="B147" s="4" t="s">
+      <c r="B148" s="4" t="s">
         <v>167</v>
       </c>
-      <c r="C147" s="5" t="s">
+      <c r="C148" s="5" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="148" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A148" s="5" t="s">
-        <v>166</v>
-      </c>
-      <c r="B148" s="4" t="s">
-        <v>168</v>
-      </c>
-      <c r="C148" s="5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="149" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="149" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A149" s="5" t="s">
         <v>166</v>
       </c>
       <c r="B149" s="4" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C149" s="5" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="150" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="150" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A150" s="5" t="s">
         <v>166</v>
       </c>
       <c r="B150" s="4" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C150" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="151" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="151" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A151" s="5" t="s">
         <v>166</v>
       </c>
       <c r="B151" s="4" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C151" s="5" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="152" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="152" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A152" s="5" t="s">
         <v>166</v>
       </c>
       <c r="B152" s="4" t="s">
-        <v>172</v>
-      </c>
-      <c r="C152" s="5"/>
-    </row>
-    <row r="153" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>171</v>
+      </c>
+      <c r="C152" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="153" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A153" s="5" t="s">
         <v>166</v>
       </c>
       <c r="B153" s="4" t="s">
-        <v>173</v>
-      </c>
-      <c r="C153" s="5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="154" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>172</v>
+      </c>
+      <c r="C153" s="5"/>
+    </row>
+    <row r="154" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A154" s="5" t="s">
         <v>166</v>
       </c>
       <c r="B154" s="4" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C154" s="5" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="155" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="155" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A155" s="5" t="s">
         <v>166</v>
       </c>
       <c r="B155" s="4" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C155" s="5" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="156" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="156" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A156" s="5" t="s">
         <v>166</v>
       </c>
       <c r="B156" s="4" t="s">
-        <v>103</v>
+        <v>175</v>
       </c>
       <c r="C156" s="5" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="157" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="157" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A157" s="5" t="s">
         <v>166</v>
       </c>
       <c r="B157" s="4" t="s">
-        <v>176</v>
+        <v>103</v>
       </c>
       <c r="C157" s="5" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="158" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="158" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A158" s="5" t="s">
         <v>166</v>
       </c>
       <c r="B158" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="C158" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="159" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A159" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="B159" s="4" t="s">
         <v>177</v>
       </c>
-      <c r="C158" s="5" t="s">
+      <c r="C159" s="5" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="159" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A159" s="0" t="s">
+    <row r="160" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A160" t="s">
         <v>178</v>
       </c>
-      <c r="B159" s="5" t="s">
+      <c r="B160" s="5" t="s">
         <v>179</v>
       </c>
-      <c r="C159" s="5" t="s">
+      <c r="C160" s="5" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="160" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A160" s="0" t="s">
+    <row r="161" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A161" t="s">
         <v>178</v>
       </c>
-      <c r="B160" s="5" t="s">
+      <c r="B161" s="5" t="s">
         <v>180</v>
       </c>
-      <c r="C160" s="5" t="s">
+      <c r="C161" s="5" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="161" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A161" s="0" t="s">
+    <row r="162" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A162" t="s">
         <v>178</v>
       </c>
-      <c r="B161" s="5" t="s">
+      <c r="B162" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="C161" s="5" t="s">
+      <c r="C162" s="5" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="162" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A162" s="0" t="s">
+    <row r="163" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A163" t="s">
         <v>178</v>
       </c>
-      <c r="B162" s="5" t="s">
+      <c r="B163" s="5" t="s">
         <v>181</v>
       </c>
-      <c r="C162" s="5" t="s">
+      <c r="C163" s="5" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="163" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A163" s="0" t="s">
+    <row r="164" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A164" t="s">
         <v>178</v>
       </c>
-      <c r="B163" s="5" t="s">
+      <c r="B164" s="5" t="s">
         <v>159</v>
-      </c>
-      <c r="C163" s="5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="164" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A164" s="0" t="s">
-        <v>182</v>
-      </c>
-      <c r="B164" s="0" t="s">
-        <v>167</v>
       </c>
       <c r="C164" s="5" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="165" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A165" s="5" t="s">
+    <row r="165" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A165" t="s">
         <v>182</v>
       </c>
-      <c r="B165" s="0" t="s">
-        <v>183</v>
+      <c r="B165" t="s">
+        <v>167</v>
       </c>
       <c r="C165" s="5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="166" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="166" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A166" s="5" t="s">
         <v>182</v>
       </c>
-      <c r="B166" s="0" t="s">
-        <v>146</v>
+      <c r="B166" t="s">
+        <v>183</v>
       </c>
       <c r="C166" s="5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="167" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="167" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A167" s="5" t="s">
         <v>182</v>
       </c>
-      <c r="B167" s="0" t="s">
-        <v>126</v>
+      <c r="B167" t="s">
+        <v>146</v>
       </c>
       <c r="C167" s="5" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="168" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="168" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A168" s="5" t="s">
         <v>182</v>
       </c>
-      <c r="B168" s="0" t="s">
+      <c r="B168" t="s">
+        <v>126</v>
+      </c>
+      <c r="C168" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="169" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A169" s="5" t="s">
+        <v>182</v>
+      </c>
+      <c r="B169" t="s">
         <v>184</v>
       </c>
-      <c r="C168" s="5" t="s">
+      <c r="C169" s="5" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="169" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A169" s="0" t="s">
+    <row r="170" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A170" t="s">
         <v>185</v>
       </c>
-      <c r="B169" s="0" t="s">
+      <c r="B170" t="s">
         <v>167</v>
       </c>
-      <c r="C169" s="5" t="s">
+      <c r="C170" s="5" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="170" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A170" s="5" t="s">
-        <v>185</v>
-      </c>
-      <c r="B170" s="0" t="s">
-        <v>175</v>
-      </c>
-      <c r="C170" s="5" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="171" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="171" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A171" s="5" t="s">
         <v>185</v>
       </c>
-      <c r="B171" s="0" t="s">
-        <v>69</v>
+      <c r="B171" t="s">
+        <v>175</v>
       </c>
       <c r="C171" s="5" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="172" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="172" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A172" s="5" t="s">
         <v>185</v>
       </c>
-      <c r="B172" s="0" t="s">
-        <v>70</v>
+      <c r="B172" t="s">
+        <v>69</v>
       </c>
       <c r="C172" s="5" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="173" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="173" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A173" s="5" t="s">
         <v>185</v>
       </c>
-      <c r="B173" s="0" t="s">
-        <v>67</v>
+      <c r="B173" t="s">
+        <v>70</v>
       </c>
       <c r="C173" s="5" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="174" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="174" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A174" s="5" t="s">
         <v>185</v>
       </c>
-      <c r="B174" s="0" t="s">
-        <v>76</v>
+      <c r="B174" t="s">
+        <v>67</v>
       </c>
       <c r="C174" s="5" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="175" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="175" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A175" s="5" t="s">
         <v>185</v>
       </c>
-      <c r="B175" s="0" t="s">
-        <v>126</v>
+      <c r="B175" t="s">
+        <v>76</v>
       </c>
       <c r="C175" s="5" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="176" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="176" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A176" s="5" t="s">
         <v>185</v>
       </c>
-      <c r="B176" s="0" t="s">
-        <v>186</v>
+      <c r="B176" t="s">
+        <v>126</v>
       </c>
       <c r="C176" s="5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="177" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="177" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A177" s="5" t="s">
         <v>185</v>
       </c>
-      <c r="B177" s="0" t="s">
-        <v>58</v>
+      <c r="B177" t="s">
+        <v>186</v>
       </c>
       <c r="C177" s="5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="178" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="178" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A178" s="5" t="s">
         <v>185</v>
       </c>
-      <c r="B178" s="0" t="s">
+      <c r="B178" t="s">
+        <v>58</v>
+      </c>
+      <c r="C178" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="179" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A179" s="5" t="s">
+        <v>185</v>
+      </c>
+      <c r="B179" t="s">
         <v>140</v>
       </c>
-      <c r="C178" s="5" t="s">
+      <c r="C179" s="5" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="179" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A179" s="5" t="s">
-        <v>187</v>
-      </c>
-      <c r="B179" s="4" t="s">
-        <v>152</v>
-      </c>
-      <c r="C179" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="D179" s="0" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="180" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="180" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A180" s="5" t="s">
         <v>187</v>
       </c>
       <c r="B180" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="C180" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="D180" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="181" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A181" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="B181" s="4" t="s">
         <v>189</v>
       </c>
-      <c r="C180" s="5" t="s">
+      <c r="C181" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="D180" s="5" t="s">
+      <c r="D181" s="5" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="181" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A181" s="0" t="s">
+    <row r="182" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A182" t="s">
         <v>190</v>
       </c>
-      <c r="B181" s="0" t="s">
+      <c r="B182" t="s">
         <v>191</v>
       </c>
-      <c r="C181" s="0" t="s">
+      <c r="C182" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="182" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A182" s="0" t="s">
+    <row r="183" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A183" t="s">
         <v>190</v>
       </c>
-      <c r="B182" s="0" t="s">
+      <c r="B183" t="s">
         <v>192</v>
       </c>
-      <c r="C182" s="0" t="s">
+      <c r="C183" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="183" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A183" s="0" t="s">
+    <row r="184" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A184" t="s">
         <v>190</v>
       </c>
-      <c r="B183" s="0" t="s">
+      <c r="B184" t="s">
         <v>25</v>
       </c>
-      <c r="C183" s="0" t="s">
+      <c r="C184" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="184" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A184" s="0" t="s">
+    <row r="185" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A185" t="s">
         <v>190</v>
       </c>
-      <c r="B184" s="0" t="s">
+      <c r="B185" t="s">
         <v>37</v>
       </c>
-      <c r="C184" s="0" t="s">
+      <c r="C185" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="185" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A185" s="0" t="s">
+    <row r="186" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A186" t="s">
         <v>190</v>
       </c>
-      <c r="B185" s="0" t="s">
+      <c r="B186" t="s">
         <v>36</v>
       </c>
-      <c r="C185" s="0" t="s">
+      <c r="C186" t="s">
         <v>36</v>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="1">
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C1:C120 C122:C180" type="list">
-      <formula1>controlled_vocabulary!$A:$A</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-  </dataValidations>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000000000000}">
+          <x14:formula1>
+            <xm:f>controlled_vocabulary!$A:$A</xm:f>
+          </x14:formula1>
+          <x14:formula2>
+            <xm:f>0</xm:f>
+          </x14:formula2>
+          <xm:sqref>C1:C120 C122:C181</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.53"/>
+    <col min="1" max="1025" width="8.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>194</v>
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fix that all-optional samples are set to zero.
Before, we encountered the issue that
in a dataset that contained neither macrophage nor monocyte data
an artificial Macrophage/Monocyte=0 entry was added as both subtypes
are optional.

Now the 'optional' rule only applies, if at least one of the child
entries is available.
</commit_message>
<xml_diff>
--- a/inst/extdata/cell_type_mapping.xlsx
+++ b/inst/extdata/cell_type_mapping.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Y:\projects\immune_deconvolution_benchmark\immunedeconv\inst\extdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Y:\projects\immune_deconvolution\benchmark_pipeline\immunedeconv\inst\extdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{5413D193-B82C-4539-9C1A-9A2C1867FC31}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{5D80353C-9992-4558-BDB8-BC7B8E3A0FA4}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14025" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14025" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="controlled_vocabulary" sheetId="1" r:id="rId1"/>
@@ -1005,8 +1005,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AMK45"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C37" sqref="C37:D37"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1311,7 +1311,6 @@
         <v>35</v>
       </c>
       <c r="C32" s="1" t="b">
-        <f>TRUE()</f>
         <v>1</v>
       </c>
       <c r="O32" s="2"/>
@@ -1431,7 +1430,7 @@
       </c>
     </row>
   </sheetData>
-  <dataValidations count="1">
+  <dataValidations disablePrompts="1" count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1 B41:B45 B32:B39 B15:B30 B12:B13 B8:B9 B3:B6" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>$A:$A</formula1>
       <formula2>0</formula2>
@@ -1446,7 +1445,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E186"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A97" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A97" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D125" sqref="D125"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
map hoek mono to Monocytes instead of Macrophage/Monocyte
</commit_message>
<xml_diff>
--- a/inst/extdata/cell_type_mapping.xlsx
+++ b/inst/extdata/cell_type_mapping.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Y:\projects\immune_deconvolution\benchmark_pipeline\immunedeconv\inst\extdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{5D80353C-9992-4558-BDB8-BC7B8E3A0FA4}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{710AABC1-3A34-4ADD-8A2C-42B0B05C99FF}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14025" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9525" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="controlled_vocabulary" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="605" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="609" uniqueCount="196">
   <si>
     <t>cell_type</t>
   </si>
@@ -1005,7 +1005,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AMK45"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
@@ -1443,10 +1443,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:E186"/>
+  <dimension ref="A1:E187"/>
   <sheetViews>
-    <sheetView topLeftCell="A97" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D125" sqref="D125"/>
+    <sheetView tabSelected="1" topLeftCell="A118" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C125" sqref="C125"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2719,7 +2719,7 @@
         <v>34</v>
       </c>
       <c r="C124" s="5" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D124" t="s">
         <v>195</v>
@@ -2730,10 +2730,13 @@
         <v>144</v>
       </c>
       <c r="B125" s="4" t="s">
-        <v>149</v>
+        <v>34</v>
       </c>
       <c r="C125" s="5" t="s">
-        <v>42</v>
+        <v>35</v>
+      </c>
+      <c r="D125" t="s">
+        <v>195</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.25">
@@ -2741,10 +2744,10 @@
         <v>144</v>
       </c>
       <c r="B126" s="4" t="s">
-        <v>76</v>
+        <v>149</v>
       </c>
       <c r="C126" s="5" t="s">
-        <v>29</v>
+        <v>42</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.25">
@@ -2752,10 +2755,10 @@
         <v>144</v>
       </c>
       <c r="B127" s="4" t="s">
-        <v>103</v>
+        <v>76</v>
       </c>
       <c r="C127" s="5" t="s">
-        <v>46</v>
+        <v>29</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.25">
@@ -2763,32 +2766,32 @@
         <v>144</v>
       </c>
       <c r="B128" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="C128" s="5" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A129" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="B129" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="C128" s="5" t="s">
+      <c r="C129" s="5" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A129" t="s">
+    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A130" t="s">
         <v>150</v>
       </c>
-      <c r="B129" s="4" t="s">
+      <c r="B130" s="4" t="s">
         <v>151</v>
       </c>
-      <c r="C129" s="5" t="s">
+      <c r="C130" s="5" t="s">
         <v>21</v>
-      </c>
-    </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A130" s="5" t="s">
-        <v>150</v>
-      </c>
-      <c r="B130" s="4" t="s">
-        <v>152</v>
-      </c>
-      <c r="C130" s="5" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.25">
@@ -2796,10 +2799,10 @@
         <v>150</v>
       </c>
       <c r="B131" s="4" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C131" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.25">
@@ -2807,10 +2810,10 @@
         <v>150</v>
       </c>
       <c r="B132" s="4" t="s">
-        <v>67</v>
+        <v>153</v>
       </c>
       <c r="C132" s="5" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.25">
@@ -2818,10 +2821,10 @@
         <v>150</v>
       </c>
       <c r="B133" s="4" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="C133" s="5" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.25">
@@ -2829,10 +2832,10 @@
         <v>150</v>
       </c>
       <c r="B134" s="4" t="s">
-        <v>154</v>
+        <v>76</v>
       </c>
       <c r="C134" s="5" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.25">
@@ -2840,10 +2843,10 @@
         <v>150</v>
       </c>
       <c r="B135" s="4" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C135" s="5" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.25">
@@ -2851,10 +2854,10 @@
         <v>150</v>
       </c>
       <c r="B136" s="4" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C136" s="5" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.25">
@@ -2862,10 +2865,10 @@
         <v>150</v>
       </c>
       <c r="B137" s="4" t="s">
-        <v>140</v>
+        <v>156</v>
       </c>
       <c r="C137" s="5" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.25">
@@ -2873,32 +2876,32 @@
         <v>150</v>
       </c>
       <c r="B138" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="C138" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A139" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="B139" s="4" t="s">
         <v>157</v>
       </c>
-      <c r="C138" s="5" t="s">
+      <c r="C139" s="5" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A139" t="s">
+    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A140" t="s">
         <v>158</v>
       </c>
-      <c r="B139" s="4" t="s">
+      <c r="B140" s="4" t="s">
         <v>159</v>
       </c>
-      <c r="C139" s="5" t="s">
+      <c r="C140" s="5" t="s">
         <v>21</v>
-      </c>
-    </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A140" s="5" t="s">
-        <v>158</v>
-      </c>
-      <c r="B140" s="4" t="s">
-        <v>160</v>
-      </c>
-      <c r="C140" s="5" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.25">
@@ -2906,10 +2909,10 @@
         <v>158</v>
       </c>
       <c r="B141" s="4" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C141" s="5" t="s">
-        <v>11</v>
+        <v>47</v>
       </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.25">
@@ -2917,10 +2920,10 @@
         <v>158</v>
       </c>
       <c r="B142" s="4" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C142" s="5" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.25">
@@ -2928,10 +2931,10 @@
         <v>158</v>
       </c>
       <c r="B143" s="4" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C143" s="5" t="s">
-        <v>46</v>
+        <v>8</v>
       </c>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.25">
@@ -2939,10 +2942,10 @@
         <v>158</v>
       </c>
       <c r="B144" s="4" t="s">
-        <v>113</v>
+        <v>163</v>
       </c>
       <c r="C144" s="5" t="s">
-        <v>37</v>
+        <v>46</v>
       </c>
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.25">
@@ -2950,10 +2953,10 @@
         <v>158</v>
       </c>
       <c r="B145" s="4" t="s">
-        <v>67</v>
+        <v>113</v>
       </c>
       <c r="C145" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.25">
@@ -2961,10 +2964,10 @@
         <v>158</v>
       </c>
       <c r="B146" s="4" t="s">
-        <v>164</v>
+        <v>67</v>
       </c>
       <c r="C146" s="5" t="s">
-        <v>25</v>
+        <v>36</v>
       </c>
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.25">
@@ -2972,30 +2975,30 @@
         <v>158</v>
       </c>
       <c r="B147" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="C147" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="148" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A148" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="B148" s="4" t="s">
         <v>165</v>
       </c>
-      <c r="C147" s="5"/>
-    </row>
-    <row r="148" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A148" t="s">
+      <c r="C148" s="5"/>
+    </row>
+    <row r="149" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A149" t="s">
         <v>166</v>
       </c>
-      <c r="B148" s="4" t="s">
+      <c r="B149" s="4" t="s">
         <v>167</v>
       </c>
-      <c r="C148" s="5" t="s">
+      <c r="C149" s="5" t="s">
         <v>21</v>
-      </c>
-    </row>
-    <row r="149" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A149" s="5" t="s">
-        <v>166</v>
-      </c>
-      <c r="B149" s="4" t="s">
-        <v>168</v>
-      </c>
-      <c r="C149" s="5" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.25">
@@ -3003,10 +3006,10 @@
         <v>166</v>
       </c>
       <c r="B150" s="4" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C150" s="5" t="s">
-        <v>50</v>
+        <v>8</v>
       </c>
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.25">
@@ -3014,10 +3017,10 @@
         <v>166</v>
       </c>
       <c r="B151" s="4" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C151" s="5" t="s">
-        <v>12</v>
+        <v>50</v>
       </c>
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.25">
@@ -3025,10 +3028,10 @@
         <v>166</v>
       </c>
       <c r="B152" s="4" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C152" s="5" t="s">
-        <v>35</v>
+        <v>12</v>
       </c>
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.25">
@@ -3036,30 +3039,30 @@
         <v>166</v>
       </c>
       <c r="B153" s="4" t="s">
-        <v>172</v>
-      </c>
-      <c r="C153" s="5"/>
+        <v>171</v>
+      </c>
+      <c r="C153" s="5" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A154" s="5" t="s">
         <v>166</v>
       </c>
       <c r="B154" s="4" t="s">
-        <v>173</v>
-      </c>
-      <c r="C154" s="5" t="s">
-        <v>18</v>
-      </c>
+        <v>172</v>
+      </c>
+      <c r="C154" s="5"/>
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A155" s="5" t="s">
         <v>166</v>
       </c>
       <c r="B155" s="4" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C155" s="5" t="s">
-        <v>47</v>
+        <v>18</v>
       </c>
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.25">
@@ -3067,10 +3070,10 @@
         <v>166</v>
       </c>
       <c r="B156" s="4" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C156" s="5" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.25">
@@ -3078,10 +3081,10 @@
         <v>166</v>
       </c>
       <c r="B157" s="4" t="s">
-        <v>103</v>
+        <v>175</v>
       </c>
       <c r="C157" s="5" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.25">
@@ -3089,10 +3092,10 @@
         <v>166</v>
       </c>
       <c r="B158" s="4" t="s">
-        <v>176</v>
+        <v>103</v>
       </c>
       <c r="C158" s="5" t="s">
-        <v>25</v>
+        <v>46</v>
       </c>
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.25">
@@ -3100,21 +3103,21 @@
         <v>166</v>
       </c>
       <c r="B159" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="C159" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="160" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A160" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="B160" s="4" t="s">
         <v>177</v>
       </c>
-      <c r="C159" s="5" t="s">
+      <c r="C160" s="5" t="s">
         <v>49</v>
-      </c>
-    </row>
-    <row r="160" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A160" t="s">
-        <v>178</v>
-      </c>
-      <c r="B160" s="5" t="s">
-        <v>179</v>
-      </c>
-      <c r="C160" s="5" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.25">
@@ -3122,10 +3125,10 @@
         <v>178</v>
       </c>
       <c r="B161" s="5" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C161" s="5" t="s">
-        <v>25</v>
+        <v>7</v>
       </c>
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.25">
@@ -3133,10 +3136,10 @@
         <v>178</v>
       </c>
       <c r="B162" s="5" t="s">
-        <v>82</v>
+        <v>180</v>
       </c>
       <c r="C162" s="5" t="s">
-        <v>42</v>
+        <v>25</v>
       </c>
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.25">
@@ -3144,10 +3147,10 @@
         <v>178</v>
       </c>
       <c r="B163" s="5" t="s">
-        <v>181</v>
+        <v>82</v>
       </c>
       <c r="C163" s="5" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.25">
@@ -3155,32 +3158,32 @@
         <v>178</v>
       </c>
       <c r="B164" s="5" t="s">
-        <v>159</v>
+        <v>181</v>
       </c>
       <c r="C164" s="5" t="s">
-        <v>21</v>
+        <v>36</v>
       </c>
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>182</v>
-      </c>
-      <c r="B165" t="s">
-        <v>167</v>
+        <v>178</v>
+      </c>
+      <c r="B165" s="5" t="s">
+        <v>159</v>
       </c>
       <c r="C165" s="5" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A166" s="5" t="s">
+      <c r="A166" t="s">
         <v>182</v>
       </c>
       <c r="B166" t="s">
-        <v>183</v>
+        <v>167</v>
       </c>
       <c r="C166" s="5" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.25">
@@ -3188,10 +3191,10 @@
         <v>182</v>
       </c>
       <c r="B167" t="s">
-        <v>146</v>
+        <v>183</v>
       </c>
       <c r="C167" s="5" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.25">
@@ -3199,10 +3202,10 @@
         <v>182</v>
       </c>
       <c r="B168" t="s">
-        <v>126</v>
+        <v>146</v>
       </c>
       <c r="C168" s="5" t="s">
-        <v>25</v>
+        <v>8</v>
       </c>
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.25">
@@ -3210,32 +3213,32 @@
         <v>182</v>
       </c>
       <c r="B169" t="s">
+        <v>126</v>
+      </c>
+      <c r="C169" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="170" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A170" s="5" t="s">
+        <v>182</v>
+      </c>
+      <c r="B170" t="s">
         <v>184</v>
       </c>
-      <c r="C169" s="5" t="s">
+      <c r="C170" s="5" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="170" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A170" t="s">
+    <row r="171" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A171" t="s">
         <v>185</v>
       </c>
-      <c r="B170" t="s">
+      <c r="B171" t="s">
         <v>167</v>
       </c>
-      <c r="C170" s="5" t="s">
+      <c r="C171" s="5" t="s">
         <v>21</v>
-      </c>
-    </row>
-    <row r="171" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A171" s="5" t="s">
-        <v>185</v>
-      </c>
-      <c r="B171" t="s">
-        <v>175</v>
-      </c>
-      <c r="C171" s="5" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.25">
@@ -3243,10 +3246,10 @@
         <v>185</v>
       </c>
       <c r="B172" t="s">
-        <v>69</v>
+        <v>175</v>
       </c>
       <c r="C172" s="5" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="173" spans="1:3" x14ac:dyDescent="0.25">
@@ -3254,10 +3257,10 @@
         <v>185</v>
       </c>
       <c r="B173" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C173" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="174" spans="1:3" x14ac:dyDescent="0.25">
@@ -3265,10 +3268,10 @@
         <v>185</v>
       </c>
       <c r="B174" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="C174" s="5" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
     </row>
     <row r="175" spans="1:3" x14ac:dyDescent="0.25">
@@ -3276,10 +3279,10 @@
         <v>185</v>
       </c>
       <c r="B175" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="C175" s="5" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
     </row>
     <row r="176" spans="1:3" x14ac:dyDescent="0.25">
@@ -3287,10 +3290,10 @@
         <v>185</v>
       </c>
       <c r="B176" t="s">
-        <v>126</v>
+        <v>76</v>
       </c>
       <c r="C176" s="5" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
     </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.25">
@@ -3298,10 +3301,10 @@
         <v>185</v>
       </c>
       <c r="B177" t="s">
-        <v>186</v>
+        <v>126</v>
       </c>
       <c r="C177" s="5" t="s">
-        <v>11</v>
+        <v>25</v>
       </c>
     </row>
     <row r="178" spans="1:4" x14ac:dyDescent="0.25">
@@ -3309,10 +3312,10 @@
         <v>185</v>
       </c>
       <c r="B178" t="s">
-        <v>58</v>
+        <v>186</v>
       </c>
       <c r="C178" s="5" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.25">
@@ -3320,24 +3323,21 @@
         <v>185</v>
       </c>
       <c r="B179" t="s">
-        <v>140</v>
+        <v>58</v>
       </c>
       <c r="C179" s="5" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
     </row>
     <row r="180" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A180" s="5" t="s">
-        <v>187</v>
-      </c>
-      <c r="B180" s="4" t="s">
-        <v>152</v>
+        <v>185</v>
+      </c>
+      <c r="B180" t="s">
+        <v>140</v>
       </c>
       <c r="C180" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="D180" t="s">
-        <v>188</v>
+        <v>18</v>
       </c>
     </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.25">
@@ -3345,24 +3345,27 @@
         <v>187</v>
       </c>
       <c r="B181" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="C181" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="D181" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="182" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A182" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="B182" s="4" t="s">
         <v>189</v>
       </c>
-      <c r="C181" s="5" t="s">
+      <c r="C182" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="D181" s="5" t="s">
+      <c r="D182" s="5" t="s">
         <v>188</v>
-      </c>
-    </row>
-    <row r="182" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A182" t="s">
-        <v>190</v>
-      </c>
-      <c r="B182" t="s">
-        <v>191</v>
-      </c>
-      <c r="C182" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="183" spans="1:4" x14ac:dyDescent="0.25">
@@ -3370,10 +3373,10 @@
         <v>190</v>
       </c>
       <c r="B183" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C183" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
     </row>
     <row r="184" spans="1:4" x14ac:dyDescent="0.25">
@@ -3381,10 +3384,10 @@
         <v>190</v>
       </c>
       <c r="B184" t="s">
-        <v>25</v>
+        <v>192</v>
       </c>
       <c r="C184" t="s">
-        <v>25</v>
+        <v>8</v>
       </c>
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.25">
@@ -3392,10 +3395,10 @@
         <v>190</v>
       </c>
       <c r="B185" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="C185" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
     </row>
     <row r="186" spans="1:4" x14ac:dyDescent="0.25">
@@ -3403,9 +3406,20 @@
         <v>190</v>
       </c>
       <c r="B186" t="s">
+        <v>37</v>
+      </c>
+      <c r="C186" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="187" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A187" t="s">
+        <v>190</v>
+      </c>
+      <c r="B187" t="s">
         <v>36</v>
       </c>
-      <c r="C186" t="s">
+      <c r="C187" t="s">
         <v>36</v>
       </c>
     </row>
@@ -3422,7 +3436,7 @@
           <x14:formula2>
             <xm:f>0</xm:f>
           </x14:formula2>
-          <xm:sqref>C1:C120 C122:C181</xm:sqref>
+          <xm:sqref>C1:C120 C122:C182</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
fix root node in cell type tree
</commit_message>
<xml_diff>
--- a/inst/extdata/cell_type_mapping.xlsx
+++ b/inst/extdata/cell_type_mapping.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="controlled_vocabulary" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="708" uniqueCount="223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="710" uniqueCount="223">
   <si>
     <t xml:space="preserve">cell_type</t>
   </si>
@@ -33,13 +33,16 @@
     <t xml:space="preserve">optional</t>
   </si>
   <si>
-    <t xml:space="preserve">description</t>
+    <t xml:space="preserve">comment</t>
   </si>
   <si>
     <t xml:space="preserve">cell</t>
   </si>
   <si>
-    <t xml:space="preserve">root</t>
+    <t xml:space="preserve">root2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">root is a protected entity in the data.tree library</t>
   </si>
   <si>
     <t xml:space="preserve">score</t>
@@ -247,9 +250,6 @@
   </si>
   <si>
     <t xml:space="preserve">method_cell_type</t>
-  </si>
-  <si>
-    <t xml:space="preserve">comment</t>
   </si>
   <si>
     <t xml:space="preserve">cibersort</t>
@@ -841,90 +841,6 @@
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>2590200</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>-25200</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>90000</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>25200</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp>
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="0" name="Ellipse 1"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="2590200" y="-25200"/>
-          <a:ext cx="2415960" cy="225360"/>
-        </a:xfrm>
-        <a:prstGeom prst="ellipse">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln w="19800">
-          <a:solidFill>
-            <a:srgbClr val="ff0000"/>
-          </a:solidFill>
-          <a:round/>
-        </a:ln>
-      </xdr:spPr>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>2285640</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>-25200</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>90000</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>25200</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp>
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="1" name="Ellipse 1"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="4050720" y="-25200"/>
-          <a:ext cx="2835000" cy="225360"/>
-        </a:xfrm>
-        <a:prstGeom prst="ellipse">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln w="19800">
-          <a:solidFill>
-            <a:srgbClr val="ff0000"/>
-          </a:solidFill>
-          <a:round/>
-        </a:ln>
-      </xdr:spPr>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
@@ -932,8 +848,8 @@
   </sheetPr>
   <dimension ref="A1:AMJ1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E66" activeCellId="0" sqref="E66"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E5" activeCellId="0" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -968,77 +884,81 @@
         <v>5</v>
       </c>
       <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
+      <c r="D2" s="1" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
+      <c r="D3" s="1" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>15</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>4</v>
@@ -1046,7 +966,7 @@
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>4</v>
@@ -1054,10 +974,10 @@
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C13" s="1" t="n">
         <v>1</v>
@@ -1065,34 +985,34 @@
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C17" s="1" t="n">
         <v>1</v>
@@ -1101,19 +1021,19 @@
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="O18" s="2"/>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C19" s="0"/>
       <c r="D19" s="0"/>
@@ -1121,53 +1041,53 @@
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="O20" s="2"/>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C21" s="1" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="O21" s="2"/>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="O22" s="2"/>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="O23" s="2"/>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C24" s="1" t="n">
         <f aca="false">TRUE()</f>
@@ -1177,10 +1097,10 @@
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B25" s="1" t="s">
         <v>31</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>30</v>
       </c>
       <c r="C25" s="1" t="n">
         <f aca="false">TRUE()</f>
@@ -1190,55 +1110,55 @@
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="O26" s="2"/>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B27" s="1" t="s">
         <v>34</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>33</v>
       </c>
       <c r="O27" s="2"/>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="O28" s="2"/>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B29" s="1" t="s">
         <v>36</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>35</v>
       </c>
       <c r="O29" s="2"/>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="O30" s="2"/>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C31" s="1" t="n">
         <v>1</v>
@@ -1247,10 +1167,10 @@
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C32" s="1" t="n">
         <v>1</v>
@@ -1259,177 +1179,177 @@
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C33" s="1" t="n">
         <v>1</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="O33" s="2"/>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C34" s="1" t="n">
         <v>1</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="O34" s="2"/>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="O35" s="2"/>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="O36" s="2"/>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C50" s="1" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C51" s="1" t="n">
         <v>1</v>
@@ -1437,18 +1357,18 @@
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B53" s="1" t="s">
         <v>59</v>
-      </c>
-      <c r="B53" s="1" t="s">
-        <v>58</v>
       </c>
       <c r="C53" s="1" t="n">
         <v>1</v>
@@ -2476,10 +2396,10 @@
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C54" s="1" t="n">
         <v>1</v>
@@ -2487,34 +2407,34 @@
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C58" s="1" t="n">
         <f aca="false">TRUE()</f>
@@ -2523,42 +2443,42 @@
     </row>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C63" s="1" t="n">
         <v>1</v>
@@ -2566,10 +2486,10 @@
     </row>
     <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C64" s="1" t="n">
         <v>1</v>
@@ -2577,10 +2497,10 @@
     </row>
     <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C65" s="1" t="n">
         <v>1</v>
@@ -2588,10 +2508,10 @@
     </row>
     <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C66" s="1" t="n">
         <v>1</v>
@@ -2619,7 +2539,6 @@
     <oddHeader/>
     <oddFooter/>
   </headerFooter>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2630,7 +2549,7 @@
   </sheetPr>
   <dimension ref="A1:F242"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A61" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A61" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D150" activeCellId="0" sqref="D150"/>
     </sheetView>
   </sheetViews>
@@ -2644,16 +2563,16 @@
   <sheetData>
     <row r="1" s="4" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>75</v>
+        <v>3</v>
       </c>
       <c r="E1" s="3"/>
       <c r="F1" s="3"/>
@@ -2666,7 +2585,7 @@
         <v>77</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D2" s="5"/>
       <c r="E2" s="5"/>
@@ -2680,7 +2599,7 @@
         <v>78</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D3" s="5"/>
       <c r="E3" s="5"/>
@@ -2694,7 +2613,7 @@
         <v>79</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D4" s="5"/>
       <c r="E4" s="5"/>
@@ -2708,7 +2627,7 @@
         <v>80</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D5" s="5"/>
       <c r="E5" s="5"/>
@@ -2722,7 +2641,7 @@
         <v>81</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D6" s="5"/>
       <c r="E6" s="5"/>
@@ -2736,7 +2655,7 @@
         <v>82</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D7" s="5"/>
       <c r="E7" s="5"/>
@@ -2750,7 +2669,7 @@
         <v>83</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D8" s="5"/>
       <c r="E8" s="5"/>
@@ -2764,7 +2683,7 @@
         <v>84</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D9" s="5"/>
       <c r="E9" s="5"/>
@@ -2778,7 +2697,7 @@
         <v>85</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D10" s="5"/>
       <c r="E10" s="5"/>
@@ -2792,7 +2711,7 @@
         <v>86</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D11" s="5"/>
       <c r="E11" s="5"/>
@@ -2806,7 +2725,7 @@
         <v>87</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D12" s="5"/>
       <c r="E12" s="5"/>
@@ -2820,7 +2739,7 @@
         <v>88</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D13" s="5"/>
       <c r="E13" s="5"/>
@@ -2834,7 +2753,7 @@
         <v>89</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D14" s="5"/>
       <c r="E14" s="5"/>
@@ -2848,7 +2767,7 @@
         <v>90</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D15" s="5"/>
       <c r="E15" s="5"/>
@@ -2862,7 +2781,7 @@
         <v>91</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D16" s="5"/>
       <c r="E16" s="5"/>
@@ -2876,7 +2795,7 @@
         <v>92</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D17" s="5"/>
       <c r="E17" s="5"/>
@@ -2890,7 +2809,7 @@
         <v>93</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D18" s="5"/>
       <c r="E18" s="5"/>
@@ -2904,7 +2823,7 @@
         <v>94</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D19" s="5"/>
       <c r="E19" s="5"/>
@@ -2918,7 +2837,7 @@
         <v>95</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D20" s="5"/>
       <c r="E20" s="5"/>
@@ -2932,7 +2851,7 @@
         <v>96</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D21" s="5"/>
       <c r="E21" s="5"/>
@@ -2946,7 +2865,7 @@
         <v>97</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D22" s="5"/>
       <c r="E22" s="5"/>
@@ -2960,7 +2879,7 @@
         <v>98</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D23" s="5"/>
       <c r="E23" s="5"/>
@@ -2974,7 +2893,7 @@
         <v>77</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D24" s="5"/>
       <c r="E24" s="5"/>
@@ -2988,7 +2907,7 @@
         <v>78</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D25" s="5"/>
       <c r="E25" s="5"/>
@@ -3002,7 +2921,7 @@
         <v>79</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D26" s="5"/>
       <c r="E26" s="5"/>
@@ -3016,7 +2935,7 @@
         <v>80</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D27" s="5"/>
       <c r="E27" s="5"/>
@@ -3030,7 +2949,7 @@
         <v>81</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D28" s="5"/>
       <c r="E28" s="5"/>
@@ -3044,7 +2963,7 @@
         <v>82</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D29" s="5"/>
       <c r="E29" s="5"/>
@@ -3058,7 +2977,7 @@
         <v>83</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D30" s="5"/>
       <c r="E30" s="5"/>
@@ -3072,7 +2991,7 @@
         <v>84</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D31" s="5"/>
       <c r="E31" s="5"/>
@@ -3086,7 +3005,7 @@
         <v>85</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D32" s="5"/>
       <c r="E32" s="5"/>
@@ -3100,7 +3019,7 @@
         <v>86</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D33" s="5"/>
       <c r="E33" s="5"/>
@@ -3114,7 +3033,7 @@
         <v>87</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D34" s="5"/>
       <c r="E34" s="5"/>
@@ -3128,7 +3047,7 @@
         <v>88</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D35" s="5"/>
       <c r="E35" s="5"/>
@@ -3142,7 +3061,7 @@
         <v>89</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D36" s="5"/>
       <c r="E36" s="5"/>
@@ -3156,7 +3075,7 @@
         <v>90</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D37" s="5"/>
       <c r="E37" s="5"/>
@@ -3170,7 +3089,7 @@
         <v>91</v>
       </c>
       <c r="C38" s="5" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D38" s="5"/>
       <c r="E38" s="5"/>
@@ -3184,7 +3103,7 @@
         <v>92</v>
       </c>
       <c r="C39" s="5" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D39" s="5"/>
       <c r="E39" s="5"/>
@@ -3198,7 +3117,7 @@
         <v>93</v>
       </c>
       <c r="C40" s="5" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D40" s="5"/>
       <c r="E40" s="5"/>
@@ -3212,7 +3131,7 @@
         <v>94</v>
       </c>
       <c r="C41" s="5" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D41" s="5"/>
       <c r="E41" s="5"/>
@@ -3226,7 +3145,7 @@
         <v>95</v>
       </c>
       <c r="C42" s="5" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D42" s="5"/>
       <c r="E42" s="5"/>
@@ -3240,7 +3159,7 @@
         <v>96</v>
       </c>
       <c r="C43" s="5" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D43" s="5"/>
       <c r="E43" s="5"/>
@@ -3254,7 +3173,7 @@
         <v>97</v>
       </c>
       <c r="C44" s="5" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D44" s="5"/>
       <c r="E44" s="5"/>
@@ -3268,7 +3187,7 @@
         <v>98</v>
       </c>
       <c r="C45" s="5" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D45" s="5"/>
       <c r="E45" s="5"/>
@@ -3282,7 +3201,7 @@
         <v>101</v>
       </c>
       <c r="C46" s="5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D46" s="5"/>
       <c r="E46" s="5"/>
@@ -3296,7 +3215,7 @@
         <v>102</v>
       </c>
       <c r="C47" s="5" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D47" s="5"/>
       <c r="E47" s="5"/>
@@ -3310,7 +3229,7 @@
         <v>103</v>
       </c>
       <c r="C48" s="5" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D48" s="5"/>
       <c r="E48" s="5"/>
@@ -3321,10 +3240,10 @@
         <v>100</v>
       </c>
       <c r="B49" s="5" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C49" s="5" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D49" s="5"/>
       <c r="E49" s="5"/>
@@ -3335,10 +3254,10 @@
         <v>100</v>
       </c>
       <c r="B50" s="5" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C50" s="5" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D50" s="5"/>
       <c r="E50" s="5"/>
@@ -3352,7 +3271,7 @@
         <v>104</v>
       </c>
       <c r="C51" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D51" s="5"/>
       <c r="E51" s="5"/>
@@ -3366,7 +3285,7 @@
         <v>106</v>
       </c>
       <c r="C52" s="5" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D52" s="5"/>
       <c r="E52" s="5"/>
@@ -3422,7 +3341,7 @@
         <v>111</v>
       </c>
       <c r="C56" s="5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D56" s="5"/>
       <c r="E56" s="5"/>
@@ -3436,7 +3355,7 @@
         <v>112</v>
       </c>
       <c r="C57" s="5" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D57" s="5"/>
       <c r="E57" s="5"/>
@@ -3450,7 +3369,7 @@
         <v>113</v>
       </c>
       <c r="C58" s="5" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D58" s="5"/>
       <c r="E58" s="5"/>
@@ -3464,7 +3383,7 @@
         <v>114</v>
       </c>
       <c r="C59" s="5" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D59" s="5"/>
       <c r="E59" s="5"/>
@@ -3478,7 +3397,7 @@
         <v>115</v>
       </c>
       <c r="C60" s="5" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D60" s="5"/>
       <c r="E60" s="5"/>
@@ -3492,7 +3411,7 @@
         <v>116</v>
       </c>
       <c r="C61" s="5" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D61" s="5"/>
       <c r="E61" s="5"/>
@@ -3506,7 +3425,7 @@
         <v>117</v>
       </c>
       <c r="C62" s="5" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D62" s="5"/>
       <c r="E62" s="5"/>
@@ -3520,7 +3439,7 @@
         <v>118</v>
       </c>
       <c r="C63" s="5" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D63" s="5"/>
       <c r="E63" s="5"/>
@@ -3534,7 +3453,7 @@
         <v>119</v>
       </c>
       <c r="C64" s="5" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D64" s="5"/>
       <c r="E64" s="5"/>
@@ -3548,7 +3467,7 @@
         <v>120</v>
       </c>
       <c r="C65" s="5" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D65" s="5"/>
       <c r="E65" s="5"/>
@@ -3590,7 +3509,7 @@
         <v>124</v>
       </c>
       <c r="C68" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D68" s="5"/>
       <c r="E68" s="5"/>
@@ -3604,7 +3523,7 @@
         <v>125</v>
       </c>
       <c r="C69" s="5" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D69" s="5"/>
       <c r="E69" s="5"/>
@@ -3618,7 +3537,7 @@
         <v>126</v>
       </c>
       <c r="C70" s="5" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D70" s="5"/>
       <c r="E70" s="5"/>
@@ -3632,7 +3551,7 @@
         <v>104</v>
       </c>
       <c r="C71" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D71" s="5"/>
       <c r="E71" s="5"/>
@@ -3646,7 +3565,7 @@
         <v>127</v>
       </c>
       <c r="C72" s="5" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D72" s="5"/>
       <c r="E72" s="5"/>
@@ -3660,7 +3579,7 @@
         <v>97</v>
       </c>
       <c r="C73" s="5" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D73" s="5"/>
       <c r="E73" s="5"/>
@@ -3702,7 +3621,7 @@
         <v>130</v>
       </c>
       <c r="C76" s="5" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D76" s="5"/>
       <c r="E76" s="5"/>
@@ -3716,7 +3635,7 @@
         <v>131</v>
       </c>
       <c r="C77" s="5" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D77" s="5"/>
       <c r="E77" s="5"/>
@@ -3744,7 +3663,7 @@
         <v>133</v>
       </c>
       <c r="C79" s="5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D79" s="5"/>
       <c r="E79" s="5"/>
@@ -3800,7 +3719,7 @@
         <v>138</v>
       </c>
       <c r="C83" s="5" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D83" s="5"/>
       <c r="E83" s="5"/>
@@ -3814,7 +3733,7 @@
         <v>91</v>
       </c>
       <c r="C84" s="5" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D84" s="5"/>
       <c r="E84" s="5"/>
@@ -3828,7 +3747,7 @@
         <v>92</v>
       </c>
       <c r="C85" s="5" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D85" s="5"/>
       <c r="E85" s="5"/>
@@ -3842,7 +3761,7 @@
         <v>139</v>
       </c>
       <c r="C86" s="5" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D86" s="5"/>
       <c r="E86" s="5"/>
@@ -3884,7 +3803,7 @@
         <v>142</v>
       </c>
       <c r="C89" s="5" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D89" s="5"/>
       <c r="E89" s="5"/>
@@ -3926,7 +3845,7 @@
         <v>89</v>
       </c>
       <c r="C92" s="5" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D92" s="5"/>
       <c r="E92" s="5"/>
@@ -3996,7 +3915,7 @@
         <v>149</v>
       </c>
       <c r="C97" s="5" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D97" s="5"/>
       <c r="E97" s="5"/>
@@ -4024,7 +3943,7 @@
         <v>98</v>
       </c>
       <c r="C99" s="5" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D99" s="5"/>
       <c r="E99" s="5"/>
@@ -4038,7 +3957,7 @@
         <v>151</v>
       </c>
       <c r="C100" s="5" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D100" s="5"/>
       <c r="E100" s="5"/>
@@ -4052,7 +3971,7 @@
         <v>152</v>
       </c>
       <c r="C101" s="5" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D101" s="5"/>
       <c r="E101" s="5"/>
@@ -4080,7 +3999,7 @@
         <v>154</v>
       </c>
       <c r="C103" s="5" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D103" s="5"/>
       <c r="E103" s="5"/>
@@ -4108,7 +4027,7 @@
         <v>79</v>
       </c>
       <c r="C105" s="5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D105" s="5"/>
       <c r="E105" s="5"/>
@@ -4206,7 +4125,7 @@
         <v>163</v>
       </c>
       <c r="C112" s="5" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D112" s="5"/>
       <c r="E112" s="5"/>
@@ -4220,7 +4139,7 @@
         <v>164</v>
       </c>
       <c r="C113" s="5" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D113" s="5"/>
       <c r="E113" s="5"/>
@@ -4234,7 +4153,7 @@
         <v>165</v>
       </c>
       <c r="C114" s="5" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D114" s="5"/>
       <c r="E114" s="5"/>
@@ -4248,7 +4167,7 @@
         <v>166</v>
       </c>
       <c r="C115" s="5" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D115" s="5"/>
       <c r="E115" s="5"/>
@@ -4262,7 +4181,7 @@
         <v>167</v>
       </c>
       <c r="C116" s="5" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D116" s="5"/>
       <c r="E116" s="5"/>
@@ -4276,7 +4195,7 @@
         <v>168</v>
       </c>
       <c r="C117" s="5" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D117" s="5"/>
       <c r="E117" s="5"/>
@@ -4290,7 +4209,7 @@
         <v>169</v>
       </c>
       <c r="C118" s="5" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D118" s="5"/>
       <c r="E118" s="5"/>
@@ -4304,7 +4223,7 @@
         <v>171</v>
       </c>
       <c r="C119" s="5" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D119" s="5"/>
       <c r="E119" s="5"/>
@@ -4318,7 +4237,7 @@
         <v>172</v>
       </c>
       <c r="C120" s="5" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D120" s="5"/>
       <c r="E120" s="5"/>
@@ -4332,7 +4251,7 @@
         <v>173</v>
       </c>
       <c r="C121" s="5" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D121" s="5"/>
       <c r="E121" s="5"/>
@@ -4346,7 +4265,7 @@
         <v>151</v>
       </c>
       <c r="C122" s="5" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D122" s="5"/>
       <c r="E122" s="5"/>
@@ -4360,7 +4279,7 @@
         <v>174</v>
       </c>
       <c r="C123" s="5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D123" s="5"/>
       <c r="E123" s="5"/>
@@ -4371,10 +4290,10 @@
         <v>170</v>
       </c>
       <c r="B124" s="5" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C124" s="5" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D124" s="5" t="s">
         <v>175</v>
@@ -4387,10 +4306,10 @@
         <v>170</v>
       </c>
       <c r="B125" s="5" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C125" s="5" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D125" s="5" t="s">
         <v>175</v>
@@ -4406,7 +4325,7 @@
         <v>176</v>
       </c>
       <c r="C126" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D126" s="5"/>
       <c r="E126" s="5"/>
@@ -4420,7 +4339,7 @@
         <v>98</v>
       </c>
       <c r="C127" s="5" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D127" s="5"/>
       <c r="E127" s="5"/>
@@ -4434,7 +4353,7 @@
         <v>127</v>
       </c>
       <c r="C128" s="5" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D128" s="5"/>
       <c r="E128" s="5"/>
@@ -4448,7 +4367,7 @@
         <v>130</v>
       </c>
       <c r="C129" s="5" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D129" s="5"/>
       <c r="E129" s="5"/>
@@ -4462,7 +4381,7 @@
         <v>178</v>
       </c>
       <c r="C130" s="5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D130" s="5"/>
       <c r="E130" s="5"/>
@@ -4476,7 +4395,7 @@
         <v>179</v>
       </c>
       <c r="C131" s="5" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D131" s="5"/>
       <c r="E131" s="5"/>
@@ -4490,7 +4409,7 @@
         <v>180</v>
       </c>
       <c r="C132" s="5" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D132" s="5"/>
       <c r="E132" s="5"/>
@@ -4504,7 +4423,7 @@
         <v>89</v>
       </c>
       <c r="C133" s="5" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D133" s="5"/>
       <c r="E133" s="5"/>
@@ -4518,7 +4437,7 @@
         <v>98</v>
       </c>
       <c r="C134" s="5" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D134" s="5"/>
       <c r="E134" s="5"/>
@@ -4532,7 +4451,7 @@
         <v>181</v>
       </c>
       <c r="C135" s="5" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D135" s="5"/>
       <c r="E135" s="5"/>
@@ -4546,7 +4465,7 @@
         <v>182</v>
       </c>
       <c r="C136" s="5" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D136" s="5"/>
       <c r="E136" s="5"/>
@@ -4560,7 +4479,7 @@
         <v>183</v>
       </c>
       <c r="C137" s="5" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D137" s="5"/>
       <c r="E137" s="5"/>
@@ -4574,7 +4493,7 @@
         <v>166</v>
       </c>
       <c r="C138" s="5" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D138" s="5"/>
       <c r="E138" s="5"/>
@@ -4588,7 +4507,7 @@
         <v>184</v>
       </c>
       <c r="C139" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D139" s="5"/>
       <c r="E139" s="5"/>
@@ -4602,7 +4521,7 @@
         <v>186</v>
       </c>
       <c r="C140" s="5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D140" s="5"/>
       <c r="E140" s="5"/>
@@ -4616,7 +4535,7 @@
         <v>187</v>
       </c>
       <c r="C141" s="5" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D141" s="5"/>
       <c r="E141" s="5"/>
@@ -4630,7 +4549,7 @@
         <v>188</v>
       </c>
       <c r="C142" s="5" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D142" s="5"/>
       <c r="E142" s="5"/>
@@ -4644,7 +4563,7 @@
         <v>189</v>
       </c>
       <c r="C143" s="5" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D143" s="5"/>
       <c r="E143" s="5"/>
@@ -4658,7 +4577,7 @@
         <v>190</v>
       </c>
       <c r="C144" s="5" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D144" s="5"/>
       <c r="E144" s="5"/>
@@ -4672,7 +4591,7 @@
         <v>138</v>
       </c>
       <c r="C145" s="5" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D145" s="5"/>
       <c r="E145" s="5"/>
@@ -4686,7 +4605,7 @@
         <v>89</v>
       </c>
       <c r="C146" s="5" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D146" s="5"/>
       <c r="E146" s="5"/>
@@ -4700,7 +4619,7 @@
         <v>191</v>
       </c>
       <c r="C147" s="5" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D147" s="5"/>
       <c r="E147" s="5"/>
@@ -4714,7 +4633,7 @@
         <v>98</v>
       </c>
       <c r="C148" s="5" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D148" s="5"/>
       <c r="E148" s="5"/>
@@ -4742,7 +4661,7 @@
         <v>195</v>
       </c>
       <c r="C150" s="5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D150" s="5"/>
       <c r="E150" s="5"/>
@@ -4756,7 +4675,7 @@
         <v>196</v>
       </c>
       <c r="C151" s="5" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D151" s="5"/>
       <c r="E151" s="5"/>
@@ -4770,7 +4689,7 @@
         <v>197</v>
       </c>
       <c r="C152" s="5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D152" s="5"/>
       <c r="E152" s="5"/>
@@ -4784,7 +4703,7 @@
         <v>198</v>
       </c>
       <c r="C153" s="5" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D153" s="5"/>
       <c r="E153" s="5"/>
@@ -4798,7 +4717,7 @@
         <v>199</v>
       </c>
       <c r="C154" s="5" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D154" s="5"/>
       <c r="E154" s="5"/>
@@ -4824,7 +4743,7 @@
         <v>201</v>
       </c>
       <c r="C156" s="5" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D156" s="5"/>
       <c r="E156" s="5"/>
@@ -4838,7 +4757,7 @@
         <v>202</v>
       </c>
       <c r="C157" s="5" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D157" s="5"/>
       <c r="E157" s="5"/>
@@ -4852,7 +4771,7 @@
         <v>203</v>
       </c>
       <c r="C158" s="5" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D158" s="5"/>
       <c r="E158" s="5"/>
@@ -4866,7 +4785,7 @@
         <v>127</v>
       </c>
       <c r="C159" s="5" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D159" s="5"/>
       <c r="E159" s="5"/>
@@ -4880,7 +4799,7 @@
         <v>204</v>
       </c>
       <c r="C160" s="5" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D160" s="5"/>
       <c r="E160" s="5"/>
@@ -4894,7 +4813,7 @@
         <v>205</v>
       </c>
       <c r="C161" s="5" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D161" s="5"/>
       <c r="E161" s="5"/>
@@ -4908,7 +4827,7 @@
         <v>207</v>
       </c>
       <c r="C162" s="5" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D162" s="5"/>
       <c r="E162" s="5"/>
@@ -4922,7 +4841,7 @@
         <v>208</v>
       </c>
       <c r="C163" s="5" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D163" s="5"/>
       <c r="E163" s="5"/>
@@ -4936,7 +4855,7 @@
         <v>104</v>
       </c>
       <c r="C164" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D164" s="5"/>
       <c r="E164" s="5"/>
@@ -4950,7 +4869,7 @@
         <v>209</v>
       </c>
       <c r="C165" s="5" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D165" s="5"/>
       <c r="E165" s="5"/>
@@ -4964,7 +4883,7 @@
         <v>186</v>
       </c>
       <c r="C166" s="5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D166" s="5"/>
       <c r="E166" s="5"/>
@@ -4978,7 +4897,7 @@
         <v>195</v>
       </c>
       <c r="C167" s="5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D167" s="5"/>
       <c r="E167" s="5"/>
@@ -4992,7 +4911,7 @@
         <v>211</v>
       </c>
       <c r="C168" s="5" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D168" s="5"/>
       <c r="E168" s="5"/>
@@ -5006,7 +4925,7 @@
         <v>172</v>
       </c>
       <c r="C169" s="5" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D169" s="5"/>
       <c r="E169" s="5"/>
@@ -5020,7 +4939,7 @@
         <v>151</v>
       </c>
       <c r="C170" s="5" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D170" s="5"/>
       <c r="E170" s="5"/>
@@ -5034,7 +4953,7 @@
         <v>212</v>
       </c>
       <c r="C171" s="5" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D171" s="5"/>
       <c r="E171" s="5"/>
@@ -5048,7 +4967,7 @@
         <v>195</v>
       </c>
       <c r="C172" s="5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D172" s="5"/>
       <c r="E172" s="5"/>
@@ -5062,7 +4981,7 @@
         <v>203</v>
       </c>
       <c r="C173" s="5" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D173" s="5"/>
       <c r="E173" s="5"/>
@@ -5076,7 +4995,7 @@
         <v>91</v>
       </c>
       <c r="C174" s="5" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D174" s="5"/>
       <c r="E174" s="5"/>
@@ -5090,7 +5009,7 @@
         <v>92</v>
       </c>
       <c r="C175" s="5" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D175" s="5"/>
       <c r="E175" s="5"/>
@@ -5104,7 +5023,7 @@
         <v>89</v>
       </c>
       <c r="C176" s="5" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D176" s="5"/>
       <c r="E176" s="5"/>
@@ -5118,7 +5037,7 @@
         <v>98</v>
       </c>
       <c r="C177" s="5" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D177" s="5"/>
       <c r="E177" s="5"/>
@@ -5132,7 +5051,7 @@
         <v>151</v>
       </c>
       <c r="C178" s="5" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D178" s="5"/>
       <c r="E178" s="5"/>
@@ -5146,7 +5065,7 @@
         <v>214</v>
       </c>
       <c r="C179" s="5" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D179" s="5"/>
       <c r="E179" s="5"/>
@@ -5160,7 +5079,7 @@
         <v>80</v>
       </c>
       <c r="C180" s="5" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D180" s="5"/>
       <c r="E180" s="5"/>
@@ -5174,7 +5093,7 @@
         <v>166</v>
       </c>
       <c r="C181" s="5" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D181" s="5"/>
       <c r="E181" s="5"/>
@@ -5188,7 +5107,7 @@
         <v>179</v>
       </c>
       <c r="C182" s="5" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D182" s="5" t="s">
         <v>216</v>
@@ -5204,7 +5123,7 @@
         <v>217</v>
       </c>
       <c r="C183" s="5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D183" s="5" t="s">
         <v>216</v>
@@ -5220,7 +5139,7 @@
         <v>219</v>
       </c>
       <c r="C184" s="5" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D184" s="5"/>
       <c r="E184" s="5"/>
@@ -5234,7 +5153,7 @@
         <v>220</v>
       </c>
       <c r="C185" s="5" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D185" s="5"/>
       <c r="E185" s="5"/>
@@ -5245,10 +5164,10 @@
         <v>218</v>
       </c>
       <c r="B186" s="5" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C186" s="5" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D186" s="5"/>
       <c r="E186" s="5"/>
@@ -5259,10 +5178,10 @@
         <v>218</v>
       </c>
       <c r="B187" s="5" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C187" s="5" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D187" s="5"/>
       <c r="E187" s="5"/>
@@ -5273,10 +5192,10 @@
         <v>218</v>
       </c>
       <c r="B188" s="5" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C188" s="5" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D188" s="5"/>
       <c r="E188" s="5"/>
@@ -5717,7 +5636,7 @@
   </sheetData>
   <dataValidations count="1">
     <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="C1:C1188" type="list">
-      <formula1>controlled_vocabulary!$A$2:$A$9999</formula1>
+      <formula1>controlled_vocabulary!$A$4:$A$9999</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
@@ -5728,7 +5647,6 @@
     <oddHeader/>
     <oddFooter/>
   </headerFooter>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
add 'other cells' for EPIC and quanTIseq.
</commit_message>
<xml_diff>
--- a/inst/extdata/cell_type_mapping.xlsx
+++ b/inst/extdata/cell_type_mapping.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="controlled_vocabulary" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="710" uniqueCount="223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="716" uniqueCount="225">
   <si>
     <t xml:space="preserve">cell_type</t>
   </si>
@@ -246,6 +246,9 @@
     <t xml:space="preserve">T cell CD8+ effector memory</t>
   </si>
   <si>
+    <t xml:space="preserve">uncharacterized cell</t>
+  </si>
+  <si>
     <t xml:space="preserve">method_dataset</t>
   </si>
   <si>
@@ -577,6 +580,9 @@
   </si>
   <si>
     <t xml:space="preserve">Dendritic.cells</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Other</t>
   </si>
   <si>
     <t xml:space="preserve">epic</t>
@@ -848,23 +854,23 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>2590200</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>-25200</xdr:rowOff>
+      <xdr:rowOff>149760</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>90000</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>25200</xdr:rowOff>
+      <xdr:colOff>89280</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>24480</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
-        <xdr:cNvPr id="0" name="Ellipse 1"/>
+        <xdr:cNvPr id="0" name="CustomShape 1"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2590200" y="-25200"/>
-          <a:ext cx="2416320" cy="225360"/>
+          <a:off x="2590200" y="149760"/>
+          <a:ext cx="2415600" cy="225000"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
           <a:avLst/>
@@ -877,6 +883,12 @@
           <a:round/>
         </a:ln>
       </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
+        <a:fontRef idx="minor"/>
+      </xdr:style>
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
@@ -884,24 +896,24 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>2590200</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>149760</xdr:rowOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>150120</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>90000</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>25200</xdr:rowOff>
+      <xdr:colOff>89280</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>24480</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
-        <xdr:cNvPr id="1" name="Ellipse 1"/>
+        <xdr:cNvPr id="1" name="CustomShape 1"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2590200" y="149760"/>
-          <a:ext cx="2416320" cy="225720"/>
+          <a:off x="2590200" y="325080"/>
+          <a:ext cx="2415600" cy="225000"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
           <a:avLst/>
@@ -914,43 +926,12 @@
           <a:round/>
         </a:ln>
       </xdr:spPr>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>2590200</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>150120</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>90000</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>25200</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp>
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="Ellipse 1"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="2590200" y="325080"/>
-          <a:ext cx="2416320" cy="225720"/>
-        </a:xfrm>
-        <a:prstGeom prst="ellipse">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln w="19800">
-          <a:solidFill>
-            <a:srgbClr val="ff0000"/>
-          </a:solidFill>
-          <a:round/>
-        </a:ln>
-      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
+        <a:fontRef idx="minor"/>
+      </xdr:style>
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
@@ -962,10 +943,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AMJ66"/>
+  <dimension ref="A1:AMJ67"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A40" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A67" activeCellId="0" sqref="A67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2633,6 +2614,14 @@
         <v>1</v>
       </c>
     </row>
+    <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A67" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
   </sheetData>
   <dataValidations count="1">
     <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="B1:B1066" type="list">
@@ -2656,10 +2645,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F242"/>
+  <dimension ref="A1:F243"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A61" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D150" activeCellId="0" sqref="D150"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A139" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B140" activeCellId="0" sqref="B140"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2672,10 +2661,10 @@
   <sheetData>
     <row r="1" s="4" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>0</v>
@@ -2688,10 +2677,10 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>10</v>
@@ -2702,10 +2691,10 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>8</v>
@@ -2716,10 +2705,10 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>11</v>
@@ -2730,10 +2719,10 @@
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="5" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>55</v>
@@ -2744,10 +2733,10 @@
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="5" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>64</v>
@@ -2758,10 +2747,10 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="5" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>67</v>
@@ -2772,10 +2761,10 @@
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="5" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C8" s="5" t="s">
         <v>66</v>
@@ -2786,10 +2775,10 @@
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="5" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C9" s="5" t="s">
         <v>65</v>
@@ -2800,10 +2789,10 @@
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="5" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C10" s="5" t="s">
         <v>62</v>
@@ -2814,10 +2803,10 @@
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="5" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C11" s="5" t="s">
         <v>56</v>
@@ -2828,10 +2817,10 @@
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="5" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C12" s="5" t="s">
         <v>47</v>
@@ -2842,10 +2831,10 @@
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="5" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C13" s="5" t="s">
         <v>46</v>
@@ -2856,10 +2845,10 @@
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="5" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C14" s="5" t="s">
         <v>32</v>
@@ -2870,10 +2859,10 @@
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="5" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C15" s="5" t="s">
         <v>26</v>
@@ -2884,10 +2873,10 @@
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="5" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C16" s="5" t="s">
         <v>29</v>
@@ -2898,10 +2887,10 @@
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="5" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C17" s="5" t="s">
         <v>30</v>
@@ -2912,10 +2901,10 @@
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="5" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C18" s="5" t="s">
         <v>43</v>
@@ -2926,10 +2915,10 @@
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="5" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C19" s="5" t="s">
         <v>41</v>
@@ -2940,10 +2929,10 @@
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="5" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C20" s="5" t="s">
         <v>33</v>
@@ -2954,10 +2943,10 @@
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="5" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C21" s="5" t="s">
         <v>35</v>
@@ -2968,10 +2957,10 @@
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="5" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C22" s="5" t="s">
         <v>44</v>
@@ -2982,10 +2971,10 @@
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="5" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C23" s="5" t="s">
         <v>45</v>
@@ -2996,10 +2985,10 @@
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="5" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C24" s="5" t="s">
         <v>10</v>
@@ -3010,10 +2999,10 @@
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="5" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C25" s="5" t="s">
         <v>8</v>
@@ -3024,10 +3013,10 @@
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="5" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C26" s="5" t="s">
         <v>11</v>
@@ -3038,10 +3027,10 @@
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="5" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C27" s="5" t="s">
         <v>55</v>
@@ -3052,10 +3041,10 @@
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="5" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C28" s="5" t="s">
         <v>64</v>
@@ -3066,10 +3055,10 @@
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="5" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C29" s="5" t="s">
         <v>67</v>
@@ -3080,10 +3069,10 @@
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="5" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C30" s="5" t="s">
         <v>66</v>
@@ -3094,10 +3083,10 @@
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="5" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C31" s="5" t="s">
         <v>65</v>
@@ -3108,10 +3097,10 @@
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="5" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C32" s="5" t="s">
         <v>62</v>
@@ -3122,10 +3111,10 @@
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="5" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C33" s="5" t="s">
         <v>56</v>
@@ -3136,10 +3125,10 @@
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="5" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C34" s="5" t="s">
         <v>47</v>
@@ -3150,10 +3139,10 @@
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="5" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C35" s="5" t="s">
         <v>46</v>
@@ -3164,10 +3153,10 @@
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="5" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C36" s="5" t="s">
         <v>32</v>
@@ -3178,10 +3167,10 @@
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="5" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C37" s="5" t="s">
         <v>26</v>
@@ -3192,10 +3181,10 @@
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="5" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C38" s="5" t="s">
         <v>29</v>
@@ -3206,10 +3195,10 @@
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="5" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C39" s="5" t="s">
         <v>30</v>
@@ -3220,10 +3209,10 @@
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="5" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C40" s="5" t="s">
         <v>43</v>
@@ -3234,10 +3223,10 @@
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="5" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C41" s="5" t="s">
         <v>41</v>
@@ -3248,10 +3237,10 @@
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="5" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B42" s="5" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C42" s="5" t="s">
         <v>33</v>
@@ -3262,10 +3251,10 @@
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="5" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B43" s="5" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C43" s="5" t="s">
         <v>35</v>
@@ -3276,10 +3265,10 @@
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="5" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B44" s="5" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C44" s="5" t="s">
         <v>44</v>
@@ -3290,10 +3279,10 @@
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="B45" s="5" t="s">
         <v>99</v>
-      </c>
-      <c r="B45" s="5" t="s">
-        <v>98</v>
       </c>
       <c r="C45" s="5" t="s">
         <v>45</v>
@@ -3304,10 +3293,10 @@
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="5" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B46" s="5" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C46" s="5" t="s">
         <v>9</v>
@@ -3318,10 +3307,10 @@
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="5" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B47" s="5" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C47" s="5" t="s">
         <v>54</v>
@@ -3332,10 +3321,10 @@
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="5" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B48" s="5" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C48" s="5" t="s">
         <v>55</v>
@@ -3346,7 +3335,7 @@
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="5" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B49" s="5" t="s">
         <v>45</v>
@@ -3360,7 +3349,7 @@
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="5" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B50" s="5" t="s">
         <v>27</v>
@@ -3374,10 +3363,10 @@
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="5" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B51" s="5" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C51" s="5" t="s">
         <v>37</v>
@@ -3388,10 +3377,10 @@
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="5" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B52" s="5" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C52" s="5" t="s">
         <v>41</v>
@@ -3402,52 +3391,52 @@
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="5" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B53" s="5" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C53" s="5"/>
       <c r="D53" s="5" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="E53" s="5"/>
       <c r="F53" s="5"/>
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="5" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B54" s="5" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C54" s="5"/>
       <c r="D54" s="5" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="E54" s="5"/>
       <c r="F54" s="5"/>
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="5" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B55" s="5" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C55" s="5"/>
       <c r="D55" s="5" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="E55" s="5"/>
       <c r="F55" s="5"/>
     </row>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="5" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B56" s="5" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C56" s="5" t="s">
         <v>9</v>
@@ -3458,10 +3447,10 @@
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="5" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B57" s="5" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C57" s="5" t="s">
         <v>63</v>
@@ -3472,10 +3461,10 @@
     </row>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="5" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B58" s="5" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C58" s="5" t="s">
         <v>64</v>
@@ -3486,10 +3475,10 @@
     </row>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="5" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B59" s="5" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C59" s="5" t="s">
         <v>59</v>
@@ -3500,10 +3489,10 @@
     </row>
     <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="5" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B60" s="5" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C60" s="5" t="s">
         <v>70</v>
@@ -3514,10 +3503,10 @@
     </row>
     <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="5" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B61" s="5" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C61" s="5" t="s">
         <v>71</v>
@@ -3528,10 +3517,10 @@
     </row>
     <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="5" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B62" s="5" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C62" s="5" t="s">
         <v>69</v>
@@ -3542,10 +3531,10 @@
     </row>
     <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="5" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B63" s="5" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C63" s="5" t="s">
         <v>55</v>
@@ -3556,10 +3545,10 @@
     </row>
     <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="5" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B64" s="5" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="C64" s="5" t="s">
         <v>72</v>
@@ -3570,10 +3559,10 @@
     </row>
     <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="5" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B65" s="5" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C65" s="5" t="s">
         <v>73</v>
@@ -3584,38 +3573,38 @@
     </row>
     <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="5" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B66" s="5" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C66" s="5"/>
       <c r="D66" s="5" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="E66" s="5"/>
       <c r="F66" s="5"/>
     </row>
     <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="5" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B67" s="5" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C67" s="5"/>
       <c r="D67" s="5" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="E67" s="5"/>
       <c r="F67" s="5"/>
     </row>
     <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="5" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B68" s="5" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C68" s="5" t="s">
         <v>12</v>
@@ -3626,10 +3615,10 @@
     </row>
     <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="5" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B69" s="5" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="C69" s="5" t="s">
         <v>22</v>
@@ -3640,10 +3629,10 @@
     </row>
     <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="5" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B70" s="5" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="C70" s="5" t="s">
         <v>39</v>
@@ -3654,10 +3643,10 @@
     </row>
     <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="B71" s="5" t="s">
         <v>105</v>
-      </c>
-      <c r="B71" s="5" t="s">
-        <v>104</v>
       </c>
       <c r="C71" s="5" t="s">
         <v>37</v>
@@ -3668,10 +3657,10 @@
     </row>
     <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="5" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B72" s="5" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="C72" s="5" t="s">
         <v>49</v>
@@ -3682,10 +3671,10 @@
     </row>
     <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="5" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B73" s="5" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C73" s="5" t="s">
         <v>44</v>
@@ -3696,38 +3685,38 @@
     </row>
     <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="5" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B74" s="5" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="C74" s="5"/>
       <c r="D74" s="5" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="E74" s="5"/>
       <c r="F74" s="5"/>
     </row>
     <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="5" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B75" s="5" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="C75" s="5"/>
       <c r="D75" s="5" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="E75" s="5"/>
       <c r="F75" s="5"/>
     </row>
     <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="5" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B76" s="5" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C76" s="5" t="s">
         <v>48</v>
@@ -3738,10 +3727,10 @@
     </row>
     <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="5" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B77" s="5" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C77" s="5" t="s">
         <v>40</v>
@@ -3752,24 +3741,24 @@
     </row>
     <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="5" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B78" s="5" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C78" s="5"/>
       <c r="D78" s="5" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="E78" s="5"/>
       <c r="F78" s="5"/>
     </row>
     <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="5" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B79" s="5" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="C79" s="5" t="s">
         <v>19</v>
@@ -3780,52 +3769,52 @@
     </row>
     <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="5" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B80" s="5" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="C80" s="5"/>
       <c r="D80" s="5" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="E80" s="5"/>
       <c r="F80" s="5"/>
     </row>
     <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="5" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B81" s="5" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="C81" s="5"/>
       <c r="D81" s="5" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="E81" s="5"/>
       <c r="F81" s="5"/>
     </row>
     <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="5" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B82" s="5" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C82" s="5"/>
       <c r="D82" s="5" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="E82" s="5"/>
       <c r="F82" s="5"/>
     </row>
     <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="5" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B83" s="5" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="C83" s="5" t="s">
         <v>27</v>
@@ -3836,10 +3825,10 @@
     </row>
     <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="5" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B84" s="5" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C84" s="5" t="s">
         <v>29</v>
@@ -3850,10 +3839,10 @@
     </row>
     <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="5" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B85" s="5" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C85" s="5" t="s">
         <v>30</v>
@@ -3864,10 +3853,10 @@
     </row>
     <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="5" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B86" s="5" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="C86" s="5" t="s">
         <v>34</v>
@@ -3878,38 +3867,38 @@
     </row>
     <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="5" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B87" s="5" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="C87" s="5"/>
       <c r="D87" s="5" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="E87" s="5"/>
       <c r="F87" s="5"/>
     </row>
     <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="5" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B88" s="5" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="C88" s="5"/>
       <c r="D88" s="5" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="E88" s="5"/>
       <c r="F88" s="5"/>
     </row>
     <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="5" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B89" s="5" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="C89" s="5" t="s">
         <v>8</v>
@@ -3920,38 +3909,38 @@
     </row>
     <row r="90" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="5" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B90" s="5" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C90" s="5"/>
       <c r="D90" s="5" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="E90" s="5"/>
       <c r="F90" s="5"/>
     </row>
     <row r="91" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="5" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B91" s="5" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C91" s="5"/>
       <c r="D91" s="5" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="E91" s="5"/>
       <c r="F91" s="5"/>
     </row>
     <row r="92" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="5" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B92" s="5" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C92" s="5" t="s">
         <v>32</v>
@@ -3962,66 +3951,66 @@
     </row>
     <row r="93" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="5" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B93" s="5" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="C93" s="5"/>
       <c r="D93" s="5" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="E93" s="5"/>
       <c r="F93" s="5"/>
     </row>
     <row r="94" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="5" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B94" s="5" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="C94" s="5"/>
       <c r="D94" s="5" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="E94" s="5"/>
       <c r="F94" s="5"/>
     </row>
     <row r="95" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="5" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B95" s="5" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="C95" s="5"/>
       <c r="D95" s="5" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="E95" s="5"/>
       <c r="F95" s="5"/>
     </row>
     <row r="96" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="5" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B96" s="5" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="C96" s="5"/>
       <c r="D96" s="5" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="E96" s="5"/>
       <c r="F96" s="5"/>
     </row>
     <row r="97" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="5" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B97" s="5" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="C97" s="5" t="s">
         <v>10</v>
@@ -4032,24 +4021,24 @@
     </row>
     <row r="98" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="5" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B98" s="5" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="C98" s="5"/>
       <c r="D98" s="5" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="E98" s="5"/>
       <c r="F98" s="5"/>
     </row>
     <row r="99" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="5" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B99" s="5" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C99" s="5" t="s">
         <v>45</v>
@@ -4060,10 +4049,10 @@
     </row>
     <row r="100" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="5" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B100" s="5" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C100" s="5" t="s">
         <v>23</v>
@@ -4074,10 +4063,10 @@
     </row>
     <row r="101" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="5" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B101" s="5" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="C101" s="5" t="s">
         <v>58</v>
@@ -4088,24 +4077,24 @@
     </row>
     <row r="102" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="5" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B102" s="5" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="C102" s="5"/>
       <c r="D102" s="5" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="E102" s="5"/>
       <c r="F102" s="5"/>
     </row>
     <row r="103" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="5" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B103" s="5" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="C103" s="5" t="s">
         <v>24</v>
@@ -4116,24 +4105,24 @@
     </row>
     <row r="104" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="5" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B104" s="5" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="C104" s="5"/>
       <c r="D104" s="5" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="E104" s="5"/>
       <c r="F104" s="5"/>
     </row>
     <row r="105" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="5" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B105" s="5" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C105" s="5" t="s">
         <v>11</v>
@@ -4144,94 +4133,94 @@
     </row>
     <row r="106" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="5" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B106" s="5" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="C106" s="5"/>
       <c r="D106" s="5" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="E106" s="5"/>
       <c r="F106" s="5"/>
     </row>
     <row r="107" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="5" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B107" s="5" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="C107" s="5"/>
       <c r="D107" s="5" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="E107" s="5"/>
       <c r="F107" s="5"/>
     </row>
     <row r="108" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="5" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B108" s="5" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="C108" s="5"/>
       <c r="D108" s="5" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="E108" s="5"/>
       <c r="F108" s="5"/>
     </row>
     <row r="109" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="5" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B109" s="5" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="C109" s="5"/>
       <c r="D109" s="5" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="E109" s="5"/>
       <c r="F109" s="5"/>
     </row>
     <row r="110" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="5" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B110" s="5" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="C110" s="5"/>
       <c r="D110" s="5" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="E110" s="5"/>
       <c r="F110" s="5"/>
     </row>
     <row r="111" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="5" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B111" s="5" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="C111" s="5"/>
       <c r="D111" s="5" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="E111" s="5"/>
       <c r="F111" s="5"/>
     </row>
     <row r="112" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="5" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B112" s="5" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="C112" s="5" t="s">
         <v>56</v>
@@ -4242,10 +4231,10 @@
     </row>
     <row r="113" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="5" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B113" s="5" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="C113" s="5" t="s">
         <v>60</v>
@@ -4256,10 +4245,10 @@
     </row>
     <row r="114" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="5" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B114" s="5" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="C114" s="5" t="s">
         <v>61</v>
@@ -4270,10 +4259,10 @@
     </row>
     <row r="115" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="5" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B115" s="5" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="C115" s="5" t="s">
         <v>62</v>
@@ -4284,10 +4273,10 @@
     </row>
     <row r="116" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="5" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B116" s="5" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="C116" s="5" t="s">
         <v>51</v>
@@ -4298,10 +4287,10 @@
     </row>
     <row r="117" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="5" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B117" s="5" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="C117" s="5" t="s">
         <v>53</v>
@@ -4312,10 +4301,10 @@
     </row>
     <row r="118" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="5" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B118" s="5" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="C118" s="5" t="s">
         <v>52</v>
@@ -4326,10 +4315,10 @@
     </row>
     <row r="119" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="5" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B119" s="5" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="C119" s="5" t="s">
         <v>25</v>
@@ -4340,10 +4329,10 @@
     </row>
     <row r="120" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="5" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B120" s="5" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="C120" s="5" t="s">
         <v>55</v>
@@ -4354,10 +4343,10 @@
     </row>
     <row r="121" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="5" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B121" s="5" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="C121" s="5" t="s">
         <v>50</v>
@@ -4368,10 +4357,10 @@
     </row>
     <row r="122" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="5" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B122" s="5" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C122" s="5" t="s">
         <v>23</v>
@@ -4382,10 +4371,10 @@
     </row>
     <row r="123" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="5" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B123" s="5" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="C123" s="5" t="s">
         <v>9</v>
@@ -4396,7 +4385,7 @@
     </row>
     <row r="124" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="5" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B124" s="5" t="s">
         <v>36</v>
@@ -4405,14 +4394,14 @@
         <v>32</v>
       </c>
       <c r="D124" s="5" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="E124" s="5"/>
       <c r="F124" s="5"/>
     </row>
     <row r="125" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="5" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B125" s="5" t="s">
         <v>36</v>
@@ -4421,17 +4410,17 @@
         <v>31</v>
       </c>
       <c r="D125" s="5" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="E125" s="5"/>
       <c r="F125" s="5"/>
     </row>
     <row r="126" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="5" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B126" s="5" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="C126" s="5" t="s">
         <v>37</v>
@@ -4442,10 +4431,10 @@
     </row>
     <row r="127" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="5" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B127" s="5" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C127" s="5" t="s">
         <v>45</v>
@@ -4456,10 +4445,10 @@
     </row>
     <row r="128" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="5" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B128" s="5" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="C128" s="5" t="s">
         <v>49</v>
@@ -4470,10 +4459,10 @@
     </row>
     <row r="129" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A129" s="5" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B129" s="5" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C129" s="5" t="s">
         <v>48</v>
@@ -4484,10 +4473,10 @@
     </row>
     <row r="130" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="5" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B130" s="5" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="C130" s="5" t="s">
         <v>9</v>
@@ -4498,10 +4487,10 @@
     </row>
     <row r="131" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="5" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B131" s="5" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="C131" s="5" t="s">
         <v>29</v>
@@ -4512,10 +4501,10 @@
     </row>
     <row r="132" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A132" s="5" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B132" s="5" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="C132" s="5" t="s">
         <v>30</v>
@@ -4526,10 +4515,10 @@
     </row>
     <row r="133" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A133" s="5" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B133" s="5" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C133" s="5" t="s">
         <v>32</v>
@@ -4540,10 +4529,10 @@
     </row>
     <row r="134" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="5" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B134" s="5" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C134" s="5" t="s">
         <v>45</v>
@@ -4554,10 +4543,10 @@
     </row>
     <row r="135" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A135" s="5" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B135" s="5" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C135" s="5" t="s">
         <v>23</v>
@@ -4568,10 +4557,10 @@
     </row>
     <row r="136" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A136" s="5" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B136" s="5" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="C136" s="5" t="s">
         <v>59</v>
@@ -4582,10 +4571,10 @@
     </row>
     <row r="137" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A137" s="5" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B137" s="5" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="C137" s="5" t="s">
         <v>55</v>
@@ -4596,10 +4585,10 @@
     </row>
     <row r="138" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A138" s="5" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B138" s="5" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="C138" s="5" t="s">
         <v>62</v>
@@ -4610,10 +4599,10 @@
     </row>
     <row r="139" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A139" s="5" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B139" s="5" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="C139" s="5" t="s">
         <v>37</v>
@@ -4624,13 +4613,13 @@
     </row>
     <row r="140" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A140" s="5" t="s">
-        <v>185</v>
+        <v>178</v>
       </c>
       <c r="B140" s="5" t="s">
         <v>186</v>
       </c>
       <c r="C140" s="5" t="s">
-        <v>9</v>
+        <v>74</v>
       </c>
       <c r="D140" s="5"/>
       <c r="E140" s="5"/>
@@ -4638,13 +4627,13 @@
     </row>
     <row r="141" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A141" s="5" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="B141" s="5" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="C141" s="5" t="s">
-        <v>48</v>
+        <v>9</v>
       </c>
       <c r="D141" s="5"/>
       <c r="E141" s="5"/>
@@ -4652,13 +4641,13 @@
     </row>
     <row r="142" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A142" s="5" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="B142" s="5" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="C142" s="5" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="D142" s="5"/>
       <c r="E142" s="5"/>
@@ -4666,13 +4655,13 @@
     </row>
     <row r="143" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A143" s="5" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="B143" s="5" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="C143" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D143" s="5"/>
       <c r="E143" s="5"/>
@@ -4680,13 +4669,13 @@
     </row>
     <row r="144" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A144" s="5" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="B144" s="5" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="C144" s="5" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="D144" s="5"/>
       <c r="E144" s="5"/>
@@ -4694,13 +4683,13 @@
     </row>
     <row r="145" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A145" s="5" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="B145" s="5" t="s">
-        <v>138</v>
+        <v>192</v>
       </c>
       <c r="C145" s="5" t="s">
-        <v>27</v>
+        <v>49</v>
       </c>
       <c r="D145" s="5"/>
       <c r="E145" s="5"/>
@@ -4708,13 +4697,13 @@
     </row>
     <row r="146" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A146" s="5" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="B146" s="5" t="s">
-        <v>89</v>
+        <v>139</v>
       </c>
       <c r="C146" s="5" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="D146" s="5"/>
       <c r="E146" s="5"/>
@@ -4722,13 +4711,13 @@
     </row>
     <row r="147" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A147" s="5" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="B147" s="5" t="s">
-        <v>191</v>
+        <v>90</v>
       </c>
       <c r="C147" s="5" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="D147" s="5"/>
       <c r="E147" s="5"/>
@@ -4736,13 +4725,13 @@
     </row>
     <row r="148" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A148" s="5" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="B148" s="5" t="s">
-        <v>98</v>
+        <v>193</v>
       </c>
       <c r="C148" s="5" t="s">
-        <v>45</v>
+        <v>23</v>
       </c>
       <c r="D148" s="5"/>
       <c r="E148" s="5"/>
@@ -4750,41 +4739,43 @@
     </row>
     <row r="149" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A149" s="5" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="B149" s="5" t="s">
-        <v>192</v>
-      </c>
-      <c r="C149" s="5"/>
-      <c r="D149" s="5" t="s">
-        <v>193</v>
-      </c>
+        <v>99</v>
+      </c>
+      <c r="C149" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="D149" s="5"/>
       <c r="E149" s="5"/>
       <c r="F149" s="5"/>
     </row>
     <row r="150" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A150" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="B150" s="5" t="s">
         <v>194</v>
       </c>
-      <c r="B150" s="5" t="s">
+      <c r="C150" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="D150" s="5" t="s">
         <v>195</v>
       </c>
-      <c r="C150" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="D150" s="5"/>
       <c r="E150" s="5"/>
       <c r="F150" s="5"/>
     </row>
     <row r="151" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A151" s="5" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="B151" s="5" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="C151" s="5" t="s">
-        <v>55</v>
+        <v>9</v>
       </c>
       <c r="D151" s="5"/>
       <c r="E151" s="5"/>
@@ -4792,13 +4783,13 @@
     </row>
     <row r="152" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A152" s="5" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="B152" s="5" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="C152" s="5" t="s">
-        <v>14</v>
+        <v>55</v>
       </c>
       <c r="D152" s="5"/>
       <c r="E152" s="5"/>
@@ -4806,13 +4797,13 @@
     </row>
     <row r="153" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A153" s="5" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="B153" s="5" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="C153" s="5" t="s">
-        <v>59</v>
+        <v>14</v>
       </c>
       <c r="D153" s="5"/>
       <c r="E153" s="5"/>
@@ -4820,13 +4811,13 @@
     </row>
     <row r="154" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A154" s="5" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="B154" s="5" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="C154" s="5" t="s">
-        <v>31</v>
+        <v>59</v>
       </c>
       <c r="D154" s="5"/>
       <c r="E154" s="5"/>
@@ -4834,39 +4825,39 @@
     </row>
     <row r="155" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A155" s="5" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="B155" s="5" t="s">
-        <v>200</v>
-      </c>
-      <c r="C155" s="5"/>
+        <v>201</v>
+      </c>
+      <c r="C155" s="5" t="s">
+        <v>31</v>
+      </c>
       <c r="D155" s="5"/>
       <c r="E155" s="5"/>
       <c r="F155" s="5"/>
     </row>
     <row r="156" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A156" s="5" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="B156" s="5" t="s">
-        <v>201</v>
-      </c>
-      <c r="C156" s="5" t="s">
-        <v>62</v>
-      </c>
+        <v>202</v>
+      </c>
+      <c r="C156" s="5"/>
       <c r="D156" s="5"/>
       <c r="E156" s="5"/>
       <c r="F156" s="5"/>
     </row>
     <row r="157" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A157" s="5" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="B157" s="5" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="C157" s="5" t="s">
-        <v>48</v>
+        <v>62</v>
       </c>
       <c r="D157" s="5"/>
       <c r="E157" s="5"/>
@@ -4874,13 +4865,13 @@
     </row>
     <row r="158" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A158" s="5" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="B158" s="5" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="C158" s="5" t="s">
-        <v>24</v>
+        <v>48</v>
       </c>
       <c r="D158" s="5"/>
       <c r="E158" s="5"/>
@@ -4888,13 +4879,13 @@
     </row>
     <row r="159" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A159" s="5" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="B159" s="5" t="s">
-        <v>127</v>
+        <v>205</v>
       </c>
       <c r="C159" s="5" t="s">
-        <v>49</v>
+        <v>24</v>
       </c>
       <c r="D159" s="5"/>
       <c r="E159" s="5"/>
@@ -4902,13 +4893,13 @@
     </row>
     <row r="160" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A160" s="5" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="B160" s="5" t="s">
-        <v>204</v>
+        <v>128</v>
       </c>
       <c r="C160" s="5" t="s">
-        <v>23</v>
+        <v>49</v>
       </c>
       <c r="D160" s="5"/>
       <c r="E160" s="5"/>
@@ -4916,13 +4907,13 @@
     </row>
     <row r="161" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A161" s="5" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="B161" s="5" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="C161" s="5" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="D161" s="5"/>
       <c r="E161" s="5"/>
@@ -4930,13 +4921,13 @@
     </row>
     <row r="162" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A162" s="5" t="s">
-        <v>206</v>
+        <v>196</v>
       </c>
       <c r="B162" s="5" t="s">
         <v>207</v>
       </c>
       <c r="C162" s="5" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="D162" s="5"/>
       <c r="E162" s="5"/>
@@ -4944,13 +4935,13 @@
     </row>
     <row r="163" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A163" s="5" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="B163" s="5" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="C163" s="5" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D163" s="5"/>
       <c r="E163" s="5"/>
@@ -4958,13 +4949,13 @@
     </row>
     <row r="164" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A164" s="5" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="B164" s="5" t="s">
-        <v>104</v>
+        <v>210</v>
       </c>
       <c r="C164" s="5" t="s">
-        <v>37</v>
+        <v>23</v>
       </c>
       <c r="D164" s="5"/>
       <c r="E164" s="5"/>
@@ -4972,13 +4963,13 @@
     </row>
     <row r="165" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A165" s="5" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="B165" s="5" t="s">
-        <v>209</v>
+        <v>105</v>
       </c>
       <c r="C165" s="5" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="D165" s="5"/>
       <c r="E165" s="5"/>
@@ -4986,13 +4977,13 @@
     </row>
     <row r="166" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A166" s="5" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="B166" s="5" t="s">
-        <v>186</v>
+        <v>211</v>
       </c>
       <c r="C166" s="5" t="s">
-        <v>9</v>
+        <v>32</v>
       </c>
       <c r="D166" s="5"/>
       <c r="E166" s="5"/>
@@ -5000,10 +4991,10 @@
     </row>
     <row r="167" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A167" s="5" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B167" s="5" t="s">
-        <v>195</v>
+        <v>188</v>
       </c>
       <c r="C167" s="5" t="s">
         <v>9</v>
@@ -5014,13 +5005,13 @@
     </row>
     <row r="168" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A168" s="5" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="B168" s="5" t="s">
-        <v>211</v>
+        <v>197</v>
       </c>
       <c r="C168" s="5" t="s">
-        <v>54</v>
+        <v>9</v>
       </c>
       <c r="D168" s="5"/>
       <c r="E168" s="5"/>
@@ -5028,13 +5019,13 @@
     </row>
     <row r="169" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A169" s="5" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="B169" s="5" t="s">
-        <v>172</v>
+        <v>213</v>
       </c>
       <c r="C169" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D169" s="5"/>
       <c r="E169" s="5"/>
@@ -5042,13 +5033,13 @@
     </row>
     <row r="170" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A170" s="5" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="B170" s="5" t="s">
-        <v>151</v>
+        <v>173</v>
       </c>
       <c r="C170" s="5" t="s">
-        <v>23</v>
+        <v>55</v>
       </c>
       <c r="D170" s="5"/>
       <c r="E170" s="5"/>
@@ -5056,13 +5047,13 @@
     </row>
     <row r="171" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A171" s="5" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="B171" s="5" t="s">
-        <v>212</v>
+        <v>152</v>
       </c>
       <c r="C171" s="5" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="D171" s="5"/>
       <c r="E171" s="5"/>
@@ -5070,13 +5061,13 @@
     </row>
     <row r="172" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A172" s="5" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B172" s="5" t="s">
-        <v>195</v>
+        <v>214</v>
       </c>
       <c r="C172" s="5" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="D172" s="5"/>
       <c r="E172" s="5"/>
@@ -5084,13 +5075,13 @@
     </row>
     <row r="173" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A173" s="5" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="B173" s="5" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
       <c r="C173" s="5" t="s">
-        <v>41</v>
+        <v>9</v>
       </c>
       <c r="D173" s="5"/>
       <c r="E173" s="5"/>
@@ -5098,13 +5089,13 @@
     </row>
     <row r="174" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A174" s="5" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="B174" s="5" t="s">
-        <v>91</v>
+        <v>205</v>
       </c>
       <c r="C174" s="5" t="s">
-        <v>29</v>
+        <v>41</v>
       </c>
       <c r="D174" s="5"/>
       <c r="E174" s="5"/>
@@ -5112,13 +5103,13 @@
     </row>
     <row r="175" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A175" s="5" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="B175" s="5" t="s">
         <v>92</v>
       </c>
       <c r="C175" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D175" s="5"/>
       <c r="E175" s="5"/>
@@ -5126,13 +5117,13 @@
     </row>
     <row r="176" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A176" s="5" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="B176" s="5" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="C176" s="5" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D176" s="5"/>
       <c r="E176" s="5"/>
@@ -5140,13 +5131,13 @@
     </row>
     <row r="177" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A177" s="5" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="B177" s="5" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="C177" s="5" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="D177" s="5"/>
       <c r="E177" s="5"/>
@@ -5154,13 +5145,13 @@
     </row>
     <row r="178" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A178" s="5" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="B178" s="5" t="s">
-        <v>151</v>
+        <v>99</v>
       </c>
       <c r="C178" s="5" t="s">
-        <v>23</v>
+        <v>45</v>
       </c>
       <c r="D178" s="5"/>
       <c r="E178" s="5"/>
@@ -5168,13 +5159,13 @@
     </row>
     <row r="179" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A179" s="5" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="B179" s="5" t="s">
-        <v>214</v>
+        <v>152</v>
       </c>
       <c r="C179" s="5" t="s">
-        <v>54</v>
+        <v>23</v>
       </c>
       <c r="D179" s="5"/>
       <c r="E179" s="5"/>
@@ -5182,13 +5173,13 @@
     </row>
     <row r="180" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A180" s="5" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="B180" s="5" t="s">
-        <v>80</v>
+        <v>216</v>
       </c>
       <c r="C180" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D180" s="5"/>
       <c r="E180" s="5"/>
@@ -5196,13 +5187,13 @@
     </row>
     <row r="181" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A181" s="5" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="B181" s="5" t="s">
-        <v>166</v>
+        <v>81</v>
       </c>
       <c r="C181" s="5" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="D181" s="5"/>
       <c r="E181" s="5"/>
@@ -5213,56 +5204,56 @@
         <v>215</v>
       </c>
       <c r="B182" s="5" t="s">
-        <v>179</v>
+        <v>167</v>
       </c>
       <c r="C182" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="D182" s="5" t="s">
-        <v>216</v>
-      </c>
+        <v>62</v>
+      </c>
+      <c r="D182" s="5"/>
       <c r="E182" s="5"/>
       <c r="F182" s="5"/>
     </row>
     <row r="183" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A183" s="5" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="B183" s="5" t="s">
-        <v>217</v>
+        <v>180</v>
       </c>
       <c r="C183" s="5" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="D183" s="5" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="E183" s="5"/>
       <c r="F183" s="5"/>
     </row>
     <row r="184" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A184" s="5" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B184" s="5" t="s">
         <v>219</v>
       </c>
       <c r="C184" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="D184" s="5"/>
+        <v>26</v>
+      </c>
+      <c r="D184" s="5" t="s">
+        <v>218</v>
+      </c>
       <c r="E184" s="5"/>
       <c r="F184" s="5"/>
     </row>
     <row r="185" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A185" s="5" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="B185" s="5" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="C185" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D185" s="5"/>
       <c r="E185" s="5"/>
@@ -5270,13 +5261,13 @@
     </row>
     <row r="186" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A186" s="5" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="B186" s="5" t="s">
-        <v>23</v>
+        <v>222</v>
       </c>
       <c r="C186" s="5" t="s">
-        <v>23</v>
+        <v>55</v>
       </c>
       <c r="D186" s="5"/>
       <c r="E186" s="5"/>
@@ -5284,13 +5275,13 @@
     </row>
     <row r="187" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A187" s="5" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="B187" s="5" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C187" s="5" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="D187" s="5"/>
       <c r="E187" s="5"/>
@@ -5298,22 +5289,28 @@
     </row>
     <row r="188" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A188" s="5" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="B188" s="5" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="C188" s="5" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="D188" s="5"/>
       <c r="E188" s="5"/>
       <c r="F188" s="5"/>
     </row>
     <row r="189" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A189" s="5"/>
-      <c r="B189" s="5"/>
-      <c r="C189" s="5"/>
+      <c r="A189" s="5" t="s">
+        <v>220</v>
+      </c>
+      <c r="B189" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C189" s="5" t="s">
+        <v>32</v>
+      </c>
       <c r="D189" s="5"/>
       <c r="E189" s="5"/>
       <c r="F189" s="5"/>
@@ -5742,9 +5739,17 @@
       <c r="E242" s="5"/>
       <c r="F242" s="5"/>
     </row>
+    <row r="243" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A243" s="5"/>
+      <c r="B243" s="5"/>
+      <c r="C243" s="5"/>
+      <c r="D243" s="5"/>
+      <c r="E243" s="5"/>
+      <c r="F243" s="5"/>
+    </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="C1:C1188" type="list">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="C1:C1189" type="list">
       <formula1>controlled_vocabulary!$A$4:$A$9999</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -5777,12 +5782,12 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Addition on tests, edit of things, etc
</commit_message>
<xml_diff>
--- a/inst/extdata/cell_type_mapping.xlsx
+++ b/inst/extdata/cell_type_mapping.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2de447d5b5f1ff5a/Desktop/Master_thesis/immunedeconv/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="188" documentId="11_B9E004A660C9D12CF4E0EE8B9BCDFA07B1516133" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7F0DC99A-65DC-414F-929D-C2EA4BCAFD13}"/>
+  <xr:revisionPtr revIDLastSave="200" documentId="11_B9E004A660C9D12CF4E0EE8B9BCDFA07B1516133" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{12D55A49-094B-4021-B6EE-04E2B268F5A9}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="21600" windowHeight="11385" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="controlled_vocabulary" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="972" uniqueCount="293">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1029" uniqueCount="294">
   <si>
     <t>cell_type</t>
   </si>
@@ -849,9 +849,6 @@
     <t>mmcp_counter</t>
   </si>
   <si>
-    <t>seqImmuCC</t>
-  </si>
-  <si>
     <t>B Cells</t>
   </si>
   <si>
@@ -870,9 +867,6 @@
     <t>NK Cells</t>
   </si>
   <si>
-    <t>DCQ</t>
-  </si>
-  <si>
     <t>Dev_B_cells</t>
   </si>
   <si>
@@ -916,6 +910,15 @@
   </si>
   <si>
     <t>Stem cell</t>
+  </si>
+  <si>
+    <t>seqimmucc</t>
+  </si>
+  <si>
+    <t>dcq</t>
+  </si>
+  <si>
+    <t>base</t>
   </si>
 </sst>
 </file>
@@ -3195,7 +3198,7 @@
     </row>
     <row r="74" spans="1:3">
       <c r="A74" s="1" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="B74" s="1" t="s">
         <v>24</v>
@@ -3203,7 +3206,7 @@
     </row>
     <row r="75" spans="1:3">
       <c r="A75" s="1" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="B75" s="1" t="s">
         <v>17</v>
@@ -3224,10 +3227,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:F269"/>
+  <dimension ref="A1:F288"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A217" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D240" sqref="D240"/>
+    <sheetView tabSelected="1" topLeftCell="A268" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A290" sqref="A290"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15"/>
@@ -6608,10 +6611,10 @@
     </row>
     <row r="241" spans="1:6">
       <c r="A241" s="5" t="s">
+        <v>291</v>
+      </c>
+      <c r="B241" s="5" t="s">
         <v>270</v>
-      </c>
-      <c r="B241" s="5" t="s">
-        <v>271</v>
       </c>
       <c r="C241" s="5" t="s">
         <v>9</v>
@@ -6622,10 +6625,10 @@
     </row>
     <row r="242" spans="1:6">
       <c r="A242" s="5" t="s">
-        <v>270</v>
+        <v>291</v>
       </c>
       <c r="B242" s="5" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C242" s="5" t="s">
         <v>53</v>
@@ -6636,10 +6639,10 @@
     </row>
     <row r="243" spans="1:6">
       <c r="A243" s="5" t="s">
-        <v>270</v>
+        <v>291</v>
       </c>
       <c r="B243" s="5" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C243" s="5" t="s">
         <v>54</v>
@@ -6650,10 +6653,10 @@
     </row>
     <row r="244" spans="1:6">
       <c r="A244" s="5" t="s">
-        <v>270</v>
+        <v>291</v>
       </c>
       <c r="B244" s="5" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C244" s="5" t="s">
         <v>36</v>
@@ -6661,7 +6664,7 @@
     </row>
     <row r="245" spans="1:6">
       <c r="A245" s="5" t="s">
-        <v>270</v>
+        <v>291</v>
       </c>
       <c r="B245" s="5" t="s">
         <v>97</v>
@@ -6672,7 +6675,7 @@
     </row>
     <row r="246" spans="1:6">
       <c r="A246" s="5" t="s">
-        <v>270</v>
+        <v>291</v>
       </c>
       <c r="B246" s="5" t="s">
         <v>138</v>
@@ -6683,10 +6686,10 @@
     </row>
     <row r="247" spans="1:6">
       <c r="A247" s="5" t="s">
-        <v>270</v>
+        <v>291</v>
       </c>
       <c r="B247" s="5" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C247" s="5" t="s">
         <v>261</v>
@@ -6694,7 +6697,7 @@
     </row>
     <row r="248" spans="1:6">
       <c r="A248" s="5" t="s">
-        <v>270</v>
+        <v>291</v>
       </c>
       <c r="B248" s="5" t="s">
         <v>89</v>
@@ -6705,7 +6708,7 @@
     </row>
     <row r="249" spans="1:6">
       <c r="A249" s="5" t="s">
-        <v>270</v>
+        <v>291</v>
       </c>
       <c r="B249" s="5" t="s">
         <v>98</v>
@@ -6716,10 +6719,10 @@
     </row>
     <row r="250" spans="1:6">
       <c r="A250" s="5" t="s">
-        <v>270</v>
+        <v>291</v>
       </c>
       <c r="B250" s="5" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C250" s="5" t="s">
         <v>22</v>
@@ -6727,9 +6730,9 @@
     </row>
     <row r="251" spans="1:6">
       <c r="A251" s="5" t="s">
-        <v>277</v>
-      </c>
-      <c r="B251" t="s">
+        <v>292</v>
+      </c>
+      <c r="B251" s="7" t="s">
         <v>249</v>
       </c>
       <c r="C251" s="5" t="s">
@@ -6738,10 +6741,10 @@
     </row>
     <row r="252" spans="1:6">
       <c r="A252" s="5" t="s">
-        <v>277</v>
-      </c>
-      <c r="B252" t="s">
-        <v>278</v>
+        <v>292</v>
+      </c>
+      <c r="B252" s="7" t="s">
+        <v>276</v>
       </c>
       <c r="C252" s="5" t="s">
         <v>10</v>
@@ -6749,10 +6752,10 @@
     </row>
     <row r="253" spans="1:6">
       <c r="A253" s="5" t="s">
+        <v>292</v>
+      </c>
+      <c r="B253" s="7" t="s">
         <v>277</v>
-      </c>
-      <c r="B253" t="s">
-        <v>279</v>
       </c>
       <c r="C253" s="5" t="s">
         <v>52</v>
@@ -6760,9 +6763,9 @@
     </row>
     <row r="254" spans="1:6">
       <c r="A254" s="5" t="s">
-        <v>277</v>
-      </c>
-      <c r="B254" t="s">
+        <v>292</v>
+      </c>
+      <c r="B254" s="7" t="s">
         <v>251</v>
       </c>
       <c r="C254" s="5" t="s">
@@ -6771,10 +6774,10 @@
     </row>
     <row r="255" spans="1:6">
       <c r="A255" s="5" t="s">
-        <v>277</v>
-      </c>
-      <c r="B255" t="s">
-        <v>280</v>
+        <v>292</v>
+      </c>
+      <c r="B255" s="7" t="s">
+        <v>278</v>
       </c>
       <c r="C255" s="5" t="s">
         <v>23</v>
@@ -6782,9 +6785,9 @@
     </row>
     <row r="256" spans="1:6">
       <c r="A256" s="5" t="s">
-        <v>277</v>
-      </c>
-      <c r="B256" t="s">
+        <v>292</v>
+      </c>
+      <c r="B256" s="7" t="s">
         <v>265</v>
       </c>
       <c r="C256" s="5" t="s">
@@ -6793,9 +6796,9 @@
     </row>
     <row r="257" spans="1:3">
       <c r="A257" s="5" t="s">
-        <v>277</v>
-      </c>
-      <c r="B257" t="s">
+        <v>292</v>
+      </c>
+      <c r="B257" s="7" t="s">
         <v>138</v>
       </c>
       <c r="C257" s="5" t="s">
@@ -6804,20 +6807,20 @@
     </row>
     <row r="258" spans="1:3">
       <c r="A258" s="5" t="s">
-        <v>277</v>
-      </c>
-      <c r="B258" t="s">
-        <v>281</v>
+        <v>292</v>
+      </c>
+      <c r="B258" s="7" t="s">
+        <v>279</v>
       </c>
       <c r="C258" s="5" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
     </row>
     <row r="259" spans="1:3">
       <c r="A259" s="5" t="s">
-        <v>277</v>
-      </c>
-      <c r="B259" t="s">
+        <v>292</v>
+      </c>
+      <c r="B259" s="7" t="s">
         <v>89</v>
       </c>
       <c r="C259" s="5" t="s">
@@ -6826,9 +6829,9 @@
     </row>
     <row r="260" spans="1:3">
       <c r="A260" s="5" t="s">
-        <v>277</v>
-      </c>
-      <c r="B260" t="s">
+        <v>292</v>
+      </c>
+      <c r="B260" s="7" t="s">
         <v>253</v>
       </c>
       <c r="C260" s="5" t="s">
@@ -6837,10 +6840,10 @@
     </row>
     <row r="261" spans="1:3">
       <c r="A261" s="5" t="s">
-        <v>277</v>
-      </c>
-      <c r="B261" t="s">
-        <v>282</v>
+        <v>292</v>
+      </c>
+      <c r="B261" s="7" t="s">
+        <v>280</v>
       </c>
       <c r="C261" s="5" t="s">
         <v>57</v>
@@ -6848,21 +6851,21 @@
     </row>
     <row r="262" spans="1:3">
       <c r="A262" s="5" t="s">
-        <v>277</v>
-      </c>
-      <c r="B262" t="s">
-        <v>283</v>
+        <v>292</v>
+      </c>
+      <c r="B262" s="7" t="s">
+        <v>281</v>
       </c>
       <c r="C262" s="5" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
     </row>
     <row r="263" spans="1:3">
       <c r="A263" s="5" t="s">
-        <v>277</v>
-      </c>
-      <c r="B263" t="s">
-        <v>284</v>
+        <v>292</v>
+      </c>
+      <c r="B263" s="7" t="s">
+        <v>282</v>
       </c>
       <c r="C263" s="5" t="s">
         <v>63</v>
@@ -6870,10 +6873,10 @@
     </row>
     <row r="264" spans="1:3">
       <c r="A264" s="5" t="s">
-        <v>277</v>
-      </c>
-      <c r="B264" t="s">
-        <v>285</v>
+        <v>292</v>
+      </c>
+      <c r="B264" s="7" t="s">
+        <v>283</v>
       </c>
       <c r="C264" s="5" t="s">
         <v>61</v>
@@ -6881,10 +6884,10 @@
     </row>
     <row r="265" spans="1:3">
       <c r="A265" s="5" t="s">
-        <v>277</v>
-      </c>
-      <c r="B265" t="s">
-        <v>286</v>
+        <v>292</v>
+      </c>
+      <c r="B265" s="7" t="s">
+        <v>284</v>
       </c>
       <c r="C265" s="9" t="s">
         <v>62</v>
@@ -6892,10 +6895,10 @@
     </row>
     <row r="266" spans="1:3">
       <c r="A266" s="5" t="s">
-        <v>277</v>
-      </c>
-      <c r="B266" t="s">
-        <v>287</v>
+        <v>292</v>
+      </c>
+      <c r="B266" s="7" t="s">
+        <v>285</v>
       </c>
       <c r="C266" s="5" t="s">
         <v>72</v>
@@ -6903,10 +6906,10 @@
     </row>
     <row r="267" spans="1:3">
       <c r="A267" s="5" t="s">
-        <v>277</v>
-      </c>
-      <c r="B267" t="s">
-        <v>288</v>
+        <v>292</v>
+      </c>
+      <c r="B267" s="7" t="s">
+        <v>286</v>
       </c>
       <c r="C267" s="5" t="s">
         <v>67</v>
@@ -6914,10 +6917,10 @@
     </row>
     <row r="268" spans="1:3">
       <c r="A268" s="5" t="s">
-        <v>277</v>
-      </c>
-      <c r="B268" t="s">
-        <v>289</v>
+        <v>292</v>
+      </c>
+      <c r="B268" s="7" t="s">
+        <v>287</v>
       </c>
       <c r="C268" s="5" t="s">
         <v>68</v>
@@ -6925,12 +6928,221 @@
     </row>
     <row r="269" spans="1:3">
       <c r="A269" s="5" t="s">
+        <v>292</v>
+      </c>
+      <c r="B269" s="7" t="s">
+        <v>288</v>
+      </c>
+      <c r="C269" s="7" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="270" spans="1:3">
+      <c r="A270" t="s">
+        <v>293</v>
+      </c>
+      <c r="B270" t="s">
+        <v>249</v>
+      </c>
+      <c r="C270" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="271" spans="1:3">
+      <c r="A271" t="s">
+        <v>293</v>
+      </c>
+      <c r="B271" t="s">
+        <v>276</v>
+      </c>
+      <c r="C271" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="272" spans="1:3">
+      <c r="A272" t="s">
+        <v>293</v>
+      </c>
+      <c r="B272" t="s">
         <v>277</v>
       </c>
-      <c r="B269" t="s">
+      <c r="C272" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="273" spans="1:3">
+      <c r="A273" t="s">
+        <v>293</v>
+      </c>
+      <c r="B273" t="s">
+        <v>251</v>
+      </c>
+      <c r="C273" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="274" spans="1:3">
+      <c r="A274" t="s">
+        <v>293</v>
+      </c>
+      <c r="B274" t="s">
+        <v>278</v>
+      </c>
+      <c r="C274" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="275" spans="1:3">
+      <c r="A275" t="s">
+        <v>293</v>
+      </c>
+      <c r="B275" t="s">
+        <v>265</v>
+      </c>
+      <c r="C275" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="276" spans="1:3">
+      <c r="A276" t="s">
+        <v>293</v>
+      </c>
+      <c r="B276" t="s">
+        <v>138</v>
+      </c>
+      <c r="C276" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="277" spans="1:3">
+      <c r="A277" t="s">
+        <v>293</v>
+      </c>
+      <c r="B277" t="s">
+        <v>279</v>
+      </c>
+      <c r="C277" t="s">
         <v>290</v>
       </c>
-      <c r="C269" s="7" t="s">
+    </row>
+    <row r="278" spans="1:3">
+      <c r="A278" t="s">
+        <v>293</v>
+      </c>
+      <c r="B278" t="s">
+        <v>89</v>
+      </c>
+      <c r="C278" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="279" spans="1:3">
+      <c r="A279" t="s">
+        <v>293</v>
+      </c>
+      <c r="B279" t="s">
+        <v>253</v>
+      </c>
+      <c r="C279" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="280" spans="1:3">
+      <c r="A280" t="s">
+        <v>293</v>
+      </c>
+      <c r="B280" t="s">
+        <v>280</v>
+      </c>
+      <c r="C280" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="281" spans="1:3">
+      <c r="A281" t="s">
+        <v>293</v>
+      </c>
+      <c r="B281" t="s">
+        <v>281</v>
+      </c>
+      <c r="C281" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="282" spans="1:3">
+      <c r="A282" t="s">
+        <v>293</v>
+      </c>
+      <c r="B282" t="s">
+        <v>282</v>
+      </c>
+      <c r="C282" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="283" spans="1:3">
+      <c r="A283" t="s">
+        <v>293</v>
+      </c>
+      <c r="B283" t="s">
+        <v>283</v>
+      </c>
+      <c r="C283" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="284" spans="1:3">
+      <c r="A284" t="s">
+        <v>293</v>
+      </c>
+      <c r="B284" t="s">
+        <v>284</v>
+      </c>
+      <c r="C284" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="285" spans="1:3">
+      <c r="A285" t="s">
+        <v>293</v>
+      </c>
+      <c r="B285" t="s">
+        <v>285</v>
+      </c>
+      <c r="C285" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="286" spans="1:3">
+      <c r="A286" t="s">
+        <v>293</v>
+      </c>
+      <c r="B286" t="s">
+        <v>286</v>
+      </c>
+      <c r="C286" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="287" spans="1:3">
+      <c r="A287" t="s">
+        <v>293</v>
+      </c>
+      <c r="B287" t="s">
+        <v>287</v>
+      </c>
+      <c r="C287" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="288" spans="1:3">
+      <c r="A288" t="s">
+        <v>293</v>
+      </c>
+      <c r="B288" t="s">
+        <v>288</v>
+      </c>
+      <c r="C288" t="s">
         <v>55</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update estimate to fit with other human deconvolution methods, and update of license
</commit_message>
<xml_diff>
--- a/inst/extdata/cell_type_mapping.xlsx
+++ b/inst/extdata/cell_type_mapping.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20387"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2de447d5b5f1ff5a/Desktop/Master_thesis/immunedeconv/inst/extdata/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\c1041161\immunedeconv\inst\extdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="200" documentId="11_B9E004A660C9D12CF4E0EE8B9BCDFA07B1516133" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{12D55A49-094B-4021-B6EE-04E2B268F5A9}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF74A6EB-5D72-4E6A-9AE3-B2ABC2451C54}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="780" yWindow="780" windowWidth="21600" windowHeight="11385" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -19,16 +19,6 @@
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
     </ext>
@@ -37,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1029" uniqueCount="294">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1045" uniqueCount="300">
   <si>
     <t>cell_type</t>
   </si>
@@ -919,6 +909,24 @@
   </si>
   <si>
     <t>base</t>
+  </si>
+  <si>
+    <t>estimate</t>
+  </si>
+  <si>
+    <t>StromalScore</t>
+  </si>
+  <si>
+    <t>ESTIMATEScore</t>
+  </si>
+  <si>
+    <t>TumorPurity</t>
+  </si>
+  <si>
+    <t>tumor purity score</t>
+  </si>
+  <si>
+    <t>tumor purity fraction</t>
   </si>
 </sst>
 </file>
@@ -1039,7 +1047,7 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normale" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1170,7 +1178,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema di Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1466,10 +1474,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AMK75"/>
+  <dimension ref="A1:AMK77"/>
   <sheetViews>
-    <sheetView topLeftCell="A49" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B77" sqref="B77"/>
+    <sheetView topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A50" sqref="A50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -1954,7 +1962,7 @@
     </row>
     <row r="50" spans="1:1024">
       <c r="A50" s="9" t="s">
-        <v>52</v>
+        <v>299</v>
       </c>
       <c r="B50" s="1" t="s">
         <v>7</v>
@@ -1962,73 +1970,61 @@
     </row>
     <row r="51" spans="1:1024">
       <c r="A51" s="9" t="s">
-        <v>53</v>
+        <v>298</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>24</v>
+        <v>7</v>
       </c>
     </row>
     <row r="52" spans="1:1024">
       <c r="A52" s="9" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>24</v>
+        <v>7</v>
       </c>
     </row>
     <row r="53" spans="1:1024">
       <c r="A53" s="9" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B53" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C53" s="1" t="b">
+    </row>
+    <row r="54" spans="1:1024">
+      <c r="A54" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1024">
+      <c r="A55" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C55" s="1" t="b">
         <f>TRUE()</f>
         <v>1</v>
       </c>
-      <c r="D53" s="1" t="s">
+      <c r="D55" s="1" t="s">
         <v>56</v>
-      </c>
-    </row>
-    <row r="54" spans="1:1024">
-      <c r="A54" s="9" t="s">
-        <v>57</v>
-      </c>
-      <c r="B54" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C54" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="55" spans="1:1024">
-      <c r="A55" s="9" t="s">
-        <v>58</v>
-      </c>
-      <c r="B55" s="1" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="56" spans="1:1024">
       <c r="A56" s="9" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>58</v>
+        <v>24</v>
       </c>
       <c r="C56" s="1">
         <v>1</v>
       </c>
-      <c r="E56"/>
-      <c r="F56"/>
-      <c r="G56"/>
-      <c r="H56"/>
-      <c r="I56"/>
-      <c r="J56"/>
-      <c r="K56"/>
-      <c r="L56"/>
-      <c r="M56"/>
       <c r="N56"/>
       <c r="O56"/>
       <c r="P56"/>
@@ -3043,111 +3039,117 @@
     </row>
     <row r="57" spans="1:1024">
       <c r="A57" s="9" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="C57" s="1">
-        <v>1</v>
+        <v>53</v>
       </c>
     </row>
     <row r="58" spans="1:1024">
       <c r="A58" s="9" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>53</v>
-      </c>
+        <v>58</v>
+      </c>
+      <c r="C58" s="1">
+        <v>1</v>
+      </c>
+      <c r="E58"/>
+      <c r="F58"/>
+      <c r="G58"/>
+      <c r="H58"/>
+      <c r="I58"/>
+      <c r="J58"/>
+      <c r="K58"/>
+      <c r="L58"/>
+      <c r="M58"/>
     </row>
     <row r="59" spans="1:1024">
       <c r="A59" s="9" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B59" s="1" t="s">
         <v>58</v>
       </c>
+      <c r="C59" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="60" spans="1:1024">
       <c r="A60" s="9" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
     </row>
     <row r="61" spans="1:1024">
       <c r="A61" s="9" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B61" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="C61" s="1" t="b">
+    </row>
+    <row r="62" spans="1:1024">
+      <c r="A62" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1024">
+      <c r="A63" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C63" s="1" t="b">
         <f>TRUE()</f>
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:1024">
-      <c r="A62" s="9" t="s">
-        <v>65</v>
-      </c>
-      <c r="B62" s="1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="63" spans="1:1024">
-      <c r="A63" s="9" t="s">
-        <v>66</v>
-      </c>
-      <c r="B63" s="1" t="s">
-        <v>62</v>
-      </c>
-    </row>
     <row r="64" spans="1:1024">
       <c r="A64" s="9" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
     </row>
     <row r="65" spans="1:3">
       <c r="A65" s="9" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
     </row>
     <row r="66" spans="1:3">
       <c r="A66" s="9" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="C66" s="1">
-        <v>1</v>
+        <v>54</v>
       </c>
     </row>
     <row r="67" spans="1:3">
       <c r="A67" s="9" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="C67" s="1">
-        <v>1</v>
+        <v>54</v>
       </c>
     </row>
     <row r="68" spans="1:3">
       <c r="A68" s="9" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="C68" s="1">
         <v>1</v>
@@ -3155,10 +3157,10 @@
     </row>
     <row r="69" spans="1:3">
       <c r="A69" s="9" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="C69" s="1">
         <v>1</v>
@@ -3166,55 +3168,77 @@
     </row>
     <row r="70" spans="1:3">
       <c r="A70" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C70" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3">
+      <c r="A71" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C71" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3">
+      <c r="A72" s="9" t="s">
         <v>241</v>
       </c>
-      <c r="B70" s="1" t="s">
+      <c r="B72" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="71" spans="1:3">
-      <c r="A71" s="10" t="s">
+    <row r="73" spans="1:3">
+      <c r="A73" s="10" t="s">
         <v>242</v>
       </c>
-      <c r="B71" s="1" t="s">
+      <c r="B73" s="1" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="72" spans="1:3">
-      <c r="A72" s="10" t="s">
+    <row r="74" spans="1:3">
+      <c r="A74" s="10" t="s">
         <v>247</v>
       </c>
-      <c r="B72" s="1" t="s">
+      <c r="B74" s="1" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="73" spans="1:3">
-      <c r="A73" s="9" t="s">
+    <row r="75" spans="1:3">
+      <c r="A75" s="9" t="s">
         <v>73</v>
-      </c>
-      <c r="B73" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="74" spans="1:3">
-      <c r="A74" s="1" t="s">
-        <v>289</v>
-      </c>
-      <c r="B74" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="75" spans="1:3">
-      <c r="A75" s="1" t="s">
-        <v>290</v>
       </c>
       <c r="B75" s="1" t="s">
         <v>17</v>
       </c>
     </row>
+    <row r="76" spans="1:3">
+      <c r="A76" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="B76" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3">
+      <c r="A77" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="B77" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B75:B1068 B73 B1:B70" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B77:B1070 B75 B1:B72" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>$A:$A</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -3227,10 +3251,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:F288"/>
+  <dimension ref="A1:F292"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A268" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A290" sqref="A290"/>
+    <sheetView tabSelected="1" topLeftCell="A256" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B290" sqref="B290"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15"/>
@@ -7146,6 +7170,50 @@
         <v>55</v>
       </c>
     </row>
+    <row r="289" spans="1:3">
+      <c r="A289" t="s">
+        <v>294</v>
+      </c>
+      <c r="B289" t="s">
+        <v>295</v>
+      </c>
+      <c r="C289" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="290" spans="1:3">
+      <c r="A290" t="s">
+        <v>294</v>
+      </c>
+      <c r="B290" t="s">
+        <v>167</v>
+      </c>
+      <c r="C290" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="291" spans="1:3">
+      <c r="A291" t="s">
+        <v>294</v>
+      </c>
+      <c r="B291" t="s">
+        <v>296</v>
+      </c>
+      <c r="C291" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="292" spans="1:3">
+      <c r="A292" t="s">
+        <v>294</v>
+      </c>
+      <c r="B292" t="s">
+        <v>297</v>
+      </c>
+      <c r="C292" t="s">
+        <v>299</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -7154,7 +7222,7 @@
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
         <x14:dataValidation type="list" operator="equal" allowBlank="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000000000000}">
           <x14:formula1>
-            <xm:f>controlled_vocabulary!$A$4:$A$10001</xm:f>
+            <xm:f>controlled_vocabulary!$A$4:$A$10003</xm:f>
           </x14:formula1>
           <x14:formula2>
             <xm:f>0</xm:f>

</xml_diff>

<commit_message>
update on cell type mappings
</commit_message>
<xml_diff>
--- a/inst/extdata/cell_type_mapping.xlsx
+++ b/inst/extdata/cell_type_mapping.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\c1041161\immunedeconv\inst\extdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C78E85D3-2E91-4F8D-8098-EDB803213B29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F554760A-5EDA-442E-9D5F-22DACEE24C6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3510" yWindow="3510" windowWidth="21600" windowHeight="11385" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15165" yWindow="-16320" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="controlled_vocabulary" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1039" uniqueCount="300">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1039" uniqueCount="299">
   <si>
     <t>cell_type</t>
   </si>
@@ -792,9 +792,6 @@
   </si>
   <si>
     <t>Mast_cells</t>
-  </si>
-  <si>
-    <t>MAST cell</t>
   </si>
   <si>
     <t>NK_cells</t>
@@ -1474,7 +1471,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AMJ77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A41" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A41" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C57" sqref="C57"/>
     </sheetView>
   </sheetViews>
@@ -2239,8 +2236,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F290"/>
   <sheetViews>
-    <sheetView topLeftCell="A270" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C283" sqref="C283"/>
+    <sheetView tabSelected="1" topLeftCell="A262" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D282" sqref="D282"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15"/>
@@ -2526,7 +2523,7 @@
         <v>106</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D20" s="9"/>
       <c r="E20" s="9"/>
@@ -2540,7 +2537,7 @@
         <v>107</v>
       </c>
       <c r="C21" s="8" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D21" s="9"/>
       <c r="E21" s="9"/>
@@ -2834,7 +2831,7 @@
         <v>106</v>
       </c>
       <c r="C42" s="8" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D42" s="9"/>
       <c r="E42" s="9"/>
@@ -2848,7 +2845,7 @@
         <v>107</v>
       </c>
       <c r="C43" s="8" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D43" s="9"/>
       <c r="E43" s="9"/>
@@ -5221,7 +5218,7 @@
         <v>254</v>
       </c>
       <c r="C212" s="10" t="s">
-        <v>255</v>
+        <v>35</v>
       </c>
       <c r="D212" s="9"/>
       <c r="E212" s="9"/>
@@ -5232,7 +5229,7 @@
         <v>250</v>
       </c>
       <c r="B213" s="10" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C213" s="10" t="s">
         <v>24</v>
@@ -5260,7 +5257,7 @@
         <v>250</v>
       </c>
       <c r="B215" s="10" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C215" s="10" t="s">
         <v>59</v>
@@ -5274,7 +5271,7 @@
         <v>250</v>
       </c>
       <c r="B216" s="10" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C216" s="10" t="s">
         <v>60</v>
@@ -5288,7 +5285,7 @@
         <v>250</v>
       </c>
       <c r="B217" s="10" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C217" s="10" t="s">
         <v>61</v>
@@ -5302,7 +5299,7 @@
         <v>250</v>
       </c>
       <c r="B218" s="10" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C218" s="10" t="s">
         <v>67</v>
@@ -5316,7 +5313,7 @@
         <v>250</v>
       </c>
       <c r="B219" s="10" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C219" s="10" t="s">
         <v>30</v>
@@ -5330,7 +5327,7 @@
         <v>250</v>
       </c>
       <c r="B220" s="10" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C220" s="10" t="s">
         <v>31</v>
@@ -5386,7 +5383,7 @@
         <v>250</v>
       </c>
       <c r="B224" s="10" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C224" s="10" t="s">
         <v>54</v>
@@ -5397,7 +5394,7 @@
     </row>
     <row r="225" spans="1:6">
       <c r="A225" s="10" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B225" s="10" t="s">
         <v>182</v>
@@ -5411,7 +5408,7 @@
     </row>
     <row r="226" spans="1:6">
       <c r="A226" s="10" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B226" s="10" t="s">
         <v>183</v>
@@ -5425,7 +5422,7 @@
     </row>
     <row r="227" spans="1:6">
       <c r="A227" s="10" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B227" s="9" t="s">
         <v>162</v>
@@ -5439,10 +5436,10 @@
     </row>
     <row r="228" spans="1:6">
       <c r="A228" s="10" t="s">
+        <v>263</v>
+      </c>
+      <c r="B228" s="9" t="s">
         <v>264</v>
-      </c>
-      <c r="B228" s="9" t="s">
-        <v>265</v>
       </c>
       <c r="C228" s="9" t="s">
         <v>9</v>
@@ -5453,10 +5450,10 @@
     </row>
     <row r="229" spans="1:6">
       <c r="A229" s="10" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B229" s="9" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C229" s="9" t="s">
         <v>8</v>
@@ -5467,10 +5464,10 @@
     </row>
     <row r="230" spans="1:6">
       <c r="A230" s="10" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B230" s="9" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C230" s="9" t="s">
         <v>32</v>
@@ -5481,7 +5478,7 @@
     </row>
     <row r="231" spans="1:6">
       <c r="A231" s="10" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B231" s="9" t="s">
         <v>100</v>
@@ -5495,10 +5492,10 @@
     </row>
     <row r="232" spans="1:6">
       <c r="A232" s="10" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B232" s="9" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C232" s="9" t="s">
         <v>41</v>
@@ -5509,13 +5506,13 @@
     </row>
     <row r="233" spans="1:6">
       <c r="A233" s="10" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B233" s="9" t="s">
         <v>150</v>
       </c>
       <c r="C233" s="9" t="s">
-        <v>255</v>
+        <v>35</v>
       </c>
       <c r="D233" s="9"/>
       <c r="E233" s="9"/>
@@ -5523,7 +5520,7 @@
     </row>
     <row r="234" spans="1:6">
       <c r="A234" s="10" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B234" s="9" t="s">
         <v>108</v>
@@ -5537,7 +5534,7 @@
     </row>
     <row r="235" spans="1:6">
       <c r="A235" s="10" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B235" s="9" t="s">
         <v>109</v>
@@ -5551,7 +5548,7 @@
     </row>
     <row r="236" spans="1:6">
       <c r="A236" s="10" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B236" s="9" t="s">
         <v>121</v>
@@ -5565,10 +5562,10 @@
     </row>
     <row r="237" spans="1:6">
       <c r="A237" s="10" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B237" s="9" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C237" s="9"/>
       <c r="D237" s="9" t="s">
@@ -5579,10 +5576,10 @@
     </row>
     <row r="238" spans="1:6">
       <c r="A238" s="10" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B238" s="9" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C238" s="9"/>
       <c r="D238" s="9" t="s">
@@ -5593,7 +5590,7 @@
     </row>
     <row r="239" spans="1:6">
       <c r="A239" s="10" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B239" s="9" t="s">
         <v>138</v>
@@ -5607,10 +5604,10 @@
     </row>
     <row r="240" spans="1:6">
       <c r="A240" s="10" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B240" s="9" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C240" s="9" t="s">
         <v>51</v>
@@ -5621,10 +5618,10 @@
     </row>
     <row r="241" spans="1:6">
       <c r="A241" s="9" t="s">
+        <v>271</v>
+      </c>
+      <c r="B241" s="9" t="s">
         <v>272</v>
-      </c>
-      <c r="B241" s="9" t="s">
-        <v>273</v>
       </c>
       <c r="C241" s="9" t="s">
         <v>9</v>
@@ -5635,10 +5632,10 @@
     </row>
     <row r="242" spans="1:6">
       <c r="A242" s="9" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B242" s="9" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C242" s="9" t="s">
         <v>59</v>
@@ -5649,10 +5646,10 @@
     </row>
     <row r="243" spans="1:6">
       <c r="A243" s="9" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B243" s="9" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C243" s="9" t="s">
         <v>60</v>
@@ -5663,10 +5660,10 @@
     </row>
     <row r="244" spans="1:6">
       <c r="A244" s="9" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B244" s="9" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C244" s="9" t="s">
         <v>38</v>
@@ -5674,7 +5671,7 @@
     </row>
     <row r="245" spans="1:6">
       <c r="A245" s="9" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B245" s="9" t="s">
         <v>108</v>
@@ -5685,7 +5682,7 @@
     </row>
     <row r="246" spans="1:6">
       <c r="A246" s="9" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B246" s="9" t="s">
         <v>149</v>
@@ -5696,18 +5693,18 @@
     </row>
     <row r="247" spans="1:6">
       <c r="A247" s="9" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B247" s="9" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C247" s="9" t="s">
-        <v>255</v>
+        <v>35</v>
       </c>
     </row>
     <row r="248" spans="1:6">
       <c r="A248" s="9" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B248" s="9" t="s">
         <v>100</v>
@@ -5718,7 +5715,7 @@
     </row>
     <row r="249" spans="1:6">
       <c r="A249" s="9" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B249" s="9" t="s">
         <v>109</v>
@@ -5729,10 +5726,10 @@
     </row>
     <row r="250" spans="1:6">
       <c r="A250" s="9" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B250" s="9" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C250" s="9" t="s">
         <v>24</v>
@@ -5740,7 +5737,7 @@
     </row>
     <row r="251" spans="1:6">
       <c r="A251" s="9" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B251" s="10" t="s">
         <v>251</v>
@@ -5751,10 +5748,10 @@
     </row>
     <row r="252" spans="1:6">
       <c r="A252" s="9" t="s">
+        <v>278</v>
+      </c>
+      <c r="B252" s="10" t="s">
         <v>279</v>
-      </c>
-      <c r="B252" s="10" t="s">
-        <v>280</v>
       </c>
       <c r="C252" s="9" t="s">
         <v>10</v>
@@ -5762,10 +5759,10 @@
     </row>
     <row r="253" spans="1:6">
       <c r="A253" s="9" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B253" s="10" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="C253" s="9" t="s">
         <v>58</v>
@@ -5773,7 +5770,7 @@
     </row>
     <row r="254" spans="1:6">
       <c r="A254" s="9" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B254" s="10" t="s">
         <v>253</v>
@@ -5784,10 +5781,10 @@
     </row>
     <row r="255" spans="1:6">
       <c r="A255" s="9" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B255" s="10" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="C255" s="9" t="s">
         <v>25</v>
@@ -5795,10 +5792,10 @@
     </row>
     <row r="256" spans="1:6">
       <c r="A256" s="9" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B256" s="10" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C256" s="9" t="s">
         <v>41</v>
@@ -5806,7 +5803,7 @@
     </row>
     <row r="257" spans="1:3">
       <c r="A257" s="9" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B257" s="10" t="s">
         <v>149</v>
@@ -5817,10 +5814,10 @@
     </row>
     <row r="258" spans="1:3">
       <c r="A258" s="9" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B258" s="10" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C258" s="9" t="s">
         <v>84</v>
@@ -5828,7 +5825,7 @@
     </row>
     <row r="259" spans="1:3">
       <c r="A259" s="9" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B259" s="10" t="s">
         <v>100</v>
@@ -5839,10 +5836,10 @@
     </row>
     <row r="260" spans="1:3">
       <c r="A260" s="9" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B260" s="10" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C260" s="9" t="s">
         <v>24</v>
@@ -5850,10 +5847,10 @@
     </row>
     <row r="261" spans="1:3">
       <c r="A261" s="9" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B261" s="10" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C261" s="9" t="s">
         <v>63</v>
@@ -5861,10 +5858,10 @@
     </row>
     <row r="262" spans="1:3">
       <c r="A262" s="9" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B262" s="10" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C262" s="9" t="s">
         <v>83</v>
@@ -5872,10 +5869,10 @@
     </row>
     <row r="263" spans="1:3">
       <c r="A263" s="9" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B263" s="10" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C263" s="9" t="s">
         <v>69</v>
@@ -5883,10 +5880,10 @@
     </row>
     <row r="264" spans="1:3">
       <c r="A264" s="9" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B264" s="10" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C264" s="9" t="s">
         <v>67</v>
@@ -5894,10 +5891,10 @@
     </row>
     <row r="265" spans="1:3">
       <c r="A265" s="9" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B265" s="10" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C265" s="4" t="s">
         <v>68</v>
@@ -5905,10 +5902,10 @@
     </row>
     <row r="266" spans="1:3">
       <c r="A266" s="9" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B266" s="10" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C266" s="9" t="s">
         <v>78</v>
@@ -5916,10 +5913,10 @@
     </row>
     <row r="267" spans="1:3">
       <c r="A267" s="9" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B267" s="10" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C267" s="9" t="s">
         <v>73</v>
@@ -5927,10 +5924,10 @@
     </row>
     <row r="268" spans="1:3">
       <c r="A268" s="9" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B268" s="10" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="C268" s="9" t="s">
         <v>74</v>
@@ -5938,10 +5935,10 @@
     </row>
     <row r="269" spans="1:3">
       <c r="A269" s="9" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B269" s="10" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C269" s="10" t="s">
         <v>61</v>
@@ -5949,7 +5946,7 @@
     </row>
     <row r="270" spans="1:3">
       <c r="A270" s="5" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B270" s="5" t="s">
         <v>251</v>
@@ -5960,10 +5957,10 @@
     </row>
     <row r="271" spans="1:3">
       <c r="A271" s="5" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B271" s="5" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C271" s="5" t="s">
         <v>10</v>
@@ -5971,10 +5968,10 @@
     </row>
     <row r="272" spans="1:3">
       <c r="A272" s="5" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B272" s="5" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="C272" s="5" t="s">
         <v>58</v>
@@ -5982,7 +5979,7 @@
     </row>
     <row r="273" spans="1:3">
       <c r="A273" s="5" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B273" s="5" t="s">
         <v>253</v>
@@ -5993,10 +5990,10 @@
     </row>
     <row r="274" spans="1:3">
       <c r="A274" s="5" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B274" s="5" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="C274" s="5" t="s">
         <v>25</v>
@@ -6004,10 +6001,10 @@
     </row>
     <row r="275" spans="1:3">
       <c r="A275" s="5" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B275" s="5" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C275" s="5" t="s">
         <v>41</v>
@@ -6015,7 +6012,7 @@
     </row>
     <row r="276" spans="1:3">
       <c r="A276" s="5" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B276" s="5" t="s">
         <v>149</v>
@@ -6026,10 +6023,10 @@
     </row>
     <row r="277" spans="1:3">
       <c r="A277" s="5" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B277" s="5" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C277" s="5" t="s">
         <v>84</v>
@@ -6037,7 +6034,7 @@
     </row>
     <row r="278" spans="1:3">
       <c r="A278" s="5" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B278" s="5" t="s">
         <v>100</v>
@@ -6048,10 +6045,10 @@
     </row>
     <row r="279" spans="1:3">
       <c r="A279" s="5" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B279" s="5" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C279" s="5" t="s">
         <v>24</v>
@@ -6059,10 +6056,10 @@
     </row>
     <row r="280" spans="1:3">
       <c r="A280" s="5" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B280" s="5" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C280" s="5" t="s">
         <v>83</v>
@@ -6070,10 +6067,10 @@
     </row>
     <row r="281" spans="1:3">
       <c r="A281" s="5" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B281" s="5" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C281" s="5" t="s">
         <v>69</v>
@@ -6081,10 +6078,10 @@
     </row>
     <row r="282" spans="1:3">
       <c r="A282" s="5" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B282" s="5" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C282" s="5" t="s">
         <v>68</v>
@@ -6092,10 +6089,10 @@
     </row>
     <row r="283" spans="1:3">
       <c r="A283" s="5" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B283" s="5" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C283" s="5" t="s">
         <v>78</v>
@@ -6103,10 +6100,10 @@
     </row>
     <row r="284" spans="1:3">
       <c r="A284" s="5" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B284" s="5" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C284" s="5" t="s">
         <v>73</v>
@@ -6114,10 +6111,10 @@
     </row>
     <row r="285" spans="1:3">
       <c r="A285" s="5" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B285" s="5" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="C285" s="5" t="s">
         <v>74</v>
@@ -6125,10 +6122,10 @@
     </row>
     <row r="286" spans="1:3">
       <c r="A286" s="5" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B286" s="5" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C286" s="5" t="s">
         <v>61</v>
@@ -6136,10 +6133,10 @@
     </row>
     <row r="287" spans="1:3">
       <c r="A287" s="5" t="s">
+        <v>293</v>
+      </c>
+      <c r="B287" s="5" t="s">
         <v>294</v>
-      </c>
-      <c r="B287" s="5" t="s">
-        <v>295</v>
       </c>
       <c r="C287" s="5" t="s">
         <v>58</v>
@@ -6147,7 +6144,7 @@
     </row>
     <row r="288" spans="1:3">
       <c r="A288" s="5" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B288" s="5" t="s">
         <v>178</v>
@@ -6158,10 +6155,10 @@
     </row>
     <row r="289" spans="1:3">
       <c r="A289" s="5" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B289" s="5" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C289" s="5" t="s">
         <v>57</v>
@@ -6169,10 +6166,10 @@
     </row>
     <row r="290" spans="1:3">
       <c r="A290" s="5" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B290" s="5" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C290" s="5" t="s">
         <v>56</v>
@@ -6211,12 +6208,12 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="5" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" s="5" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
   </sheetData>

</xml_diff>